<commit_message>
Update payment data in templates
</commit_message>
<xml_diff>
--- a/api/Templates/CSFunding 2018-19 Bulk Invoice Summary - Template.xlsx
+++ b/api/Templates/CSFunding 2018-19 Bulk Invoice Summary - Template.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="261">
   <si>
     <t>Pennsylvania Cyber Charter School</t>
   </si>
@@ -143,52 +143,250 @@
     <t>${Districts[0].Students[1].CurrentIep}</t>
   </si>
   <si>
+    <t>${Districts[0].Students[1].PASecuredID}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[1].Address1}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[1].FirstDay}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[1].LastDay}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[1].IsSpecialEducation}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[1].Address2}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[1].Grade}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[1].FormerIep}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[1].Address3}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[2].FullName}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[2].DateOfBirth}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[2].CurrentIep}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[2].PASecuredID}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[2].Address1}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[2].FirstDay}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[2].LastDay}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[2].IsSpecialEducation}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[2].Address2}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[2].Grade}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[2].FormerIep}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[2].Address3}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[3].FullName}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[3].DateOfBirth}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[3].CurrentIep}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[3].PASecuredID}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[3].Address1}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[3].FirstDay}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[3].LastDay}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[3].IsSpecialEducation}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[3].Address2}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[3].Grade}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[3].FormerIep}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[3].Address3}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[4].FullName}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[4].DateOfBirth}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[4].CurrentIep}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[4].PASecuredID}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[4].Address1}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[4].FirstDay}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[4].LastDay}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[4].IsSpecialEducation}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[4].Address2}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[4].Grade}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[4].FormerIep}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[4].Address3}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[5].FullName}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[5].DateOfBirth}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[5].CurrentIep}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[5].PASecuredID}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[5].Address1}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[5].FirstDay}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[5].LastDay}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[5].IsSpecialEducation}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[5].Address2}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[5].Grade}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[5].FormerIep}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[5].Address3}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[6].FullName}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[6].DateOfBirth}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[6].CurrentIep}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[6].PASecuredID}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[6].Address1}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[6].FirstDay}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[6].LastDay}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[6].IsSpecialEducation}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[6].Address2}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[6].Grade}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[6].FormerIep}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[6].Address3}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[7].FullName}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[7].DateOfBirth}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[7].CurrentIep}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[7].PASecuredID}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[7].Address1}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[7].FirstDay}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[7].LastDay}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[7].IsSpecialEducation}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[7].Address2}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[7].Grade}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[7].FormerIep}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Students[7].Address3}</t>
+  </si>
+  <si>
     <t>Summary Information Sheet</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[1].PASecuredID}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[1].Address1}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[1].FirstDay}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[1].LastDay}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[1].IsSpecialEducation}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[1].Address2}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[1].Grade}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[1].FormerIep}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[1].Address3}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[2].FullName}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[2].DateOfBirth}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[2].CurrentIep}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[2].PASecuredID}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[2].Address1}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[2].FirstDay}</t>
   </si>
   <si>
     <r>
@@ -239,220 +437,25 @@
     </r>
   </si>
   <si>
-    <t>${Districts[0].Students[2].LastDay}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[2].IsSpecialEducation}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[2].Address2}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[2].Grade}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[2].FormerIep}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[2].Address3}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[3].FullName}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[3].DateOfBirth}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[3].CurrentIep}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[3].PASecuredID}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[3].Address1}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[3].FirstDay}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[3].LastDay}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[3].IsSpecialEducation}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[3].Address2}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[3].Grade}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[3].FormerIep}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[3].Address3}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[4].FullName}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[4].DateOfBirth}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[4].CurrentIep}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[4].PASecuredID}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[4].Address1}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[4].FirstDay}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[4].LastDay}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[4].IsSpecialEducation}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[4].Address2}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[4].Grade}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[4].FormerIep}</t>
-  </si>
-  <si>
     <t>Invoice Prep Date:</t>
   </si>
   <si>
-    <t>${Districts[0].Students[4].Address3}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[5].FullName}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[5].DateOfBirth}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[5].CurrentIep}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[5].PASecuredID}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[5].Address1}</t>
-  </si>
-  <si>
     <t>Date Sent to SD:</t>
   </si>
   <si>
-    <t>${Districts[0].Students[5].FirstDay}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[5].LastDay}</t>
-  </si>
-  <si>
     <t>${ToSchoolDistrict}</t>
   </si>
   <si>
-    <t>${Districts[0].Students[5].IsSpecialEducation}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[5].Address2}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[5].Grade}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[5].FormerIep}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[5].Address3}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[6].FullName}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[6].DateOfBirth}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[6].CurrentIep}</t>
-  </si>
-  <si>
     <t>Date Sent to PDE:</t>
   </si>
   <si>
     <t>${ToPDE}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[6].PASecuredID}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[6].Address1}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[6].FirstDay}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[6].LastDay}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[6].IsSpecialEducation}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[6].Address2}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[6].Grade}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[6].FormerIep}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[6].Address3}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[7].FullName}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[7].DateOfBirth}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[7].CurrentIep}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[7].PASecuredID}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[7].Address1}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[7].FirstDay}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[7].LastDay}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[7].IsSpecialEducation}</t>
   </si>
   <si>
     <t>JUL
 ${Districts[0].FirstYear}</t>
   </si>
   <si>
-    <t>${Districts[0].Students[7].Address2}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[7].Grade}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Students[7].FormerIep}</t>
-  </si>
-  <si>
     <t>AUG
 ${Districts[0].FirstYear}</t>
   </si>
@@ -500,9 +503,6 @@
 Due</t>
   </si>
   <si>
-    <t>${Districts[0].Students[7].Address3}</t>
-  </si>
-  <si>
     <t>Nonspecial Education</t>
   </si>
   <si>
@@ -620,13 +620,13 @@
     <t>${Districts[0].Transactions.July.Payment.CheckAmount}</t>
   </si>
   <si>
-    <t>${Districts[0].Transaction.July.Payment.CheckNumber}</t>
+    <t>${Districts[0].Transactions.July.Payment.CheckNumber}</t>
   </si>
   <si>
     <t>${Districts[0].Transactions.July.Payment.Date}</t>
   </si>
   <si>
-    <t>${Districts[0].Transactions.July.Payment.Amount}</t>
+    <t>${Districts[0].Transactions.July.Payment.UniPayAmount}</t>
   </si>
   <si>
     <t>${Districts[0].Transactions.July.Refund}</t>
@@ -635,163 +635,196 @@
     <t>August</t>
   </si>
   <si>
-    <t>${Districts[0].Transactions.August.Payment.Amount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transaction.August.Payment.CheckNumber}</t>
+    <t>${Districts[0].Transactions.August.Payment.CheckAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.August.Payment.CheckNumber}</t>
   </si>
   <si>
     <t>${Districts[0].Transactions.August.Payment.Date}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.August.Payment.UniPayAmount}</t>
+  </si>
+  <si>
     <t>${Districts[0].Transactions.August.Refund}</t>
   </si>
   <si>
     <t>September</t>
   </si>
   <si>
-    <t>${Districts[0].Transactions.September.Payment.Amount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transaction.September.Payment.CheckNumber}</t>
+    <t>${Districts[0].Transactions.September.Payment.CheckAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.September.Payment.CheckNumber}</t>
   </si>
   <si>
     <t>${Districts[0].Transactions.September.Payment.Date}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.September.Payment.UniPayAmount}</t>
+  </si>
+  <si>
     <t>${Districts[0].Transactions.September.Refund}</t>
   </si>
   <si>
     <t>October</t>
   </si>
   <si>
-    <t>${Districts[0].Transactions.October.Payment.Amount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transaction.October.Payment.CheckNumber}</t>
+    <t>${Districts[0].Transactions.October.Payment.CheckAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.October.Payment.CheckNumber}</t>
   </si>
   <si>
     <t>${Districts[0].Transactions.October.Payment.Date}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.October.Payment.UniPayAmount}</t>
+  </si>
+  <si>
     <t>${Districts[0].Transactions.October.Refund}</t>
   </si>
   <si>
     <t>November</t>
   </si>
   <si>
-    <t>${Districts[0].Transactions.November.Payment.Amount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transaction.November.Payment.CheckNumber}</t>
+    <t>${Districts[0].Transactions.November.Payment.CheckAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.November.Payment.CheckNumber}</t>
   </si>
   <si>
     <t>${Districts[0].Transactions.November.Payment.Date}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.November.Payment.UniPayAmount}</t>
+  </si>
+  <si>
     <t>${Districts[0].Transactions.November.Refund}</t>
   </si>
   <si>
     <t>December</t>
   </si>
   <si>
-    <t>${Districts[0].Transactions.December.Payment.Amount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transaction.December.Payment.CheckNumber}</t>
+    <t>${Districts[0].Transactions.December.Payment.CheckAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.December.Payment.CheckNumber}</t>
   </si>
   <si>
     <t>${Districts[0].Transactions.December.Payment.Date}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.December.Payment.UniPayAmount}</t>
+  </si>
+  <si>
     <t>${Districts[0].Transactions.December.Refund}</t>
   </si>
   <si>
     <t>January, ${Districts[0].SecondYear}</t>
   </si>
   <si>
-    <t>${Districts[0].Transactions.January.Payment.Amount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transaction.January.Payment.CheckNumber}</t>
+    <t>${Districts[0].Transactions.January.Payment.CheckAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.January.Payment.CheckNumber}</t>
   </si>
   <si>
     <t>${Districts[0].Transactions.January.Payment.Date}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.January.Payment.UniPayAmount}</t>
+  </si>
+  <si>
     <t>${Districts[0].Transactions.January.Refund}</t>
   </si>
   <si>
     <t>February</t>
   </si>
   <si>
-    <t>${Districts[0].Transactions.February.Payment.Amount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transaction.February.Payment.CheckNumber}</t>
+    <t>${Districts[0].Transactions.February.Payment.CheckAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.February.Payment.CheckNumber}</t>
   </si>
   <si>
     <t>${Districts[0].Transactions.February.Payment.Date}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.February.Payment.UniPayAmount}</t>
+  </si>
+  <si>
     <t>${Districts[0].Transactions.February.Refund}</t>
   </si>
   <si>
     <t>March</t>
   </si>
   <si>
-    <t>${Districts[0].Transactions.March.Payment.Amount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transaction.March.Payment.CheckNumber}</t>
+    <t>${Districts[0].Transactions.March.Payment.CheckAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.March.Payment.CheckNumber}</t>
   </si>
   <si>
     <t>${Districts[0].Transactions.March.Payment.Date}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.March.Payment.UniPayAmount}</t>
+  </si>
+  <si>
     <t>${Districts[0].Transactions.March.Refund}</t>
   </si>
   <si>
     <t>April</t>
   </si>
   <si>
-    <t>${Districts[0].Transactions.April.Payment.Amount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transaction.April.Payment.CheckNumber}</t>
+    <t>${Districts[0].Transactions.April.Payment.CheckAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.April.Payment.CheckNumber}</t>
   </si>
   <si>
     <t>${Districts[0].Transactions.April.Payment.Date}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.April.Payment.UniPayAmount}</t>
+  </si>
+  <si>
     <t>${Districts[0].Transactions.April.Refund}</t>
   </si>
   <si>
     <t>May</t>
   </si>
   <si>
-    <t>${Districts[0].Transactions.May.Payment.Amount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transaction.May.Payment.CheckNumber}</t>
+    <t>${Districts[0].Transactions.May.Payment.CheckAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.May.Payment.CheckNumber}</t>
   </si>
   <si>
     <t>${Districts[0].Transactions.May.Payment.Date}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.May.Payment.UniPayAmount}</t>
+  </si>
+  <si>
     <t>${Districts[0].Transactions.May.Refund}</t>
   </si>
   <si>
     <t>June</t>
   </si>
   <si>
-    <t>${Districts[0].Transactions.June.Payment.Amount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transaction.June.Payment.CheckNumber}</t>
+    <t>${Districts[0].Transactions.June.Payment.CheckAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.June.Payment.CheckNumber}</t>
   </si>
   <si>
     <t>${Districts[0].Transactions.June.Payment.Date}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.June.Payment.UniPayAmount}</t>
   </si>
   <si>
     <t>${Districts[0].Transactions.June.Refund}</t>
@@ -1174,9 +1207,6 @@
         <color rgb="FF000000"/>
       </right>
       <top/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -1186,6 +1216,9 @@
         <color rgb="FF000000"/>
       </right>
       <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
     </border>
     <border>
       <left style="thin">
@@ -1426,6 +1459,12 @@
     <xf borderId="3" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -1453,27 +1492,18 @@
     <xf borderId="5" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="5" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="5" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="6" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="5" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="5" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
@@ -1600,6 +1630,21 @@
     <xf borderId="24" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf borderId="25" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="4" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -1624,33 +1669,21 @@
     <xf borderId="5" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf borderId="7" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="7" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="25" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="26" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="27" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="28" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="27" fillId="2" fontId="11" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -1712,7 +1745,7 @@
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="37" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="37" fillId="4" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
@@ -1721,7 +1754,7 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="35" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="36" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
@@ -1739,10 +1772,10 @@
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="38" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="40" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="40" fillId="4" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
@@ -1751,7 +1784,7 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="38" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="39" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
@@ -1772,10 +1805,10 @@
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="41" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="43" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="43" fillId="4" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
@@ -1784,7 +1817,7 @@
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="41" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="42" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
@@ -1908,13 +1941,13 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="15"/>
+      <c r="A1" s="6"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="18"/>
+      <c r="G1" s="7"/>
       <c r="H1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1923,214 +1956,214 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="21"/>
+      <c r="N1" s="67"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="64"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="16"/>
-      <c r="H2" s="11" t="s">
+      <c r="A2" s="68"/>
+      <c r="B2" s="12"/>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
+      <c r="E2" s="12"/>
+      <c r="F2" s="12"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="12"/>
+      <c r="I2" s="12"/>
+      <c r="J2" s="12"/>
+      <c r="K2" s="12"/>
+      <c r="L2" s="12"/>
+      <c r="M2" s="12"/>
+      <c r="N2" s="14"/>
     </row>
     <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="64"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="10"/>
-      <c r="G3" s="16"/>
-      <c r="H3" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-      <c r="N3" s="12"/>
+      <c r="A3" s="68"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="12"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="14"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="64"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="16"/>
-      <c r="H4" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-      <c r="N4" s="12"/>
+      <c r="A4" s="68"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="17"/>
+      <c r="H4" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="14"/>
     </row>
     <row r="5" ht="19.5" customHeight="1">
-      <c r="A5" s="65"/>
-      <c r="B5" s="66"/>
-      <c r="C5" s="66"/>
-      <c r="D5" s="66"/>
-      <c r="E5" s="66"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="66"/>
-      <c r="I5" s="66"/>
-      <c r="J5" s="66"/>
-      <c r="K5" s="66"/>
-      <c r="L5" s="66"/>
-      <c r="M5" s="66"/>
-      <c r="N5" s="67"/>
+      <c r="A5" s="69"/>
+      <c r="B5" s="70"/>
+      <c r="C5" s="70"/>
+      <c r="D5" s="70"/>
+      <c r="E5" s="70"/>
+      <c r="F5" s="70"/>
+      <c r="G5" s="70"/>
+      <c r="H5" s="70"/>
+      <c r="I5" s="70"/>
+      <c r="J5" s="70"/>
+      <c r="K5" s="70"/>
+      <c r="L5" s="70"/>
+      <c r="M5" s="70"/>
+      <c r="N5" s="71"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="68" t="s">
+      <c r="A6" s="72" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="20"/>
-      <c r="C6" s="16"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
-      <c r="G6" s="66"/>
-      <c r="H6" s="16"/>
-      <c r="I6" s="16"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="69" t="s">
-        <v>89</v>
-      </c>
-      <c r="L6" s="16"/>
-      <c r="M6" s="16"/>
-      <c r="N6" s="23" t="s">
+      <c r="C6" s="17"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="70"/>
+      <c r="H6" s="17"/>
+      <c r="I6" s="17"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="73" t="s">
+        <v>126</v>
+      </c>
+      <c r="L6" s="17"/>
+      <c r="M6" s="17"/>
+      <c r="N6" s="22" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="68" t="s">
+      <c r="A7" s="72" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="20"/>
-      <c r="C7" s="16"/>
-      <c r="D7" s="16"/>
-      <c r="E7" s="16"/>
-      <c r="F7" s="17"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="17"/>
-      <c r="I7" s="17"/>
-      <c r="J7" s="17"/>
-      <c r="K7" s="69" t="s">
-        <v>96</v>
-      </c>
-      <c r="L7" s="16"/>
-      <c r="M7" s="16"/>
-      <c r="N7" s="23" t="s">
-        <v>99</v>
+      <c r="C7" s="17"/>
+      <c r="D7" s="17"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="18"/>
+      <c r="G7" s="18"/>
+      <c r="H7" s="18"/>
+      <c r="I7" s="18"/>
+      <c r="J7" s="18"/>
+      <c r="K7" s="73" t="s">
+        <v>127</v>
+      </c>
+      <c r="L7" s="17"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="22" t="s">
+        <v>128</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="70"/>
+      <c r="A8" s="74"/>
       <c r="B8" s="20"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="16"/>
-      <c r="E8" s="16"/>
-      <c r="F8" s="17"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="17"/>
-      <c r="I8" s="17"/>
-      <c r="J8" s="17"/>
-      <c r="K8" s="69" t="s">
-        <v>108</v>
-      </c>
-      <c r="L8" s="16"/>
-      <c r="M8" s="16"/>
-      <c r="N8" s="23" t="s">
-        <v>109</v>
+      <c r="C8" s="17"/>
+      <c r="D8" s="17"/>
+      <c r="E8" s="17"/>
+      <c r="F8" s="18"/>
+      <c r="G8" s="18"/>
+      <c r="H8" s="18"/>
+      <c r="I8" s="18"/>
+      <c r="J8" s="18"/>
+      <c r="K8" s="73" t="s">
+        <v>129</v>
+      </c>
+      <c r="L8" s="17"/>
+      <c r="M8" s="17"/>
+      <c r="N8" s="22" t="s">
+        <v>130</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="6"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="71"/>
-      <c r="D9" s="71"/>
-      <c r="E9" s="71"/>
-      <c r="F9" s="71"/>
-      <c r="G9" s="71"/>
-      <c r="H9" s="71"/>
-      <c r="I9" s="71"/>
-      <c r="J9" s="71"/>
-      <c r="K9" s="16"/>
-      <c r="L9" s="16"/>
-      <c r="M9" s="16"/>
-      <c r="N9" s="67"/>
+      <c r="A9" s="8"/>
+      <c r="B9" s="18"/>
+      <c r="C9" s="75"/>
+      <c r="D9" s="75"/>
+      <c r="E9" s="75"/>
+      <c r="F9" s="75"/>
+      <c r="G9" s="75"/>
+      <c r="H9" s="75"/>
+      <c r="I9" s="75"/>
+      <c r="J9" s="75"/>
+      <c r="K9" s="17"/>
+      <c r="L9" s="17"/>
+      <c r="M9" s="17"/>
+      <c r="N9" s="71"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="6"/>
-      <c r="B10" s="73"/>
-      <c r="C10" s="74"/>
-      <c r="D10" s="74"/>
-      <c r="E10" s="74"/>
-      <c r="F10" s="74"/>
-      <c r="G10" s="74"/>
-      <c r="H10" s="74"/>
-      <c r="I10" s="74"/>
-      <c r="J10" s="74"/>
-      <c r="K10" s="24"/>
-      <c r="L10" s="24"/>
-      <c r="M10" s="24"/>
-      <c r="N10" s="67"/>
+      <c r="A10" s="8"/>
+      <c r="B10" s="76"/>
+      <c r="C10" s="77"/>
+      <c r="D10" s="77"/>
+      <c r="E10" s="77"/>
+      <c r="F10" s="77"/>
+      <c r="G10" s="77"/>
+      <c r="H10" s="77"/>
+      <c r="I10" s="77"/>
+      <c r="J10" s="77"/>
+      <c r="K10" s="23"/>
+      <c r="L10" s="23"/>
+      <c r="M10" s="23"/>
+      <c r="N10" s="71"/>
     </row>
     <row r="11" ht="39.0" customHeight="1">
-      <c r="A11" s="75"/>
-      <c r="B11" s="77" t="s">
-        <v>127</v>
-      </c>
-      <c r="C11" s="77" t="s">
+      <c r="A11" s="78"/>
+      <c r="B11" s="79" t="s">
         <v>131</v>
       </c>
-      <c r="D11" s="77" t="s">
+      <c r="C11" s="79" t="s">
         <v>132</v>
       </c>
-      <c r="E11" s="77" t="s">
+      <c r="D11" s="79" t="s">
         <v>133</v>
       </c>
-      <c r="F11" s="77" t="s">
+      <c r="E11" s="79" t="s">
         <v>134</v>
       </c>
-      <c r="G11" s="77" t="s">
+      <c r="F11" s="79" t="s">
         <v>135</v>
       </c>
-      <c r="H11" s="77" t="s">
+      <c r="G11" s="79" t="s">
         <v>136</v>
       </c>
-      <c r="I11" s="77" t="s">
+      <c r="H11" s="79" t="s">
         <v>137</v>
       </c>
-      <c r="J11" s="77" t="s">
+      <c r="I11" s="79" t="s">
         <v>138</v>
       </c>
-      <c r="K11" s="77" t="s">
+      <c r="J11" s="79" t="s">
         <v>139</v>
       </c>
-      <c r="L11" s="77" t="s">
+      <c r="K11" s="79" t="s">
         <v>140</v>
       </c>
-      <c r="M11" s="77" t="s">
+      <c r="L11" s="79" t="s">
         <v>141</v>
       </c>
-      <c r="N11" s="79" t="s">
+      <c r="M11" s="79" t="s">
         <v>142</v>
+      </c>
+      <c r="N11" s="80" t="s">
+        <v>143</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1">
@@ -2240,17 +2273,17 @@
       <c r="N14" s="87"/>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="6"/>
-      <c r="B15" s="16"/>
-      <c r="C15" s="16"/>
-      <c r="D15" s="16"/>
-      <c r="E15" s="16"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="16"/>
-      <c r="H15" s="16"/>
-      <c r="I15" s="16"/>
-      <c r="J15" s="16"/>
-      <c r="K15" s="16"/>
+      <c r="A15" s="8"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="17"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
       <c r="L15" s="88"/>
       <c r="M15" s="89" t="s">
         <v>170</v>
@@ -2261,50 +2294,50 @@
       </c>
     </row>
     <row r="16" ht="13.5" customHeight="1">
-      <c r="A16" s="6"/>
-      <c r="B16" s="16"/>
-      <c r="C16" s="16"/>
-      <c r="D16" s="16"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="16"/>
-      <c r="H16" s="16"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="16"/>
-      <c r="K16" s="16"/>
-      <c r="L16" s="16"/>
-      <c r="M16" s="16"/>
-      <c r="N16" s="67"/>
+      <c r="A16" s="8"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+      <c r="H16" s="17"/>
+      <c r="I16" s="17"/>
+      <c r="J16" s="17"/>
+      <c r="K16" s="17"/>
+      <c r="L16" s="17"/>
+      <c r="M16" s="17"/>
+      <c r="N16" s="71"/>
     </row>
     <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="6"/>
-      <c r="B17" s="16"/>
-      <c r="C17" s="16"/>
-      <c r="D17" s="16"/>
-      <c r="E17" s="69" t="s">
+      <c r="A17" s="8"/>
+      <c r="B17" s="17"/>
+      <c r="C17" s="17"/>
+      <c r="D17" s="17"/>
+      <c r="E17" s="73" t="s">
         <v>171</v>
       </c>
-      <c r="F17" s="16"/>
+      <c r="F17" s="17"/>
       <c r="G17" s="91" t="s">
         <v>172</v>
       </c>
       <c r="H17" s="91" t="s">
         <v>172</v>
       </c>
-      <c r="I17" s="69" t="s">
+      <c r="I17" s="73" t="s">
         <v>173</v>
       </c>
-      <c r="J17" s="16"/>
-      <c r="K17" s="69" t="s">
+      <c r="J17" s="17"/>
+      <c r="K17" s="73" t="s">
         <v>174</v>
       </c>
-      <c r="L17" s="16"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="67"/>
+      <c r="L17" s="17"/>
+      <c r="M17" s="17"/>
+      <c r="N17" s="71"/>
     </row>
     <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="6"/>
-      <c r="B18" s="16"/>
+      <c r="A18" s="8"/>
+      <c r="B18" s="17"/>
       <c r="C18" s="92" t="s">
         <v>175</v>
       </c>
@@ -2327,12 +2360,12 @@
         <v>180</v>
       </c>
       <c r="L18" s="96"/>
-      <c r="M18" s="16"/>
-      <c r="N18" s="67"/>
+      <c r="M18" s="17"/>
+      <c r="N18" s="71"/>
     </row>
     <row r="19" ht="13.5" customHeight="1">
-      <c r="A19" s="6"/>
-      <c r="B19" s="16"/>
+      <c r="A19" s="8"/>
+      <c r="B19" s="17"/>
       <c r="C19" s="97" t="s">
         <v>181</v>
       </c>
@@ -2355,12 +2388,12 @@
         <v>186</v>
       </c>
       <c r="L19" s="106"/>
-      <c r="M19" s="16"/>
-      <c r="N19" s="67"/>
+      <c r="M19" s="17"/>
+      <c r="N19" s="71"/>
     </row>
     <row r="20" ht="13.5" customHeight="1">
-      <c r="A20" s="6"/>
-      <c r="B20" s="16"/>
+      <c r="A20" s="8"/>
+      <c r="B20" s="17"/>
       <c r="C20" s="107" t="s">
         <v>187</v>
       </c>
@@ -2377,298 +2410,298 @@
       </c>
       <c r="I20" s="113"/>
       <c r="J20" s="114" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="K20" s="115" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="L20" s="116"/>
-      <c r="M20" s="16"/>
-      <c r="N20" s="67"/>
+      <c r="M20" s="17"/>
+      <c r="N20" s="71"/>
     </row>
     <row r="21" ht="13.5" customHeight="1">
-      <c r="A21" s="6"/>
-      <c r="B21" s="16"/>
-      <c r="C21" s="69" t="s">
-        <v>192</v>
+      <c r="A21" s="8"/>
+      <c r="B21" s="17"/>
+      <c r="C21" s="73" t="s">
+        <v>193</v>
       </c>
       <c r="D21" s="117"/>
       <c r="E21" s="109"/>
       <c r="F21" s="110" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="G21" s="111" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="H21" s="112" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="I21" s="113"/>
       <c r="J21" s="114" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="K21" s="115" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="L21" s="116"/>
-      <c r="M21" s="16"/>
-      <c r="N21" s="67"/>
+      <c r="M21" s="17"/>
+      <c r="N21" s="71"/>
     </row>
     <row r="22" ht="13.5" customHeight="1">
-      <c r="A22" s="6"/>
-      <c r="B22" s="16"/>
-      <c r="C22" s="69" t="s">
-        <v>197</v>
+      <c r="A22" s="8"/>
+      <c r="B22" s="17"/>
+      <c r="C22" s="73" t="s">
+        <v>199</v>
       </c>
       <c r="D22" s="117"/>
       <c r="E22" s="109"/>
       <c r="F22" s="110" t="s">
-        <v>198</v>
+        <v>200</v>
       </c>
       <c r="G22" s="111" t="s">
-        <v>199</v>
+        <v>201</v>
       </c>
       <c r="H22" s="112" t="s">
-        <v>200</v>
+        <v>202</v>
       </c>
       <c r="I22" s="113"/>
       <c r="J22" s="114" t="s">
-        <v>198</v>
+        <v>203</v>
       </c>
       <c r="K22" s="115" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="L22" s="116"/>
-      <c r="M22" s="16"/>
-      <c r="N22" s="67"/>
+      <c r="M22" s="17"/>
+      <c r="N22" s="71"/>
     </row>
     <row r="23" ht="13.5" customHeight="1">
-      <c r="A23" s="6"/>
-      <c r="B23" s="16"/>
-      <c r="C23" s="69" t="s">
-        <v>202</v>
+      <c r="A23" s="8"/>
+      <c r="B23" s="17"/>
+      <c r="C23" s="73" t="s">
+        <v>205</v>
       </c>
       <c r="D23" s="117"/>
       <c r="E23" s="109"/>
       <c r="F23" s="110" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="G23" s="111" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="H23" s="112" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="I23" s="113"/>
       <c r="J23" s="114" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="K23" s="115" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="L23" s="116"/>
-      <c r="M23" s="16"/>
+      <c r="M23" s="17"/>
       <c r="N23" s="118"/>
     </row>
     <row r="24" ht="13.5" customHeight="1">
-      <c r="A24" s="6"/>
-      <c r="B24" s="16"/>
-      <c r="C24" s="69" t="s">
-        <v>207</v>
+      <c r="A24" s="8"/>
+      <c r="B24" s="17"/>
+      <c r="C24" s="73" t="s">
+        <v>211</v>
       </c>
       <c r="D24" s="117"/>
       <c r="E24" s="109"/>
       <c r="F24" s="110" t="s">
-        <v>208</v>
+        <v>212</v>
       </c>
       <c r="G24" s="111" t="s">
-        <v>209</v>
+        <v>213</v>
       </c>
       <c r="H24" s="112" t="s">
-        <v>210</v>
+        <v>214</v>
       </c>
       <c r="I24" s="113"/>
       <c r="J24" s="114" t="s">
-        <v>208</v>
+        <v>215</v>
       </c>
       <c r="K24" s="115" t="s">
-        <v>211</v>
+        <v>216</v>
       </c>
       <c r="L24" s="116"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="67"/>
+      <c r="M24" s="17"/>
+      <c r="N24" s="71"/>
     </row>
     <row r="25" ht="13.5" customHeight="1">
-      <c r="A25" s="6"/>
-      <c r="B25" s="16"/>
-      <c r="C25" s="69" t="s">
-        <v>212</v>
+      <c r="A25" s="8"/>
+      <c r="B25" s="17"/>
+      <c r="C25" s="73" t="s">
+        <v>217</v>
       </c>
       <c r="D25" s="117"/>
       <c r="E25" s="109"/>
       <c r="F25" s="110" t="s">
-        <v>213</v>
+        <v>218</v>
       </c>
       <c r="G25" s="111" t="s">
-        <v>214</v>
+        <v>219</v>
       </c>
       <c r="H25" s="112" t="s">
-        <v>215</v>
+        <v>220</v>
       </c>
       <c r="I25" s="113"/>
       <c r="J25" s="114" t="s">
-        <v>213</v>
+        <v>221</v>
       </c>
       <c r="K25" s="115" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
       <c r="L25" s="116"/>
-      <c r="M25" s="16"/>
-      <c r="N25" s="67"/>
+      <c r="M25" s="17"/>
+      <c r="N25" s="71"/>
     </row>
     <row r="26" ht="13.5" customHeight="1">
-      <c r="A26" s="6"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="69" t="s">
-        <v>217</v>
+      <c r="A26" s="8"/>
+      <c r="B26" s="17"/>
+      <c r="C26" s="73" t="s">
+        <v>223</v>
       </c>
       <c r="D26" s="117"/>
       <c r="E26" s="109"/>
       <c r="F26" s="110" t="s">
-        <v>218</v>
+        <v>224</v>
       </c>
       <c r="G26" s="111" t="s">
-        <v>219</v>
+        <v>225</v>
       </c>
       <c r="H26" s="112" t="s">
-        <v>220</v>
+        <v>226</v>
       </c>
       <c r="I26" s="113"/>
       <c r="J26" s="114" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="K26" s="115" t="s">
-        <v>221</v>
+        <v>228</v>
       </c>
       <c r="L26" s="116"/>
-      <c r="M26" s="16"/>
-      <c r="N26" s="67"/>
+      <c r="M26" s="17"/>
+      <c r="N26" s="71"/>
     </row>
     <row r="27" ht="13.5" customHeight="1">
-      <c r="A27" s="6"/>
-      <c r="B27" s="16"/>
-      <c r="C27" s="69" t="s">
-        <v>222</v>
+      <c r="A27" s="8"/>
+      <c r="B27" s="17"/>
+      <c r="C27" s="73" t="s">
+        <v>229</v>
       </c>
       <c r="D27" s="117"/>
       <c r="E27" s="109"/>
       <c r="F27" s="110" t="s">
-        <v>223</v>
+        <v>230</v>
       </c>
       <c r="G27" s="111" t="s">
-        <v>224</v>
+        <v>231</v>
       </c>
       <c r="H27" s="112" t="s">
-        <v>225</v>
+        <v>232</v>
       </c>
       <c r="I27" s="113"/>
       <c r="J27" s="114" t="s">
-        <v>223</v>
+        <v>233</v>
       </c>
       <c r="K27" s="115" t="s">
-        <v>226</v>
+        <v>234</v>
       </c>
       <c r="L27" s="116"/>
-      <c r="M27" s="16"/>
-      <c r="N27" s="67"/>
+      <c r="M27" s="17"/>
+      <c r="N27" s="71"/>
     </row>
     <row r="28" ht="13.5" customHeight="1">
-      <c r="A28" s="6"/>
-      <c r="B28" s="16"/>
-      <c r="C28" s="69" t="s">
-        <v>227</v>
+      <c r="A28" s="8"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="73" t="s">
+        <v>235</v>
       </c>
       <c r="D28" s="117"/>
       <c r="E28" s="109"/>
       <c r="F28" s="110" t="s">
-        <v>228</v>
+        <v>236</v>
       </c>
       <c r="G28" s="111" t="s">
-        <v>229</v>
+        <v>237</v>
       </c>
       <c r="H28" s="112" t="s">
-        <v>230</v>
+        <v>238</v>
       </c>
       <c r="I28" s="113"/>
       <c r="J28" s="114" t="s">
-        <v>228</v>
+        <v>239</v>
       </c>
       <c r="K28" s="115" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="L28" s="116"/>
-      <c r="M28" s="16"/>
-      <c r="N28" s="67"/>
+      <c r="M28" s="17"/>
+      <c r="N28" s="71"/>
     </row>
     <row r="29" ht="13.5" customHeight="1">
-      <c r="A29" s="6"/>
-      <c r="B29" s="16"/>
-      <c r="C29" s="69" t="s">
-        <v>232</v>
+      <c r="A29" s="8"/>
+      <c r="B29" s="17"/>
+      <c r="C29" s="73" t="s">
+        <v>241</v>
       </c>
       <c r="D29" s="117"/>
       <c r="E29" s="109"/>
       <c r="F29" s="110" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="G29" s="111" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="H29" s="112" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="I29" s="113"/>
       <c r="J29" s="114" t="s">
-        <v>233</v>
+        <v>245</v>
       </c>
       <c r="K29" s="115" t="s">
-        <v>236</v>
+        <v>246</v>
       </c>
       <c r="L29" s="116"/>
-      <c r="M29" s="16"/>
-      <c r="N29" s="67"/>
+      <c r="M29" s="17"/>
+      <c r="N29" s="71"/>
     </row>
     <row r="30" ht="13.5" customHeight="1">
-      <c r="A30" s="6"/>
-      <c r="B30" s="16"/>
+      <c r="A30" s="8"/>
+      <c r="B30" s="17"/>
       <c r="C30" s="94" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="D30" s="119"/>
       <c r="E30" s="120"/>
       <c r="F30" s="121" t="s">
-        <v>238</v>
+        <v>248</v>
       </c>
       <c r="G30" s="122" t="s">
-        <v>239</v>
+        <v>249</v>
       </c>
       <c r="H30" s="123" t="s">
-        <v>240</v>
+        <v>250</v>
       </c>
       <c r="I30" s="124"/>
       <c r="J30" s="125" t="s">
-        <v>238</v>
+        <v>251</v>
       </c>
       <c r="K30" s="126" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
       <c r="L30" s="127"/>
-      <c r="M30" s="16"/>
-      <c r="N30" s="67"/>
+      <c r="M30" s="17"/>
+      <c r="N30" s="71"/>
     </row>
     <row r="31" ht="13.5" customHeight="1">
-      <c r="A31" s="6"/>
-      <c r="B31" s="16"/>
+      <c r="A31" s="8"/>
+      <c r="B31" s="17"/>
       <c r="C31" s="128"/>
       <c r="D31" s="128"/>
       <c r="E31" s="129"/>
@@ -2688,13 +2721,13 @@
         <f>SUM(L19:L30)</f>
         <v>0</v>
       </c>
-      <c r="M31" s="16"/>
-      <c r="N31" s="67"/>
+      <c r="M31" s="17"/>
+      <c r="N31" s="71"/>
     </row>
     <row r="32" ht="13.5" customHeight="1">
       <c r="A32" s="131"/>
       <c r="B32" s="132" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="C32" s="133" t="s">
         <v>0</v>
@@ -2708,14 +2741,14 @@
       <c r="J32" s="135"/>
       <c r="K32" s="135"/>
       <c r="L32" s="135"/>
-      <c r="M32" s="16"/>
-      <c r="N32" s="67"/>
+      <c r="M32" s="17"/>
+      <c r="N32" s="71"/>
     </row>
     <row r="33" ht="13.5" customHeight="1">
       <c r="A33" s="137"/>
       <c r="B33" s="138"/>
       <c r="C33" s="133" t="s">
-        <v>243</v>
+        <v>254</v>
       </c>
       <c r="D33" s="134"/>
       <c r="E33" s="135"/>
@@ -2726,44 +2759,44 @@
       <c r="J33" s="135"/>
       <c r="K33" s="135"/>
       <c r="L33" s="135"/>
-      <c r="M33" s="16"/>
-      <c r="N33" s="67"/>
+      <c r="M33" s="17"/>
+      <c r="N33" s="71"/>
     </row>
     <row r="34" ht="13.5" customHeight="1">
       <c r="A34" s="137"/>
       <c r="B34" s="138"/>
       <c r="C34" s="133" t="s">
-        <v>244</v>
-      </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
-      <c r="F34" s="16"/>
-      <c r="G34" s="16"/>
-      <c r="H34" s="16"/>
-      <c r="I34" s="16"/>
-      <c r="J34" s="16"/>
-      <c r="K34" s="16"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="16"/>
-      <c r="N34" s="67"/>
+        <v>255</v>
+      </c>
+      <c r="D34" s="17"/>
+      <c r="E34" s="17"/>
+      <c r="F34" s="17"/>
+      <c r="G34" s="17"/>
+      <c r="H34" s="17"/>
+      <c r="I34" s="17"/>
+      <c r="J34" s="17"/>
+      <c r="K34" s="17"/>
+      <c r="L34" s="17"/>
+      <c r="M34" s="17"/>
+      <c r="N34" s="71"/>
     </row>
     <row r="35" ht="13.5" customHeight="1">
       <c r="A35" s="137"/>
       <c r="B35" s="138"/>
       <c r="C35" s="133" t="s">
-        <v>245</v>
-      </c>
-      <c r="D35" s="16"/>
+        <v>256</v>
+      </c>
+      <c r="D35" s="17"/>
       <c r="E35" s="139"/>
-      <c r="F35" s="16"/>
-      <c r="G35" s="16"/>
-      <c r="H35" s="16"/>
-      <c r="I35" s="16"/>
-      <c r="J35" s="16"/>
-      <c r="K35" s="16"/>
-      <c r="L35" s="16"/>
+      <c r="F35" s="17"/>
+      <c r="G35" s="17"/>
+      <c r="H35" s="17"/>
+      <c r="I35" s="17"/>
+      <c r="J35" s="17"/>
+      <c r="K35" s="17"/>
+      <c r="L35" s="17"/>
       <c r="M35" s="89" t="s">
-        <v>246</v>
+        <v>257</v>
       </c>
       <c r="N35" s="140">
         <f>ROUND(F31+J31-L31,2)</f>
@@ -2773,28 +2806,28 @@
     <row r="36" ht="14.25" customHeight="1">
       <c r="A36" s="137"/>
       <c r="B36" s="141" t="s">
-        <v>247</v>
+        <v>258</v>
       </c>
       <c r="C36" s="142" t="s">
-        <v>248</v>
-      </c>
-      <c r="D36" s="16"/>
+        <v>259</v>
+      </c>
+      <c r="D36" s="17"/>
       <c r="E36" s="139"/>
-      <c r="F36" s="16"/>
-      <c r="G36" s="16"/>
-      <c r="H36" s="16"/>
-      <c r="I36" s="16"/>
-      <c r="J36" s="16"/>
-      <c r="K36" s="16"/>
-      <c r="L36" s="16"/>
-      <c r="M36" s="16"/>
+      <c r="F36" s="17"/>
+      <c r="G36" s="17"/>
+      <c r="H36" s="17"/>
+      <c r="I36" s="17"/>
+      <c r="J36" s="17"/>
+      <c r="K36" s="17"/>
+      <c r="L36" s="17"/>
+      <c r="M36" s="17"/>
       <c r="N36" s="143"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
       <c r="A37" s="144"/>
       <c r="B37" s="138"/>
       <c r="C37" s="142" t="s">
-        <v>249</v>
+        <v>260</v>
       </c>
       <c r="D37" s="145"/>
       <c r="E37" s="146"/>
@@ -3842,836 +3875,836 @@
       <c r="K1" s="5"/>
     </row>
     <row r="2">
-      <c r="A2" s="6"/>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="8" t="s">
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7"/>
-      <c r="K2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="9"/>
+      <c r="K2" s="11"/>
     </row>
     <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="6"/>
-      <c r="B3" s="10"/>
-      <c r="C3" s="10"/>
-      <c r="D3" s="10"/>
-      <c r="E3" s="10"/>
-      <c r="F3" s="11" t="s">
+      <c r="A3" s="8"/>
+      <c r="B3" s="12"/>
+      <c r="C3" s="12"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="10"/>
-      <c r="K3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="12"/>
+      <c r="I3" s="12"/>
+      <c r="J3" s="12"/>
+      <c r="K3" s="14"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="6"/>
-      <c r="B4" s="10"/>
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="11" t="s">
+      <c r="A4" s="8"/>
+      <c r="B4" s="12"/>
+      <c r="C4" s="12"/>
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="14"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="6"/>
-      <c r="B5" s="13" t="s">
+      <c r="A5" s="8"/>
+      <c r="B5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="16"/>
-      <c r="F5" s="16"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="17"/>
-      <c r="I5" s="17"/>
-      <c r="J5" s="17"/>
+      <c r="C5" s="16"/>
+      <c r="D5" s="16"/>
+      <c r="E5" s="17"/>
+      <c r="F5" s="17"/>
+      <c r="G5" s="18"/>
+      <c r="H5" s="18"/>
+      <c r="I5" s="18"/>
+      <c r="J5" s="18"/>
       <c r="K5" s="19"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="6"/>
-      <c r="B6" s="13" t="s">
+      <c r="A6" s="8"/>
+      <c r="B6" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="16"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="16"/>
-      <c r="F6" s="16"/>
+      <c r="C6" s="17"/>
+      <c r="D6" s="16"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="14"/>
-      <c r="K6" s="23" t="s">
+      <c r="I6" s="21"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="22" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="6"/>
-      <c r="B7" s="24"/>
-      <c r="C7" s="24"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
-      <c r="F7" s="24"/>
-      <c r="G7" s="24"/>
-      <c r="H7" s="24"/>
-      <c r="I7" s="24"/>
-      <c r="J7" s="24"/>
-      <c r="K7" s="25"/>
+      <c r="A7" s="8"/>
+      <c r="B7" s="23"/>
+      <c r="C7" s="23"/>
+      <c r="D7" s="23"/>
+      <c r="E7" s="23"/>
+      <c r="F7" s="23"/>
+      <c r="G7" s="23"/>
+      <c r="H7" s="23"/>
+      <c r="I7" s="23"/>
+      <c r="J7" s="23"/>
+      <c r="K7" s="24"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="26"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="29"/>
-      <c r="F8" s="30" t="s">
+      <c r="A8" s="25"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="31" t="s">
+      <c r="G8" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="32"/>
-      <c r="I8" s="33" t="s">
+      <c r="H8" s="31"/>
+      <c r="I8" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="34"/>
-      <c r="K8" s="31" t="s">
+      <c r="J8" s="33"/>
+      <c r="K8" s="30" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="26"/>
-      <c r="B9" s="35" t="s">
+      <c r="A9" s="25"/>
+      <c r="B9" s="34" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="38"/>
-      <c r="F9" s="39"/>
-      <c r="G9" s="35" t="s">
+      <c r="C9" s="35"/>
+      <c r="D9" s="36"/>
+      <c r="E9" s="37"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="34" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="40" t="s">
+      <c r="H9" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="40" t="s">
+      <c r="I9" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="35" t="s">
+      <c r="J9" s="34" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="41" t="s">
+      <c r="K9" s="40" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="26"/>
-      <c r="B10" s="35" t="s">
+      <c r="A10" s="25"/>
+      <c r="B10" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="42" t="s">
+      <c r="C10" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="D10" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="38"/>
-      <c r="F10" s="31" t="s">
+      <c r="E10" s="37"/>
+      <c r="F10" s="30" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="35" t="s">
+      <c r="G10" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="40" t="s">
+      <c r="H10" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="44" t="s">
+      <c r="I10" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="35" t="s">
+      <c r="J10" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="31" t="s">
+      <c r="K10" s="30" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="26"/>
-      <c r="B11" s="39"/>
-      <c r="C11" s="39"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="46"/>
-      <c r="F11" s="39"/>
-      <c r="G11" s="41" t="s">
+      <c r="A11" s="25"/>
+      <c r="B11" s="38"/>
+      <c r="C11" s="38"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="47"/>
-      <c r="I11" s="48" t="s">
+      <c r="H11" s="46"/>
+      <c r="I11" s="47" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="41" t="s">
+      <c r="J11" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="41" t="s">
+      <c r="K11" s="40" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="26"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="49"/>
-      <c r="D12" s="50" t="s">
+      <c r="A12" s="25"/>
+      <c r="B12" s="48"/>
+      <c r="C12" s="48"/>
+      <c r="D12" s="49" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="51"/>
-      <c r="F12" s="52" t="s">
+      <c r="E12" s="50"/>
+      <c r="F12" s="51" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="53"/>
-      <c r="H12" s="53"/>
-      <c r="I12" s="53"/>
-      <c r="J12" s="49"/>
-      <c r="K12" s="52" t="s">
+      <c r="G12" s="52"/>
+      <c r="H12" s="52"/>
+      <c r="I12" s="52"/>
+      <c r="J12" s="48"/>
+      <c r="K12" s="51" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="26"/>
-      <c r="B13" s="54">
+      <c r="A13" s="25"/>
+      <c r="B13" s="53">
         <v>1.0</v>
       </c>
-      <c r="C13" s="55" t="s">
+      <c r="C13" s="54" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="56" t="s">
+      <c r="D13" s="55" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="57"/>
-      <c r="F13" s="58"/>
-      <c r="G13" s="54"/>
-      <c r="H13" s="59" t="s">
+      <c r="E13" s="56"/>
+      <c r="F13" s="57"/>
+      <c r="G13" s="53"/>
+      <c r="H13" s="58" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="59" t="s">
+      <c r="I13" s="58" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="55" t="s">
+      <c r="J13" s="54" t="s">
         <v>35</v>
       </c>
-      <c r="K13" s="60"/>
+      <c r="K13" s="59"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="26"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="54"/>
-      <c r="D14" s="56" t="s">
+      <c r="A14" s="25"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="53"/>
+      <c r="D14" s="55" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="57"/>
-      <c r="F14" s="61" t="s">
+      <c r="E14" s="56"/>
+      <c r="F14" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="54"/>
-      <c r="H14" s="54"/>
-      <c r="I14" s="54"/>
-      <c r="J14" s="54"/>
-      <c r="K14" s="52" t="s">
+      <c r="G14" s="53"/>
+      <c r="H14" s="53"/>
+      <c r="I14" s="53"/>
+      <c r="J14" s="53"/>
+      <c r="K14" s="51" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="26"/>
-      <c r="B15" s="60"/>
-      <c r="C15" s="60"/>
-      <c r="D15" s="62" t="s">
+      <c r="A15" s="25"/>
+      <c r="B15" s="59"/>
+      <c r="C15" s="59"/>
+      <c r="D15" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="63"/>
-      <c r="F15" s="60"/>
-      <c r="G15" s="60"/>
-      <c r="H15" s="60"/>
-      <c r="I15" s="60"/>
-      <c r="J15" s="60"/>
-      <c r="K15" s="60"/>
+      <c r="E15" s="62"/>
+      <c r="F15" s="59"/>
+      <c r="G15" s="59"/>
+      <c r="H15" s="59"/>
+      <c r="I15" s="59"/>
+      <c r="J15" s="59"/>
+      <c r="K15" s="59"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="26"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="50" t="s">
+      <c r="A16" s="25"/>
+      <c r="B16" s="48"/>
+      <c r="C16" s="48"/>
+      <c r="D16" s="49" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="51"/>
-      <c r="F16" s="52" t="s">
+      <c r="E16" s="50"/>
+      <c r="F16" s="51" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="53"/>
-      <c r="H16" s="53"/>
-      <c r="I16" s="53"/>
-      <c r="J16" s="49"/>
-      <c r="K16" s="52" t="s">
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="48"/>
+      <c r="K16" s="51" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="26"/>
-      <c r="B17" s="54">
+      <c r="A17" s="25"/>
+      <c r="B17" s="53">
         <f>B13+1</f>
         <v>2</v>
       </c>
-      <c r="C17" s="55" t="s">
+      <c r="C17" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="55" t="s">
         <v>44</v>
       </c>
-      <c r="D17" s="56" t="s">
+      <c r="E17" s="56"/>
+      <c r="F17" s="57"/>
+      <c r="G17" s="53"/>
+      <c r="H17" s="58" t="s">
         <v>45</v>
       </c>
-      <c r="E17" s="57"/>
-      <c r="F17" s="58"/>
-      <c r="G17" s="54"/>
-      <c r="H17" s="59" t="s">
+      <c r="I17" s="58" t="s">
         <v>46</v>
       </c>
-      <c r="I17" s="59" t="s">
+      <c r="J17" s="54" t="s">
         <v>47</v>
       </c>
-      <c r="J17" s="55" t="s">
+      <c r="K17" s="59"/>
+    </row>
+    <row r="18" ht="12.75" customHeight="1">
+      <c r="A18" s="25"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="K17" s="60"/>
-    </row>
-    <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="26"/>
-      <c r="B18" s="54"/>
-      <c r="C18" s="54"/>
-      <c r="D18" s="56" t="s">
+      <c r="E18" s="56"/>
+      <c r="F18" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="E18" s="57"/>
-      <c r="F18" s="61" t="s">
+      <c r="G18" s="53"/>
+      <c r="H18" s="53"/>
+      <c r="I18" s="53"/>
+      <c r="J18" s="53"/>
+      <c r="K18" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="54"/>
-      <c r="H18" s="54"/>
-      <c r="I18" s="54"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="52" t="s">
+    </row>
+    <row r="19" ht="12.75" customHeight="1">
+      <c r="A19" s="25"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="61" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="26"/>
-      <c r="B19" s="60"/>
-      <c r="C19" s="60"/>
-      <c r="D19" s="62" t="s">
+      <c r="E19" s="62"/>
+      <c r="F19" s="59"/>
+      <c r="G19" s="59"/>
+      <c r="H19" s="59"/>
+      <c r="I19" s="59"/>
+      <c r="J19" s="59"/>
+      <c r="K19" s="59"/>
+    </row>
+    <row r="20" ht="12.75" customHeight="1">
+      <c r="A20" s="25"/>
+      <c r="B20" s="48"/>
+      <c r="C20" s="48"/>
+      <c r="D20" s="49" t="s">
         <v>52</v>
       </c>
-      <c r="E19" s="63"/>
-      <c r="F19" s="60"/>
-      <c r="G19" s="60"/>
-      <c r="H19" s="60"/>
-      <c r="I19" s="60"/>
-      <c r="J19" s="60"/>
-      <c r="K19" s="60"/>
-    </row>
-    <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="26"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="50" t="s">
+      <c r="E20" s="50"/>
+      <c r="F20" s="51" t="s">
         <v>53</v>
       </c>
-      <c r="E20" s="51"/>
-      <c r="F20" s="52" t="s">
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="48"/>
+      <c r="K20" s="51" t="s">
         <v>54</v>
       </c>
-      <c r="G20" s="53"/>
-      <c r="H20" s="53"/>
-      <c r="I20" s="53"/>
-      <c r="J20" s="49"/>
-      <c r="K20" s="52" t="s">
-        <v>55</v>
-      </c>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="26"/>
-      <c r="B21" s="54">
+      <c r="A21" s="25"/>
+      <c r="B21" s="53">
         <f>B17+1</f>
         <v>3</v>
       </c>
-      <c r="C21" s="55" t="s">
+      <c r="C21" s="54" t="s">
+        <v>55</v>
+      </c>
+      <c r="D21" s="55" t="s">
         <v>56</v>
       </c>
-      <c r="D21" s="56" t="s">
+      <c r="E21" s="56"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="53"/>
+      <c r="H21" s="58" t="s">
         <v>57</v>
       </c>
-      <c r="E21" s="57"/>
-      <c r="F21" s="58"/>
-      <c r="G21" s="54"/>
-      <c r="H21" s="59" t="s">
+      <c r="I21" s="58" t="s">
         <v>58</v>
       </c>
-      <c r="I21" s="59" t="s">
+      <c r="J21" s="54" t="s">
+        <v>59</v>
+      </c>
+      <c r="K21" s="59"/>
+    </row>
+    <row r="22" ht="12.75" customHeight="1">
+      <c r="A22" s="25"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="53"/>
+      <c r="D22" s="55" t="s">
         <v>60</v>
       </c>
-      <c r="J21" s="55" t="s">
+      <c r="E22" s="56"/>
+      <c r="F22" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="K21" s="60"/>
-    </row>
-    <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="26"/>
-      <c r="B22" s="54"/>
-      <c r="C22" s="54"/>
-      <c r="D22" s="56" t="s">
+      <c r="G22" s="53"/>
+      <c r="H22" s="53"/>
+      <c r="I22" s="53"/>
+      <c r="J22" s="53"/>
+      <c r="K22" s="51" t="s">
         <v>62</v>
       </c>
-      <c r="E22" s="57"/>
-      <c r="F22" s="61" t="s">
+    </row>
+    <row r="23" ht="12.75" customHeight="1">
+      <c r="A23" s="25"/>
+      <c r="B23" s="59"/>
+      <c r="C23" s="59"/>
+      <c r="D23" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="G22" s="54"/>
-      <c r="H22" s="54"/>
-      <c r="I22" s="54"/>
-      <c r="J22" s="54"/>
-      <c r="K22" s="52" t="s">
+      <c r="E23" s="62"/>
+      <c r="F23" s="59"/>
+      <c r="G23" s="59"/>
+      <c r="H23" s="59"/>
+      <c r="I23" s="59"/>
+      <c r="J23" s="59"/>
+      <c r="K23" s="59"/>
+    </row>
+    <row r="24" ht="12.75" customHeight="1">
+      <c r="A24" s="25"/>
+      <c r="B24" s="48"/>
+      <c r="C24" s="48"/>
+      <c r="D24" s="49" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="26"/>
-      <c r="B23" s="60"/>
-      <c r="C23" s="60"/>
-      <c r="D23" s="62" t="s">
+      <c r="E24" s="50"/>
+      <c r="F24" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="E23" s="63"/>
-      <c r="F23" s="60"/>
-      <c r="G23" s="60"/>
-      <c r="H23" s="60"/>
-      <c r="I23" s="60"/>
-      <c r="J23" s="60"/>
-      <c r="K23" s="60"/>
-    </row>
-    <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="26"/>
-      <c r="B24" s="49"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="50" t="s">
+      <c r="G24" s="52"/>
+      <c r="H24" s="52"/>
+      <c r="I24" s="52"/>
+      <c r="J24" s="48"/>
+      <c r="K24" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="E24" s="51"/>
-      <c r="F24" s="52" t="s">
-        <v>67</v>
-      </c>
-      <c r="G24" s="53"/>
-      <c r="H24" s="53"/>
-      <c r="I24" s="53"/>
-      <c r="J24" s="49"/>
-      <c r="K24" s="52" t="s">
-        <v>68</v>
-      </c>
     </row>
     <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="26"/>
-      <c r="B25" s="54">
+      <c r="A25" s="25"/>
+      <c r="B25" s="53">
         <f>B21+1</f>
         <v>4</v>
       </c>
-      <c r="C25" s="55" t="s">
+      <c r="C25" s="54" t="s">
+        <v>67</v>
+      </c>
+      <c r="D25" s="55" t="s">
+        <v>68</v>
+      </c>
+      <c r="E25" s="56"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="53"/>
+      <c r="H25" s="58" t="s">
         <v>69</v>
       </c>
-      <c r="D25" s="56" t="s">
+      <c r="I25" s="58" t="s">
         <v>70</v>
       </c>
-      <c r="E25" s="57"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="54"/>
-      <c r="H25" s="59" t="s">
+      <c r="J25" s="54" t="s">
         <v>71</v>
       </c>
-      <c r="I25" s="59" t="s">
+      <c r="K25" s="59"/>
+    </row>
+    <row r="26" ht="12.75" customHeight="1">
+      <c r="A26" s="25"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="55" t="s">
         <v>72</v>
       </c>
-      <c r="J25" s="55" t="s">
+      <c r="E26" s="56"/>
+      <c r="F26" s="60" t="s">
         <v>73</v>
       </c>
-      <c r="K25" s="60"/>
-    </row>
-    <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="26"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="54"/>
-      <c r="D26" s="56" t="s">
+      <c r="G26" s="53"/>
+      <c r="H26" s="53"/>
+      <c r="I26" s="53"/>
+      <c r="J26" s="53"/>
+      <c r="K26" s="51" t="s">
         <v>74</v>
       </c>
-      <c r="E26" s="57"/>
-      <c r="F26" s="61" t="s">
+    </row>
+    <row r="27" ht="12.75" customHeight="1">
+      <c r="A27" s="25"/>
+      <c r="B27" s="59"/>
+      <c r="C27" s="59"/>
+      <c r="D27" s="61" t="s">
         <v>75</v>
       </c>
-      <c r="G26" s="54"/>
-      <c r="H26" s="54"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="54"/>
-      <c r="K26" s="52" t="s">
+      <c r="E27" s="62"/>
+      <c r="F27" s="59"/>
+      <c r="G27" s="59"/>
+      <c r="H27" s="59"/>
+      <c r="I27" s="59"/>
+      <c r="J27" s="59"/>
+      <c r="K27" s="59"/>
+    </row>
+    <row r="28" ht="12.75" customHeight="1">
+      <c r="A28" s="25"/>
+      <c r="B28" s="48"/>
+      <c r="C28" s="48"/>
+      <c r="D28" s="49" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" s="26"/>
-      <c r="B27" s="60"/>
-      <c r="C27" s="60"/>
-      <c r="D27" s="62" t="s">
+      <c r="E28" s="50"/>
+      <c r="F28" s="51" t="s">
         <v>77</v>
       </c>
-      <c r="E27" s="63"/>
-      <c r="F27" s="60"/>
-      <c r="G27" s="60"/>
-      <c r="H27" s="60"/>
-      <c r="I27" s="60"/>
-      <c r="J27" s="60"/>
-      <c r="K27" s="60"/>
-    </row>
-    <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" s="26"/>
-      <c r="B28" s="49"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="50" t="s">
+      <c r="G28" s="52"/>
+      <c r="H28" s="52"/>
+      <c r="I28" s="52"/>
+      <c r="J28" s="48"/>
+      <c r="K28" s="51" t="s">
         <v>78</v>
       </c>
-      <c r="E28" s="51"/>
-      <c r="F28" s="52" t="s">
-        <v>79</v>
-      </c>
-      <c r="G28" s="53"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="53"/>
-      <c r="J28" s="49"/>
-      <c r="K28" s="52" t="s">
-        <v>80</v>
-      </c>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="26"/>
-      <c r="B29" s="54">
+      <c r="A29" s="25"/>
+      <c r="B29" s="53">
         <f>B25+1</f>
         <v>5</v>
       </c>
-      <c r="C29" s="55" t="s">
+      <c r="C29" s="54" t="s">
+        <v>79</v>
+      </c>
+      <c r="D29" s="55" t="s">
+        <v>80</v>
+      </c>
+      <c r="E29" s="56"/>
+      <c r="F29" s="57"/>
+      <c r="G29" s="53"/>
+      <c r="H29" s="58" t="s">
         <v>81</v>
       </c>
-      <c r="D29" s="56" t="s">
+      <c r="I29" s="58" t="s">
         <v>82</v>
       </c>
-      <c r="E29" s="57"/>
-      <c r="F29" s="58"/>
-      <c r="G29" s="54"/>
-      <c r="H29" s="59" t="s">
+      <c r="J29" s="54" t="s">
         <v>83</v>
       </c>
-      <c r="I29" s="59" t="s">
+      <c r="K29" s="59"/>
+    </row>
+    <row r="30" ht="12.75" customHeight="1">
+      <c r="A30" s="25"/>
+      <c r="B30" s="53"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="J29" s="55" t="s">
+      <c r="E30" s="56"/>
+      <c r="F30" s="60" t="s">
         <v>85</v>
       </c>
-      <c r="K29" s="60"/>
-    </row>
-    <row r="30" ht="12.75" customHeight="1">
-      <c r="A30" s="26"/>
-      <c r="B30" s="54"/>
-      <c r="C30" s="54"/>
-      <c r="D30" s="56" t="s">
+      <c r="G30" s="53"/>
+      <c r="H30" s="53"/>
+      <c r="I30" s="53"/>
+      <c r="J30" s="53"/>
+      <c r="K30" s="51" t="s">
         <v>86</v>
       </c>
-      <c r="E30" s="57"/>
-      <c r="F30" s="61" t="s">
+    </row>
+    <row r="31" ht="12.75" customHeight="1">
+      <c r="A31" s="25"/>
+      <c r="B31" s="59"/>
+      <c r="C31" s="59"/>
+      <c r="D31" s="61" t="s">
         <v>87</v>
       </c>
-      <c r="G30" s="54"/>
-      <c r="H30" s="54"/>
-      <c r="I30" s="54"/>
-      <c r="J30" s="54"/>
-      <c r="K30" s="52" t="s">
+      <c r="E31" s="62"/>
+      <c r="F31" s="59"/>
+      <c r="G31" s="59"/>
+      <c r="H31" s="59"/>
+      <c r="I31" s="59"/>
+      <c r="J31" s="59"/>
+      <c r="K31" s="59"/>
+    </row>
+    <row r="32" ht="12.75" customHeight="1">
+      <c r="A32" s="25"/>
+      <c r="B32" s="48"/>
+      <c r="C32" s="48"/>
+      <c r="D32" s="49" t="s">
         <v>88</v>
       </c>
-    </row>
-    <row r="31" ht="12.75" customHeight="1">
-      <c r="A31" s="26"/>
-      <c r="B31" s="60"/>
-      <c r="C31" s="60"/>
-      <c r="D31" s="62" t="s">
+      <c r="E32" s="50"/>
+      <c r="F32" s="51" t="s">
+        <v>89</v>
+      </c>
+      <c r="G32" s="52"/>
+      <c r="H32" s="52"/>
+      <c r="I32" s="52"/>
+      <c r="J32" s="48"/>
+      <c r="K32" s="51" t="s">
         <v>90</v>
       </c>
-      <c r="E31" s="63"/>
-      <c r="F31" s="60"/>
-      <c r="G31" s="60"/>
-      <c r="H31" s="60"/>
-      <c r="I31" s="60"/>
-      <c r="J31" s="60"/>
-      <c r="K31" s="60"/>
-    </row>
-    <row r="32" ht="12.75" customHeight="1">
-      <c r="A32" s="26"/>
-      <c r="B32" s="49"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="50" t="s">
-        <v>91</v>
-      </c>
-      <c r="E32" s="51"/>
-      <c r="F32" s="52" t="s">
-        <v>92</v>
-      </c>
-      <c r="G32" s="53"/>
-      <c r="H32" s="53"/>
-      <c r="I32" s="53"/>
-      <c r="J32" s="49"/>
-      <c r="K32" s="52" t="s">
-        <v>93</v>
-      </c>
     </row>
     <row r="33" ht="12.75" customHeight="1">
-      <c r="A33" s="26"/>
-      <c r="B33" s="54">
+      <c r="A33" s="25"/>
+      <c r="B33" s="53">
         <f>B29+1</f>
         <v>6</v>
       </c>
-      <c r="C33" s="55" t="s">
+      <c r="C33" s="54" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" s="55" t="s">
+        <v>92</v>
+      </c>
+      <c r="E33" s="56"/>
+      <c r="F33" s="57"/>
+      <c r="G33" s="53"/>
+      <c r="H33" s="58" t="s">
+        <v>93</v>
+      </c>
+      <c r="I33" s="58" t="s">
         <v>94</v>
       </c>
-      <c r="D33" s="56" t="s">
+      <c r="J33" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="E33" s="57"/>
-      <c r="F33" s="58"/>
-      <c r="G33" s="54"/>
-      <c r="H33" s="59" t="s">
+      <c r="K33" s="59"/>
+    </row>
+    <row r="34" ht="12.75" customHeight="1">
+      <c r="A34" s="25"/>
+      <c r="B34" s="53"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="55" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" s="56"/>
+      <c r="F34" s="60" t="s">
         <v>97</v>
       </c>
-      <c r="I33" s="59" t="s">
+      <c r="G34" s="53"/>
+      <c r="H34" s="53"/>
+      <c r="I34" s="53"/>
+      <c r="J34" s="53"/>
+      <c r="K34" s="51" t="s">
         <v>98</v>
       </c>
-      <c r="J33" s="55" t="s">
+    </row>
+    <row r="35" ht="12.75" customHeight="1">
+      <c r="A35" s="25"/>
+      <c r="B35" s="59"/>
+      <c r="C35" s="59"/>
+      <c r="D35" s="61" t="s">
+        <v>99</v>
+      </c>
+      <c r="E35" s="62"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="59"/>
+      <c r="H35" s="59"/>
+      <c r="I35" s="59"/>
+      <c r="J35" s="59"/>
+      <c r="K35" s="59"/>
+    </row>
+    <row r="36" ht="12.75" customHeight="1">
+      <c r="A36" s="25"/>
+      <c r="B36" s="48"/>
+      <c r="C36" s="48"/>
+      <c r="D36" s="49" t="s">
         <v>100</v>
       </c>
-      <c r="K33" s="60"/>
-    </row>
-    <row r="34" ht="12.75" customHeight="1">
-      <c r="A34" s="26"/>
-      <c r="B34" s="54"/>
-      <c r="C34" s="54"/>
-      <c r="D34" s="56" t="s">
+      <c r="E36" s="50"/>
+      <c r="F36" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="E34" s="57"/>
-      <c r="F34" s="61" t="s">
+      <c r="G36" s="52"/>
+      <c r="H36" s="52"/>
+      <c r="I36" s="52"/>
+      <c r="J36" s="48"/>
+      <c r="K36" s="51" t="s">
         <v>102</v>
       </c>
-      <c r="G34" s="54"/>
-      <c r="H34" s="54"/>
-      <c r="I34" s="54"/>
-      <c r="J34" s="54"/>
-      <c r="K34" s="52" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="35" ht="12.75" customHeight="1">
-      <c r="A35" s="26"/>
-      <c r="B35" s="60"/>
-      <c r="C35" s="60"/>
-      <c r="D35" s="62" t="s">
-        <v>104</v>
-      </c>
-      <c r="E35" s="63"/>
-      <c r="F35" s="60"/>
-      <c r="G35" s="60"/>
-      <c r="H35" s="60"/>
-      <c r="I35" s="60"/>
-      <c r="J35" s="60"/>
-      <c r="K35" s="60"/>
-    </row>
-    <row r="36" ht="12.75" customHeight="1">
-      <c r="A36" s="26"/>
-      <c r="B36" s="49"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="50" t="s">
-        <v>105</v>
-      </c>
-      <c r="E36" s="51"/>
-      <c r="F36" s="52" t="s">
-        <v>106</v>
-      </c>
-      <c r="G36" s="53"/>
-      <c r="H36" s="53"/>
-      <c r="I36" s="53"/>
-      <c r="J36" s="49"/>
-      <c r="K36" s="52" t="s">
-        <v>107</v>
-      </c>
     </row>
     <row r="37" ht="12.75" customHeight="1">
-      <c r="A37" s="26"/>
-      <c r="B37" s="54">
+      <c r="A37" s="25"/>
+      <c r="B37" s="53">
         <f>B33+1</f>
         <v>7</v>
       </c>
-      <c r="C37" s="55" t="s">
+      <c r="C37" s="54" t="s">
+        <v>103</v>
+      </c>
+      <c r="D37" s="55" t="s">
+        <v>104</v>
+      </c>
+      <c r="E37" s="56"/>
+      <c r="F37" s="63"/>
+      <c r="G37" s="53"/>
+      <c r="H37" s="58" t="s">
+        <v>105</v>
+      </c>
+      <c r="I37" s="58" t="s">
+        <v>106</v>
+      </c>
+      <c r="J37" s="54" t="s">
+        <v>107</v>
+      </c>
+      <c r="K37" s="59"/>
+    </row>
+    <row r="38" ht="12.75" customHeight="1">
+      <c r="A38" s="25"/>
+      <c r="B38" s="53"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="55" t="s">
+        <v>108</v>
+      </c>
+      <c r="E38" s="56"/>
+      <c r="F38" s="60" t="s">
+        <v>109</v>
+      </c>
+      <c r="G38" s="53"/>
+      <c r="H38" s="53"/>
+      <c r="I38" s="53"/>
+      <c r="J38" s="53"/>
+      <c r="K38" s="51" t="s">
         <v>110</v>
       </c>
-      <c r="D37" s="56" t="s">
+    </row>
+    <row r="39" ht="12.75" customHeight="1">
+      <c r="A39" s="25"/>
+      <c r="B39" s="59"/>
+      <c r="C39" s="59"/>
+      <c r="D39" s="61" t="s">
         <v>111</v>
       </c>
-      <c r="E37" s="57"/>
-      <c r="F37" s="72"/>
-      <c r="G37" s="54"/>
-      <c r="H37" s="59" t="s">
+      <c r="E39" s="62"/>
+      <c r="F39" s="59"/>
+      <c r="G39" s="59"/>
+      <c r="H39" s="59"/>
+      <c r="I39" s="59"/>
+      <c r="J39" s="59"/>
+      <c r="K39" s="59"/>
+    </row>
+    <row r="40" ht="12.75" customHeight="1">
+      <c r="A40" s="25"/>
+      <c r="B40" s="48"/>
+      <c r="C40" s="48"/>
+      <c r="D40" s="49" t="s">
         <v>112</v>
       </c>
-      <c r="I37" s="59" t="s">
+      <c r="E40" s="50"/>
+      <c r="F40" s="51" t="s">
         <v>113</v>
       </c>
-      <c r="J37" s="55" t="s">
+      <c r="G40" s="52"/>
+      <c r="H40" s="52"/>
+      <c r="I40" s="52"/>
+      <c r="J40" s="48"/>
+      <c r="K40" s="51" t="s">
         <v>114</v>
       </c>
-      <c r="K37" s="60"/>
-    </row>
-    <row r="38" ht="12.75" customHeight="1">
-      <c r="A38" s="26"/>
-      <c r="B38" s="54"/>
-      <c r="C38" s="54"/>
-      <c r="D38" s="56" t="s">
-        <v>115</v>
-      </c>
-      <c r="E38" s="57"/>
-      <c r="F38" s="61" t="s">
-        <v>116</v>
-      </c>
-      <c r="G38" s="54"/>
-      <c r="H38" s="54"/>
-      <c r="I38" s="54"/>
-      <c r="J38" s="54"/>
-      <c r="K38" s="52" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="39" ht="12.75" customHeight="1">
-      <c r="A39" s="26"/>
-      <c r="B39" s="60"/>
-      <c r="C39" s="60"/>
-      <c r="D39" s="62" t="s">
-        <v>118</v>
-      </c>
-      <c r="E39" s="63"/>
-      <c r="F39" s="60"/>
-      <c r="G39" s="60"/>
-      <c r="H39" s="60"/>
-      <c r="I39" s="60"/>
-      <c r="J39" s="60"/>
-      <c r="K39" s="60"/>
-    </row>
-    <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="26"/>
-      <c r="B40" s="49"/>
-      <c r="C40" s="49"/>
-      <c r="D40" s="50" t="s">
-        <v>119</v>
-      </c>
-      <c r="E40" s="51"/>
-      <c r="F40" s="52" t="s">
-        <v>120</v>
-      </c>
-      <c r="G40" s="53"/>
-      <c r="H40" s="53"/>
-      <c r="I40" s="53"/>
-      <c r="J40" s="49"/>
-      <c r="K40" s="52" t="s">
-        <v>121</v>
-      </c>
     </row>
     <row r="41" ht="12.75" customHeight="1">
-      <c r="A41" s="26"/>
-      <c r="B41" s="54">
+      <c r="A41" s="25"/>
+      <c r="B41" s="53">
         <f>B37+1</f>
         <v>8</v>
       </c>
-      <c r="C41" s="55" t="s">
+      <c r="C41" s="54" t="s">
+        <v>115</v>
+      </c>
+      <c r="D41" s="55" t="s">
+        <v>116</v>
+      </c>
+      <c r="E41" s="56"/>
+      <c r="F41" s="57"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="58" t="s">
+        <v>117</v>
+      </c>
+      <c r="I41" s="58" t="s">
+        <v>118</v>
+      </c>
+      <c r="J41" s="54" t="s">
+        <v>119</v>
+      </c>
+      <c r="K41" s="59"/>
+    </row>
+    <row r="42" ht="12.75" customHeight="1">
+      <c r="A42" s="64"/>
+      <c r="B42" s="53"/>
+      <c r="C42" s="53"/>
+      <c r="D42" s="55" t="s">
+        <v>120</v>
+      </c>
+      <c r="E42" s="56"/>
+      <c r="F42" s="60" t="s">
+        <v>121</v>
+      </c>
+      <c r="G42" s="53"/>
+      <c r="H42" s="53"/>
+      <c r="I42" s="53"/>
+      <c r="J42" s="53"/>
+      <c r="K42" s="51" t="s">
         <v>122</v>
       </c>
-      <c r="D41" s="56" t="s">
+    </row>
+    <row r="43" ht="12.75" customHeight="1">
+      <c r="A43" s="65"/>
+      <c r="B43" s="59"/>
+      <c r="C43" s="59"/>
+      <c r="D43" s="61" t="s">
         <v>123</v>
       </c>
-      <c r="E41" s="57"/>
-      <c r="F41" s="58"/>
-      <c r="G41" s="54"/>
-      <c r="H41" s="59" t="s">
-        <v>124</v>
-      </c>
-      <c r="I41" s="59" t="s">
-        <v>125</v>
-      </c>
-      <c r="J41" s="55" t="s">
-        <v>126</v>
-      </c>
-      <c r="K41" s="60"/>
-    </row>
-    <row r="42" ht="12.75" customHeight="1">
-      <c r="A42" s="76"/>
-      <c r="B42" s="54"/>
-      <c r="C42" s="54"/>
-      <c r="D42" s="56" t="s">
-        <v>128</v>
-      </c>
-      <c r="E42" s="57"/>
-      <c r="F42" s="61" t="s">
-        <v>129</v>
-      </c>
-      <c r="G42" s="54"/>
-      <c r="H42" s="54"/>
-      <c r="I42" s="54"/>
-      <c r="J42" s="54"/>
-      <c r="K42" s="52" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="78"/>
-      <c r="B43" s="60"/>
-      <c r="C43" s="60"/>
-      <c r="D43" s="62" t="s">
-        <v>143</v>
-      </c>
-      <c r="E43" s="63"/>
-      <c r="F43" s="60"/>
-      <c r="G43" s="60"/>
-      <c r="H43" s="60"/>
-      <c r="I43" s="60"/>
-      <c r="J43" s="60"/>
-      <c r="K43" s="60"/>
+      <c r="E43" s="62"/>
+      <c r="F43" s="59"/>
+      <c r="G43" s="59"/>
+      <c r="H43" s="59"/>
+      <c r="I43" s="59"/>
+      <c r="J43" s="59"/>
+      <c r="K43" s="59"/>
     </row>
     <row r="44" ht="12.75" customHeight="1">
-      <c r="A44" s="80"/>
-      <c r="B44" s="80"/>
-      <c r="C44" s="80"/>
-      <c r="D44" s="80"/>
-      <c r="E44" s="80"/>
-      <c r="F44" s="80"/>
-      <c r="G44" s="80"/>
-      <c r="H44" s="80"/>
-      <c r="I44" s="80"/>
-      <c r="J44" s="80"/>
-      <c r="K44" s="80"/>
+      <c r="A44" s="66"/>
+      <c r="B44" s="66"/>
+      <c r="C44" s="66"/>
+      <c r="D44" s="66"/>
+      <c r="E44" s="66"/>
+      <c r="F44" s="66"/>
+      <c r="G44" s="66"/>
+      <c r="H44" s="66"/>
+      <c r="I44" s="66"/>
+      <c r="J44" s="66"/>
+      <c r="K44" s="66"/>
     </row>
     <row r="45" ht="15.75" customHeight="1"/>
     <row r="46" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Use Scope for header dates
</commit_message>
<xml_diff>
--- a/api/Templates/CSFunding 2018-19 Bulk Invoice Summary - Template.xlsx
+++ b/api/Templates/CSFunding 2018-19 Bulk Invoice Summary - Template.xlsx
@@ -23,7 +23,7 @@
     <t>Individual Student Information Sheet</t>
   </si>
   <si>
-    <t>For the Months of July ${FirstYear} to ${AsOfMonth} ${AsOfYear}</t>
+    <t>For the Months of July ${FirstYear} to ${ScopeMonth} ${ScopeYear}</t>
   </si>
   <si>
     <t>${Districts[0].SchoolDistrict.Aun}</t>
@@ -389,52 +389,7 @@
     <t>Summary Information Sheet</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color rgb="FF000000"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t xml:space="preserve">For the Months of </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color rgb="FF800000"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t xml:space="preserve">July </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color rgb="FF000000"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t>2018 to</t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color rgb="FF800000"/>
-        <sz val="10.0"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <rFont val="Arial"/>
-        <b/>
-        <color rgb="FF800000"/>
-        <sz val="10.0"/>
-        <u/>
-      </rPr>
-      <t>${AsOfMonth} ${AsOfYear}</t>
-    </r>
+    <t>For the Months of July 2018 to ${ScopeMonth} ${ScopeYear}</t>
   </si>
   <si>
     <t>Invoice Prep Date:</t>
@@ -1440,7 +1395,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="151">
+  <cellXfs count="152">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -1453,18 +1408,18 @@
     <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="2" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="3" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
     <xf borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
@@ -1485,6 +1440,9 @@
     </xf>
     <xf borderId="6" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="5" fillId="2" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
@@ -1941,14 +1899,14 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="6"/>
+      <c r="A1" s="4"/>
       <c r="B1" s="2"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="4" t="s">
+      <c r="G1" s="5"/>
+      <c r="H1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="I1" s="2"/>
@@ -1956,16 +1914,16 @@
       <c r="K1" s="2"/>
       <c r="L1" s="2"/>
       <c r="M1" s="2"/>
-      <c r="N1" s="67"/>
+      <c r="N1" s="68"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="68"/>
+      <c r="A2" s="69"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
       <c r="E2" s="12"/>
       <c r="F2" s="12"/>
-      <c r="G2" s="17"/>
+      <c r="G2" s="18"/>
       <c r="H2" s="13" t="s">
         <v>1</v>
       </c>
@@ -1977,13 +1935,13 @@
       <c r="N2" s="14"/>
     </row>
     <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="68"/>
+      <c r="A3" s="69"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
       <c r="F3" s="12"/>
-      <c r="G3" s="17"/>
+      <c r="G3" s="18"/>
       <c r="H3" s="13" t="s">
         <v>124</v>
       </c>
@@ -1995,14 +1953,14 @@
       <c r="N3" s="14"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="68"/>
+      <c r="A4" s="69"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
       <c r="F4" s="12"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="13" t="s">
+      <c r="G4" s="18"/>
+      <c r="H4" s="15" t="s">
         <v>125</v>
       </c>
       <c r="I4" s="12"/>
@@ -2013,848 +1971,848 @@
       <c r="N4" s="14"/>
     </row>
     <row r="5" ht="19.5" customHeight="1">
-      <c r="A5" s="69"/>
-      <c r="B5" s="70"/>
-      <c r="C5" s="70"/>
-      <c r="D5" s="70"/>
-      <c r="E5" s="70"/>
-      <c r="F5" s="70"/>
-      <c r="G5" s="70"/>
-      <c r="H5" s="70"/>
-      <c r="I5" s="70"/>
-      <c r="J5" s="70"/>
-      <c r="K5" s="70"/>
-      <c r="L5" s="70"/>
-      <c r="M5" s="70"/>
-      <c r="N5" s="71"/>
+      <c r="A5" s="70"/>
+      <c r="B5" s="71"/>
+      <c r="C5" s="71"/>
+      <c r="D5" s="71"/>
+      <c r="E5" s="71"/>
+      <c r="F5" s="71"/>
+      <c r="G5" s="71"/>
+      <c r="H5" s="71"/>
+      <c r="I5" s="71"/>
+      <c r="J5" s="71"/>
+      <c r="K5" s="71"/>
+      <c r="L5" s="71"/>
+      <c r="M5" s="71"/>
+      <c r="N5" s="72"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
-      <c r="A6" s="72" t="s">
+      <c r="A6" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="20"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="70"/>
-      <c r="H6" s="17"/>
-      <c r="I6" s="17"/>
-      <c r="J6" s="17"/>
-      <c r="K6" s="73" t="s">
+      <c r="B6" s="21"/>
+      <c r="C6" s="18"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="71"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="74" t="s">
         <v>126</v>
       </c>
-      <c r="L6" s="17"/>
-      <c r="M6" s="17"/>
-      <c r="N6" s="22" t="s">
+      <c r="L6" s="18"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="23" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" ht="13.5" customHeight="1">
-      <c r="A7" s="72" t="s">
+      <c r="A7" s="73" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="20"/>
-      <c r="C7" s="17"/>
-      <c r="D7" s="17"/>
-      <c r="E7" s="17"/>
-      <c r="F7" s="18"/>
-      <c r="G7" s="18"/>
-      <c r="H7" s="18"/>
-      <c r="I7" s="18"/>
-      <c r="J7" s="18"/>
-      <c r="K7" s="73" t="s">
+      <c r="B7" s="21"/>
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+      <c r="E7" s="18"/>
+      <c r="F7" s="19"/>
+      <c r="G7" s="19"/>
+      <c r="H7" s="19"/>
+      <c r="I7" s="19"/>
+      <c r="J7" s="19"/>
+      <c r="K7" s="74" t="s">
         <v>127</v>
       </c>
-      <c r="L7" s="17"/>
-      <c r="M7" s="17"/>
-      <c r="N7" s="22" t="s">
+      <c r="L7" s="18"/>
+      <c r="M7" s="18"/>
+      <c r="N7" s="23" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="8" ht="13.5" customHeight="1">
-      <c r="A8" s="74"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="17"/>
-      <c r="D8" s="17"/>
-      <c r="E8" s="17"/>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="18"/>
-      <c r="I8" s="18"/>
-      <c r="J8" s="18"/>
-      <c r="K8" s="73" t="s">
+      <c r="A8" s="75"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="18"/>
+      <c r="D8" s="18"/>
+      <c r="E8" s="18"/>
+      <c r="F8" s="19"/>
+      <c r="G8" s="19"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="19"/>
+      <c r="J8" s="19"/>
+      <c r="K8" s="74" t="s">
         <v>129</v>
       </c>
-      <c r="L8" s="17"/>
-      <c r="M8" s="17"/>
-      <c r="N8" s="22" t="s">
+      <c r="L8" s="18"/>
+      <c r="M8" s="18"/>
+      <c r="N8" s="23" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1">
       <c r="A9" s="8"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="75"/>
-      <c r="D9" s="75"/>
-      <c r="E9" s="75"/>
-      <c r="F9" s="75"/>
-      <c r="G9" s="75"/>
-      <c r="H9" s="75"/>
-      <c r="I9" s="75"/>
-      <c r="J9" s="75"/>
-      <c r="K9" s="17"/>
-      <c r="L9" s="17"/>
-      <c r="M9" s="17"/>
-      <c r="N9" s="71"/>
+      <c r="B9" s="19"/>
+      <c r="C9" s="76"/>
+      <c r="D9" s="76"/>
+      <c r="E9" s="76"/>
+      <c r="F9" s="76"/>
+      <c r="G9" s="76"/>
+      <c r="H9" s="76"/>
+      <c r="I9" s="76"/>
+      <c r="J9" s="76"/>
+      <c r="K9" s="18"/>
+      <c r="L9" s="18"/>
+      <c r="M9" s="18"/>
+      <c r="N9" s="72"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
       <c r="A10" s="8"/>
-      <c r="B10" s="76"/>
-      <c r="C10" s="77"/>
-      <c r="D10" s="77"/>
-      <c r="E10" s="77"/>
-      <c r="F10" s="77"/>
-      <c r="G10" s="77"/>
-      <c r="H10" s="77"/>
-      <c r="I10" s="77"/>
-      <c r="J10" s="77"/>
-      <c r="K10" s="23"/>
-      <c r="L10" s="23"/>
-      <c r="M10" s="23"/>
-      <c r="N10" s="71"/>
+      <c r="B10" s="77"/>
+      <c r="C10" s="78"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="78"/>
+      <c r="F10" s="78"/>
+      <c r="G10" s="78"/>
+      <c r="H10" s="78"/>
+      <c r="I10" s="78"/>
+      <c r="J10" s="78"/>
+      <c r="K10" s="24"/>
+      <c r="L10" s="24"/>
+      <c r="M10" s="24"/>
+      <c r="N10" s="72"/>
     </row>
     <row r="11" ht="39.0" customHeight="1">
-      <c r="A11" s="78"/>
-      <c r="B11" s="79" t="s">
+      <c r="A11" s="79"/>
+      <c r="B11" s="80" t="s">
         <v>131</v>
       </c>
-      <c r="C11" s="79" t="s">
+      <c r="C11" s="80" t="s">
         <v>132</v>
       </c>
-      <c r="D11" s="79" t="s">
+      <c r="D11" s="80" t="s">
         <v>133</v>
       </c>
-      <c r="E11" s="79" t="s">
+      <c r="E11" s="80" t="s">
         <v>134</v>
       </c>
-      <c r="F11" s="79" t="s">
+      <c r="F11" s="80" t="s">
         <v>135</v>
       </c>
-      <c r="G11" s="79" t="s">
+      <c r="G11" s="80" t="s">
         <v>136</v>
       </c>
-      <c r="H11" s="79" t="s">
+      <c r="H11" s="80" t="s">
         <v>137</v>
       </c>
-      <c r="I11" s="79" t="s">
+      <c r="I11" s="80" t="s">
         <v>138</v>
       </c>
-      <c r="J11" s="79" t="s">
+      <c r="J11" s="80" t="s">
         <v>139</v>
       </c>
-      <c r="K11" s="79" t="s">
+      <c r="K11" s="80" t="s">
         <v>140</v>
       </c>
-      <c r="L11" s="79" t="s">
+      <c r="L11" s="80" t="s">
         <v>141</v>
       </c>
-      <c r="M11" s="79" t="s">
+      <c r="M11" s="80" t="s">
         <v>142</v>
       </c>
-      <c r="N11" s="80" t="s">
+      <c r="N11" s="81" t="s">
         <v>143</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="81" t="s">
+      <c r="A12" s="82" t="s">
         <v>144</v>
       </c>
-      <c r="B12" s="82" t="s">
+      <c r="B12" s="83" t="s">
         <v>145</v>
       </c>
-      <c r="C12" s="82" t="s">
+      <c r="C12" s="83" t="s">
         <v>146</v>
       </c>
-      <c r="D12" s="82" t="s">
+      <c r="D12" s="83" t="s">
         <v>147</v>
       </c>
-      <c r="E12" s="82" t="s">
+      <c r="E12" s="83" t="s">
         <v>148</v>
       </c>
-      <c r="F12" s="82" t="s">
+      <c r="F12" s="83" t="s">
         <v>149</v>
       </c>
-      <c r="G12" s="82" t="s">
+      <c r="G12" s="83" t="s">
         <v>150</v>
       </c>
-      <c r="H12" s="82" t="s">
+      <c r="H12" s="83" t="s">
         <v>151</v>
       </c>
-      <c r="I12" s="82" t="s">
+      <c r="I12" s="83" t="s">
         <v>152</v>
       </c>
-      <c r="J12" s="82" t="s">
+      <c r="J12" s="83" t="s">
         <v>153</v>
       </c>
-      <c r="K12" s="82" t="s">
+      <c r="K12" s="83" t="s">
         <v>154</v>
       </c>
-      <c r="L12" s="82" t="s">
+      <c r="L12" s="83" t="s">
         <v>155</v>
       </c>
-      <c r="M12" s="83" t="s">
+      <c r="M12" s="84" t="s">
         <v>156</v>
       </c>
-      <c r="N12" s="84" t="str">
+      <c r="N12" s="85" t="str">
         <f t="shared" ref="N12:N13" si="1">ROUND(SUMIF(B12:L12,"&gt;0")*M12/12,2)</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="81" t="s">
+      <c r="A13" s="82" t="s">
         <v>157</v>
       </c>
-      <c r="B13" s="82" t="s">
+      <c r="B13" s="83" t="s">
         <v>158</v>
       </c>
-      <c r="C13" s="82" t="s">
+      <c r="C13" s="83" t="s">
         <v>159</v>
       </c>
-      <c r="D13" s="82" t="s">
+      <c r="D13" s="83" t="s">
         <v>160</v>
       </c>
-      <c r="E13" s="82" t="s">
+      <c r="E13" s="83" t="s">
         <v>161</v>
       </c>
-      <c r="F13" s="82" t="s">
+      <c r="F13" s="83" t="s">
         <v>162</v>
       </c>
-      <c r="G13" s="82" t="s">
+      <c r="G13" s="83" t="s">
         <v>163</v>
       </c>
-      <c r="H13" s="82" t="s">
+      <c r="H13" s="83" t="s">
         <v>164</v>
       </c>
-      <c r="I13" s="82" t="s">
+      <c r="I13" s="83" t="s">
         <v>165</v>
       </c>
-      <c r="J13" s="82" t="s">
+      <c r="J13" s="83" t="s">
         <v>166</v>
       </c>
-      <c r="K13" s="82" t="s">
+      <c r="K13" s="83" t="s">
         <v>167</v>
       </c>
-      <c r="L13" s="82" t="s">
+      <c r="L13" s="83" t="s">
         <v>168</v>
       </c>
-      <c r="M13" s="83" t="s">
+      <c r="M13" s="84" t="s">
         <v>169</v>
       </c>
-      <c r="N13" s="84" t="str">
+      <c r="N13" s="85" t="str">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="85"/>
-      <c r="B14" s="86"/>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
-      <c r="J14" s="86"/>
-      <c r="K14" s="86"/>
-      <c r="L14" s="86"/>
-      <c r="M14" s="86"/>
-      <c r="N14" s="87"/>
+      <c r="A14" s="86"/>
+      <c r="B14" s="87"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="87"/>
+      <c r="E14" s="87"/>
+      <c r="F14" s="87"/>
+      <c r="G14" s="87"/>
+      <c r="H14" s="87"/>
+      <c r="I14" s="87"/>
+      <c r="J14" s="87"/>
+      <c r="K14" s="87"/>
+      <c r="L14" s="87"/>
+      <c r="M14" s="87"/>
+      <c r="N14" s="88"/>
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="8"/>
-      <c r="B15" s="17"/>
-      <c r="C15" s="17"/>
-      <c r="D15" s="17"/>
-      <c r="E15" s="17"/>
-      <c r="F15" s="17"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="17"/>
-      <c r="I15" s="17"/>
-      <c r="J15" s="17"/>
-      <c r="K15" s="17"/>
-      <c r="L15" s="88"/>
-      <c r="M15" s="89" t="s">
+      <c r="B15" s="18"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="18"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="89"/>
+      <c r="M15" s="90" t="s">
         <v>170</v>
       </c>
-      <c r="N15" s="90" t="str">
+      <c r="N15" s="91" t="str">
         <f>SUM(N12:N13)</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="16" ht="13.5" customHeight="1">
       <c r="A16" s="8"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="17"/>
-      <c r="D16" s="17"/>
-      <c r="E16" s="17"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="17"/>
-      <c r="I16" s="17"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="17"/>
-      <c r="L16" s="17"/>
-      <c r="M16" s="17"/>
-      <c r="N16" s="71"/>
+      <c r="B16" s="18"/>
+      <c r="C16" s="18"/>
+      <c r="D16" s="18"/>
+      <c r="E16" s="18"/>
+      <c r="F16" s="18"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="18"/>
+      <c r="I16" s="18"/>
+      <c r="J16" s="18"/>
+      <c r="K16" s="18"/>
+      <c r="L16" s="18"/>
+      <c r="M16" s="18"/>
+      <c r="N16" s="72"/>
     </row>
     <row r="17" ht="13.5" customHeight="1">
       <c r="A17" s="8"/>
-      <c r="B17" s="17"/>
-      <c r="C17" s="17"/>
-      <c r="D17" s="17"/>
-      <c r="E17" s="73" t="s">
+      <c r="B17" s="18"/>
+      <c r="C17" s="18"/>
+      <c r="D17" s="18"/>
+      <c r="E17" s="74" t="s">
         <v>171</v>
       </c>
-      <c r="F17" s="17"/>
-      <c r="G17" s="91" t="s">
+      <c r="F17" s="18"/>
+      <c r="G17" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="H17" s="91" t="s">
+      <c r="H17" s="92" t="s">
         <v>172</v>
       </c>
-      <c r="I17" s="73" t="s">
+      <c r="I17" s="74" t="s">
         <v>173</v>
       </c>
-      <c r="J17" s="17"/>
-      <c r="K17" s="73" t="s">
+      <c r="J17" s="18"/>
+      <c r="K17" s="74" t="s">
         <v>174</v>
       </c>
-      <c r="L17" s="17"/>
-      <c r="M17" s="17"/>
-      <c r="N17" s="71"/>
+      <c r="L17" s="18"/>
+      <c r="M17" s="18"/>
+      <c r="N17" s="72"/>
     </row>
     <row r="18" ht="13.5" customHeight="1">
       <c r="A18" s="8"/>
-      <c r="B18" s="17"/>
-      <c r="C18" s="92" t="s">
+      <c r="B18" s="18"/>
+      <c r="C18" s="93" t="s">
         <v>175</v>
       </c>
-      <c r="D18" s="93"/>
-      <c r="E18" s="94" t="s">
+      <c r="D18" s="94"/>
+      <c r="E18" s="95" t="s">
         <v>176</v>
       </c>
-      <c r="F18" s="93"/>
-      <c r="G18" s="95" t="s">
+      <c r="F18" s="94"/>
+      <c r="G18" s="96" t="s">
         <v>177</v>
       </c>
-      <c r="H18" s="95" t="s">
+      <c r="H18" s="96" t="s">
         <v>178</v>
       </c>
-      <c r="I18" s="94" t="s">
+      <c r="I18" s="95" t="s">
         <v>179</v>
       </c>
-      <c r="J18" s="96"/>
-      <c r="K18" s="94" t="s">
+      <c r="J18" s="97"/>
+      <c r="K18" s="95" t="s">
         <v>180</v>
       </c>
-      <c r="L18" s="96"/>
-      <c r="M18" s="17"/>
-      <c r="N18" s="71"/>
+      <c r="L18" s="97"/>
+      <c r="M18" s="18"/>
+      <c r="N18" s="72"/>
     </row>
     <row r="19" ht="13.5" customHeight="1">
       <c r="A19" s="8"/>
-      <c r="B19" s="17"/>
-      <c r="C19" s="97" t="s">
+      <c r="B19" s="18"/>
+      <c r="C19" s="98" t="s">
         <v>181</v>
       </c>
-      <c r="D19" s="98"/>
-      <c r="E19" s="99"/>
-      <c r="F19" s="100" t="s">
+      <c r="D19" s="99"/>
+      <c r="E19" s="100"/>
+      <c r="F19" s="101" t="s">
         <v>182</v>
       </c>
-      <c r="G19" s="101" t="s">
+      <c r="G19" s="102" t="s">
         <v>183</v>
       </c>
-      <c r="H19" s="102" t="s">
+      <c r="H19" s="103" t="s">
         <v>184</v>
       </c>
-      <c r="I19" s="103"/>
-      <c r="J19" s="104" t="s">
+      <c r="I19" s="104"/>
+      <c r="J19" s="105" t="s">
         <v>185</v>
       </c>
-      <c r="K19" s="105" t="s">
+      <c r="K19" s="106" t="s">
         <v>186</v>
       </c>
-      <c r="L19" s="106"/>
-      <c r="M19" s="17"/>
-      <c r="N19" s="71"/>
+      <c r="L19" s="107"/>
+      <c r="M19" s="18"/>
+      <c r="N19" s="72"/>
     </row>
     <row r="20" ht="13.5" customHeight="1">
       <c r="A20" s="8"/>
-      <c r="B20" s="17"/>
-      <c r="C20" s="107" t="s">
+      <c r="B20" s="18"/>
+      <c r="C20" s="108" t="s">
         <v>187</v>
       </c>
-      <c r="D20" s="108"/>
-      <c r="E20" s="109"/>
-      <c r="F20" s="110" t="s">
+      <c r="D20" s="109"/>
+      <c r="E20" s="110"/>
+      <c r="F20" s="111" t="s">
         <v>188</v>
       </c>
-      <c r="G20" s="111" t="s">
+      <c r="G20" s="112" t="s">
         <v>189</v>
       </c>
-      <c r="H20" s="112" t="s">
+      <c r="H20" s="113" t="s">
         <v>190</v>
       </c>
-      <c r="I20" s="113"/>
-      <c r="J20" s="114" t="s">
+      <c r="I20" s="114"/>
+      <c r="J20" s="115" t="s">
         <v>191</v>
       </c>
-      <c r="K20" s="115" t="s">
+      <c r="K20" s="116" t="s">
         <v>192</v>
       </c>
-      <c r="L20" s="116"/>
-      <c r="M20" s="17"/>
-      <c r="N20" s="71"/>
+      <c r="L20" s="117"/>
+      <c r="M20" s="18"/>
+      <c r="N20" s="72"/>
     </row>
     <row r="21" ht="13.5" customHeight="1">
       <c r="A21" s="8"/>
-      <c r="B21" s="17"/>
-      <c r="C21" s="73" t="s">
+      <c r="B21" s="18"/>
+      <c r="C21" s="74" t="s">
         <v>193</v>
       </c>
-      <c r="D21" s="117"/>
-      <c r="E21" s="109"/>
-      <c r="F21" s="110" t="s">
+      <c r="D21" s="118"/>
+      <c r="E21" s="110"/>
+      <c r="F21" s="111" t="s">
         <v>194</v>
       </c>
-      <c r="G21" s="111" t="s">
+      <c r="G21" s="112" t="s">
         <v>195</v>
       </c>
-      <c r="H21" s="112" t="s">
+      <c r="H21" s="113" t="s">
         <v>196</v>
       </c>
-      <c r="I21" s="113"/>
-      <c r="J21" s="114" t="s">
+      <c r="I21" s="114"/>
+      <c r="J21" s="115" t="s">
         <v>197</v>
       </c>
-      <c r="K21" s="115" t="s">
+      <c r="K21" s="116" t="s">
         <v>198</v>
       </c>
-      <c r="L21" s="116"/>
-      <c r="M21" s="17"/>
-      <c r="N21" s="71"/>
+      <c r="L21" s="117"/>
+      <c r="M21" s="18"/>
+      <c r="N21" s="72"/>
     </row>
     <row r="22" ht="13.5" customHeight="1">
       <c r="A22" s="8"/>
-      <c r="B22" s="17"/>
-      <c r="C22" s="73" t="s">
+      <c r="B22" s="18"/>
+      <c r="C22" s="74" t="s">
         <v>199</v>
       </c>
-      <c r="D22" s="117"/>
-      <c r="E22" s="109"/>
-      <c r="F22" s="110" t="s">
+      <c r="D22" s="118"/>
+      <c r="E22" s="110"/>
+      <c r="F22" s="111" t="s">
         <v>200</v>
       </c>
-      <c r="G22" s="111" t="s">
+      <c r="G22" s="112" t="s">
         <v>201</v>
       </c>
-      <c r="H22" s="112" t="s">
+      <c r="H22" s="113" t="s">
         <v>202</v>
       </c>
-      <c r="I22" s="113"/>
-      <c r="J22" s="114" t="s">
+      <c r="I22" s="114"/>
+      <c r="J22" s="115" t="s">
         <v>203</v>
       </c>
-      <c r="K22" s="115" t="s">
+      <c r="K22" s="116" t="s">
         <v>204</v>
       </c>
-      <c r="L22" s="116"/>
-      <c r="M22" s="17"/>
-      <c r="N22" s="71"/>
+      <c r="L22" s="117"/>
+      <c r="M22" s="18"/>
+      <c r="N22" s="72"/>
     </row>
     <row r="23" ht="13.5" customHeight="1">
       <c r="A23" s="8"/>
-      <c r="B23" s="17"/>
-      <c r="C23" s="73" t="s">
+      <c r="B23" s="18"/>
+      <c r="C23" s="74" t="s">
         <v>205</v>
       </c>
-      <c r="D23" s="117"/>
-      <c r="E23" s="109"/>
-      <c r="F23" s="110" t="s">
+      <c r="D23" s="118"/>
+      <c r="E23" s="110"/>
+      <c r="F23" s="111" t="s">
         <v>206</v>
       </c>
-      <c r="G23" s="111" t="s">
+      <c r="G23" s="112" t="s">
         <v>207</v>
       </c>
-      <c r="H23" s="112" t="s">
+      <c r="H23" s="113" t="s">
         <v>208</v>
       </c>
-      <c r="I23" s="113"/>
-      <c r="J23" s="114" t="s">
+      <c r="I23" s="114"/>
+      <c r="J23" s="115" t="s">
         <v>209</v>
       </c>
-      <c r="K23" s="115" t="s">
+      <c r="K23" s="116" t="s">
         <v>210</v>
       </c>
-      <c r="L23" s="116"/>
-      <c r="M23" s="17"/>
-      <c r="N23" s="118"/>
+      <c r="L23" s="117"/>
+      <c r="M23" s="18"/>
+      <c r="N23" s="119"/>
     </row>
     <row r="24" ht="13.5" customHeight="1">
       <c r="A24" s="8"/>
-      <c r="B24" s="17"/>
-      <c r="C24" s="73" t="s">
+      <c r="B24" s="18"/>
+      <c r="C24" s="74" t="s">
         <v>211</v>
       </c>
-      <c r="D24" s="117"/>
-      <c r="E24" s="109"/>
-      <c r="F24" s="110" t="s">
+      <c r="D24" s="118"/>
+      <c r="E24" s="110"/>
+      <c r="F24" s="111" t="s">
         <v>212</v>
       </c>
-      <c r="G24" s="111" t="s">
+      <c r="G24" s="112" t="s">
         <v>213</v>
       </c>
-      <c r="H24" s="112" t="s">
+      <c r="H24" s="113" t="s">
         <v>214</v>
       </c>
-      <c r="I24" s="113"/>
-      <c r="J24" s="114" t="s">
+      <c r="I24" s="114"/>
+      <c r="J24" s="115" t="s">
         <v>215</v>
       </c>
-      <c r="K24" s="115" t="s">
+      <c r="K24" s="116" t="s">
         <v>216</v>
       </c>
-      <c r="L24" s="116"/>
-      <c r="M24" s="17"/>
-      <c r="N24" s="71"/>
+      <c r="L24" s="117"/>
+      <c r="M24" s="18"/>
+      <c r="N24" s="72"/>
     </row>
     <row r="25" ht="13.5" customHeight="1">
       <c r="A25" s="8"/>
-      <c r="B25" s="17"/>
-      <c r="C25" s="73" t="s">
+      <c r="B25" s="18"/>
+      <c r="C25" s="74" t="s">
         <v>217</v>
       </c>
-      <c r="D25" s="117"/>
-      <c r="E25" s="109"/>
-      <c r="F25" s="110" t="s">
+      <c r="D25" s="118"/>
+      <c r="E25" s="110"/>
+      <c r="F25" s="111" t="s">
         <v>218</v>
       </c>
-      <c r="G25" s="111" t="s">
+      <c r="G25" s="112" t="s">
         <v>219</v>
       </c>
-      <c r="H25" s="112" t="s">
+      <c r="H25" s="113" t="s">
         <v>220</v>
       </c>
-      <c r="I25" s="113"/>
-      <c r="J25" s="114" t="s">
+      <c r="I25" s="114"/>
+      <c r="J25" s="115" t="s">
         <v>221</v>
       </c>
-      <c r="K25" s="115" t="s">
+      <c r="K25" s="116" t="s">
         <v>222</v>
       </c>
-      <c r="L25" s="116"/>
-      <c r="M25" s="17"/>
-      <c r="N25" s="71"/>
+      <c r="L25" s="117"/>
+      <c r="M25" s="18"/>
+      <c r="N25" s="72"/>
     </row>
     <row r="26" ht="13.5" customHeight="1">
       <c r="A26" s="8"/>
-      <c r="B26" s="17"/>
-      <c r="C26" s="73" t="s">
+      <c r="B26" s="18"/>
+      <c r="C26" s="74" t="s">
         <v>223</v>
       </c>
-      <c r="D26" s="117"/>
-      <c r="E26" s="109"/>
-      <c r="F26" s="110" t="s">
+      <c r="D26" s="118"/>
+      <c r="E26" s="110"/>
+      <c r="F26" s="111" t="s">
         <v>224</v>
       </c>
-      <c r="G26" s="111" t="s">
+      <c r="G26" s="112" t="s">
         <v>225</v>
       </c>
-      <c r="H26" s="112" t="s">
+      <c r="H26" s="113" t="s">
         <v>226</v>
       </c>
-      <c r="I26" s="113"/>
-      <c r="J26" s="114" t="s">
+      <c r="I26" s="114"/>
+      <c r="J26" s="115" t="s">
         <v>227</v>
       </c>
-      <c r="K26" s="115" t="s">
+      <c r="K26" s="116" t="s">
         <v>228</v>
       </c>
-      <c r="L26" s="116"/>
-      <c r="M26" s="17"/>
-      <c r="N26" s="71"/>
+      <c r="L26" s="117"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="72"/>
     </row>
     <row r="27" ht="13.5" customHeight="1">
       <c r="A27" s="8"/>
-      <c r="B27" s="17"/>
-      <c r="C27" s="73" t="s">
+      <c r="B27" s="18"/>
+      <c r="C27" s="74" t="s">
         <v>229</v>
       </c>
-      <c r="D27" s="117"/>
-      <c r="E27" s="109"/>
-      <c r="F27" s="110" t="s">
+      <c r="D27" s="118"/>
+      <c r="E27" s="110"/>
+      <c r="F27" s="111" t="s">
         <v>230</v>
       </c>
-      <c r="G27" s="111" t="s">
+      <c r="G27" s="112" t="s">
         <v>231</v>
       </c>
-      <c r="H27" s="112" t="s">
+      <c r="H27" s="113" t="s">
         <v>232</v>
       </c>
-      <c r="I27" s="113"/>
-      <c r="J27" s="114" t="s">
+      <c r="I27" s="114"/>
+      <c r="J27" s="115" t="s">
         <v>233</v>
       </c>
-      <c r="K27" s="115" t="s">
+      <c r="K27" s="116" t="s">
         <v>234</v>
       </c>
-      <c r="L27" s="116"/>
-      <c r="M27" s="17"/>
-      <c r="N27" s="71"/>
+      <c r="L27" s="117"/>
+      <c r="M27" s="18"/>
+      <c r="N27" s="72"/>
     </row>
     <row r="28" ht="13.5" customHeight="1">
       <c r="A28" s="8"/>
-      <c r="B28" s="17"/>
-      <c r="C28" s="73" t="s">
+      <c r="B28" s="18"/>
+      <c r="C28" s="74" t="s">
         <v>235</v>
       </c>
-      <c r="D28" s="117"/>
-      <c r="E28" s="109"/>
-      <c r="F28" s="110" t="s">
+      <c r="D28" s="118"/>
+      <c r="E28" s="110"/>
+      <c r="F28" s="111" t="s">
         <v>236</v>
       </c>
-      <c r="G28" s="111" t="s">
+      <c r="G28" s="112" t="s">
         <v>237</v>
       </c>
-      <c r="H28" s="112" t="s">
+      <c r="H28" s="113" t="s">
         <v>238</v>
       </c>
-      <c r="I28" s="113"/>
-      <c r="J28" s="114" t="s">
+      <c r="I28" s="114"/>
+      <c r="J28" s="115" t="s">
         <v>239</v>
       </c>
-      <c r="K28" s="115" t="s">
+      <c r="K28" s="116" t="s">
         <v>240</v>
       </c>
-      <c r="L28" s="116"/>
-      <c r="M28" s="17"/>
-      <c r="N28" s="71"/>
+      <c r="L28" s="117"/>
+      <c r="M28" s="18"/>
+      <c r="N28" s="72"/>
     </row>
     <row r="29" ht="13.5" customHeight="1">
       <c r="A29" s="8"/>
-      <c r="B29" s="17"/>
-      <c r="C29" s="73" t="s">
+      <c r="B29" s="18"/>
+      <c r="C29" s="74" t="s">
         <v>241</v>
       </c>
-      <c r="D29" s="117"/>
-      <c r="E29" s="109"/>
-      <c r="F29" s="110" t="s">
+      <c r="D29" s="118"/>
+      <c r="E29" s="110"/>
+      <c r="F29" s="111" t="s">
         <v>242</v>
       </c>
-      <c r="G29" s="111" t="s">
+      <c r="G29" s="112" t="s">
         <v>243</v>
       </c>
-      <c r="H29" s="112" t="s">
+      <c r="H29" s="113" t="s">
         <v>244</v>
       </c>
-      <c r="I29" s="113"/>
-      <c r="J29" s="114" t="s">
+      <c r="I29" s="114"/>
+      <c r="J29" s="115" t="s">
         <v>245</v>
       </c>
-      <c r="K29" s="115" t="s">
+      <c r="K29" s="116" t="s">
         <v>246</v>
       </c>
-      <c r="L29" s="116"/>
-      <c r="M29" s="17"/>
-      <c r="N29" s="71"/>
+      <c r="L29" s="117"/>
+      <c r="M29" s="18"/>
+      <c r="N29" s="72"/>
     </row>
     <row r="30" ht="13.5" customHeight="1">
       <c r="A30" s="8"/>
-      <c r="B30" s="17"/>
-      <c r="C30" s="94" t="s">
+      <c r="B30" s="18"/>
+      <c r="C30" s="95" t="s">
         <v>247</v>
       </c>
-      <c r="D30" s="119"/>
-      <c r="E30" s="120"/>
-      <c r="F30" s="121" t="s">
+      <c r="D30" s="120"/>
+      <c r="E30" s="121"/>
+      <c r="F30" s="122" t="s">
         <v>248</v>
       </c>
-      <c r="G30" s="122" t="s">
+      <c r="G30" s="123" t="s">
         <v>249</v>
       </c>
-      <c r="H30" s="123" t="s">
+      <c r="H30" s="124" t="s">
         <v>250</v>
       </c>
-      <c r="I30" s="124"/>
-      <c r="J30" s="125" t="s">
+      <c r="I30" s="125"/>
+      <c r="J30" s="126" t="s">
         <v>251</v>
       </c>
-      <c r="K30" s="126" t="s">
+      <c r="K30" s="127" t="s">
         <v>252</v>
       </c>
-      <c r="L30" s="127"/>
-      <c r="M30" s="17"/>
-      <c r="N30" s="71"/>
+      <c r="L30" s="128"/>
+      <c r="M30" s="18"/>
+      <c r="N30" s="72"/>
     </row>
     <row r="31" ht="13.5" customHeight="1">
       <c r="A31" s="8"/>
-      <c r="B31" s="17"/>
-      <c r="C31" s="128"/>
-      <c r="D31" s="128"/>
-      <c r="E31" s="129"/>
-      <c r="F31" s="130">
+      <c r="B31" s="18"/>
+      <c r="C31" s="129"/>
+      <c r="D31" s="129"/>
+      <c r="E31" s="130"/>
+      <c r="F31" s="131">
         <f>SUM(F19:F30)</f>
         <v>0</v>
       </c>
-      <c r="G31" s="129"/>
-      <c r="H31" s="129"/>
-      <c r="I31" s="129"/>
-      <c r="J31" s="129">
+      <c r="G31" s="130"/>
+      <c r="H31" s="130"/>
+      <c r="I31" s="130"/>
+      <c r="J31" s="130">
         <f>SUM(J19:J30)</f>
         <v>0</v>
       </c>
-      <c r="K31" s="129"/>
-      <c r="L31" s="129">
+      <c r="K31" s="130"/>
+      <c r="L31" s="130">
         <f>SUM(L19:L30)</f>
         <v>0</v>
       </c>
-      <c r="M31" s="17"/>
-      <c r="N31" s="71"/>
+      <c r="M31" s="18"/>
+      <c r="N31" s="72"/>
     </row>
     <row r="32" ht="13.5" customHeight="1">
-      <c r="A32" s="131"/>
-      <c r="B32" s="132" t="s">
+      <c r="A32" s="132"/>
+      <c r="B32" s="133" t="s">
         <v>253</v>
       </c>
-      <c r="C32" s="133" t="s">
+      <c r="C32" s="134" t="s">
         <v>0</v>
       </c>
-      <c r="D32" s="134"/>
-      <c r="E32" s="135"/>
-      <c r="F32" s="136"/>
-      <c r="G32" s="135"/>
-      <c r="H32" s="135"/>
-      <c r="I32" s="135"/>
-      <c r="J32" s="135"/>
-      <c r="K32" s="135"/>
-      <c r="L32" s="135"/>
-      <c r="M32" s="17"/>
-      <c r="N32" s="71"/>
+      <c r="D32" s="135"/>
+      <c r="E32" s="136"/>
+      <c r="F32" s="137"/>
+      <c r="G32" s="136"/>
+      <c r="H32" s="136"/>
+      <c r="I32" s="136"/>
+      <c r="J32" s="136"/>
+      <c r="K32" s="136"/>
+      <c r="L32" s="136"/>
+      <c r="M32" s="18"/>
+      <c r="N32" s="72"/>
     </row>
     <row r="33" ht="13.5" customHeight="1">
-      <c r="A33" s="137"/>
-      <c r="B33" s="138"/>
-      <c r="C33" s="133" t="s">
+      <c r="A33" s="138"/>
+      <c r="B33" s="139"/>
+      <c r="C33" s="134" t="s">
         <v>254</v>
       </c>
-      <c r="D33" s="134"/>
-      <c r="E33" s="135"/>
-      <c r="F33" s="136"/>
-      <c r="G33" s="135"/>
-      <c r="H33" s="135"/>
-      <c r="I33" s="135"/>
-      <c r="J33" s="135"/>
-      <c r="K33" s="135"/>
-      <c r="L33" s="135"/>
-      <c r="M33" s="17"/>
-      <c r="N33" s="71"/>
+      <c r="D33" s="135"/>
+      <c r="E33" s="136"/>
+      <c r="F33" s="137"/>
+      <c r="G33" s="136"/>
+      <c r="H33" s="136"/>
+      <c r="I33" s="136"/>
+      <c r="J33" s="136"/>
+      <c r="K33" s="136"/>
+      <c r="L33" s="136"/>
+      <c r="M33" s="18"/>
+      <c r="N33" s="72"/>
     </row>
     <row r="34" ht="13.5" customHeight="1">
-      <c r="A34" s="137"/>
-      <c r="B34" s="138"/>
-      <c r="C34" s="133" t="s">
+      <c r="A34" s="138"/>
+      <c r="B34" s="139"/>
+      <c r="C34" s="134" t="s">
         <v>255</v>
       </c>
-      <c r="D34" s="17"/>
-      <c r="E34" s="17"/>
-      <c r="F34" s="17"/>
-      <c r="G34" s="17"/>
-      <c r="H34" s="17"/>
-      <c r="I34" s="17"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="17"/>
-      <c r="L34" s="17"/>
-      <c r="M34" s="17"/>
-      <c r="N34" s="71"/>
+      <c r="D34" s="18"/>
+      <c r="E34" s="18"/>
+      <c r="F34" s="18"/>
+      <c r="G34" s="18"/>
+      <c r="H34" s="18"/>
+      <c r="I34" s="18"/>
+      <c r="J34" s="18"/>
+      <c r="K34" s="18"/>
+      <c r="L34" s="18"/>
+      <c r="M34" s="18"/>
+      <c r="N34" s="72"/>
     </row>
     <row r="35" ht="13.5" customHeight="1">
-      <c r="A35" s="137"/>
-      <c r="B35" s="138"/>
-      <c r="C35" s="133" t="s">
+      <c r="A35" s="138"/>
+      <c r="B35" s="139"/>
+      <c r="C35" s="134" t="s">
         <v>256</v>
       </c>
-      <c r="D35" s="17"/>
-      <c r="E35" s="139"/>
-      <c r="F35" s="17"/>
-      <c r="G35" s="17"/>
-      <c r="H35" s="17"/>
-      <c r="I35" s="17"/>
-      <c r="J35" s="17"/>
-      <c r="K35" s="17"/>
-      <c r="L35" s="17"/>
-      <c r="M35" s="89" t="s">
+      <c r="D35" s="18"/>
+      <c r="E35" s="140"/>
+      <c r="F35" s="18"/>
+      <c r="G35" s="18"/>
+      <c r="H35" s="18"/>
+      <c r="I35" s="18"/>
+      <c r="J35" s="18"/>
+      <c r="K35" s="18"/>
+      <c r="L35" s="18"/>
+      <c r="M35" s="90" t="s">
         <v>257</v>
       </c>
-      <c r="N35" s="140">
+      <c r="N35" s="141">
         <f>ROUND(F31+J31-L31,2)</f>
         <v>0</v>
       </c>
     </row>
     <row r="36" ht="14.25" customHeight="1">
-      <c r="A36" s="137"/>
-      <c r="B36" s="141" t="s">
+      <c r="A36" s="138"/>
+      <c r="B36" s="142" t="s">
         <v>258</v>
       </c>
-      <c r="C36" s="142" t="s">
+      <c r="C36" s="143" t="s">
         <v>259</v>
       </c>
-      <c r="D36" s="17"/>
-      <c r="E36" s="139"/>
-      <c r="F36" s="17"/>
-      <c r="G36" s="17"/>
-      <c r="H36" s="17"/>
-      <c r="I36" s="17"/>
-      <c r="J36" s="17"/>
-      <c r="K36" s="17"/>
-      <c r="L36" s="17"/>
-      <c r="M36" s="17"/>
-      <c r="N36" s="143"/>
+      <c r="D36" s="18"/>
+      <c r="E36" s="140"/>
+      <c r="F36" s="18"/>
+      <c r="G36" s="18"/>
+      <c r="H36" s="18"/>
+      <c r="I36" s="18"/>
+      <c r="J36" s="18"/>
+      <c r="K36" s="18"/>
+      <c r="L36" s="18"/>
+      <c r="M36" s="18"/>
+      <c r="N36" s="144"/>
     </row>
     <row r="37" ht="15.75" customHeight="1">
-      <c r="A37" s="144"/>
-      <c r="B37" s="138"/>
-      <c r="C37" s="142" t="s">
+      <c r="A37" s="145"/>
+      <c r="B37" s="139"/>
+      <c r="C37" s="143" t="s">
         <v>260</v>
       </c>
-      <c r="D37" s="145"/>
-      <c r="E37" s="146"/>
-      <c r="F37" s="147"/>
-      <c r="G37" s="147"/>
-      <c r="H37" s="147"/>
-      <c r="I37" s="147"/>
-      <c r="J37" s="147"/>
-      <c r="K37" s="147"/>
-      <c r="L37" s="147"/>
-      <c r="M37" s="147"/>
-      <c r="N37" s="148"/>
+      <c r="D37" s="146"/>
+      <c r="E37" s="147"/>
+      <c r="F37" s="148"/>
+      <c r="G37" s="148"/>
+      <c r="H37" s="148"/>
+      <c r="I37" s="148"/>
+      <c r="J37" s="148"/>
+      <c r="K37" s="148"/>
+      <c r="L37" s="148"/>
+      <c r="M37" s="148"/>
+      <c r="N37" s="149"/>
     </row>
     <row r="38" ht="13.5" customHeight="1">
-      <c r="D38" s="147"/>
-      <c r="F38" s="147"/>
-      <c r="G38" s="147"/>
-      <c r="H38" s="147"/>
-      <c r="I38" s="147"/>
-      <c r="J38" s="147"/>
-      <c r="K38" s="147"/>
-      <c r="L38" s="147"/>
-      <c r="M38" s="149" t="str">
+      <c r="D38" s="148"/>
+      <c r="F38" s="148"/>
+      <c r="G38" s="148"/>
+      <c r="H38" s="148"/>
+      <c r="I38" s="148"/>
+      <c r="J38" s="148"/>
+      <c r="K38" s="148"/>
+      <c r="L38" s="148"/>
+      <c r="M38" s="150" t="str">
         <f>IF(N15-N35&gt;=0,"Net Due to Charter School:","Net Due to School District:")</f>
         <v>#VALUE!</v>
       </c>
-      <c r="N38" s="150" t="str">
+      <c r="N38" s="151" t="str">
         <f>ROUND(ABS(N15-N35),2)</f>
         <v>#VALUE!</v>
       </c>
@@ -3865,14 +3823,14 @@
       <c r="C1" s="2"/>
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
-      <c r="F1" s="4" t="s">
+      <c r="F1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="3"/>
       <c r="H1" s="3"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
-      <c r="K1" s="5"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2">
       <c r="A2" s="8"/>
@@ -3910,7 +3868,7 @@
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
       <c r="E4" s="12"/>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="15" t="s">
         <v>3</v>
       </c>
       <c r="G4" s="12"/>
@@ -3921,790 +3879,790 @@
     </row>
     <row r="5" ht="12.75" customHeight="1">
       <c r="A5" s="8"/>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="16" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="16"/>
-      <c r="D5" s="16"/>
-      <c r="E5" s="17"/>
-      <c r="F5" s="17"/>
-      <c r="G5" s="18"/>
-      <c r="H5" s="18"/>
-      <c r="I5" s="18"/>
-      <c r="J5" s="18"/>
-      <c r="K5" s="19"/>
+      <c r="C5" s="17"/>
+      <c r="D5" s="17"/>
+      <c r="E5" s="18"/>
+      <c r="F5" s="18"/>
+      <c r="G5" s="19"/>
+      <c r="H5" s="19"/>
+      <c r="I5" s="19"/>
+      <c r="J5" s="19"/>
+      <c r="K5" s="20"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
       <c r="A6" s="8"/>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="17"/>
-      <c r="D6" s="16"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="21"/>
-      <c r="J6" s="16"/>
-      <c r="K6" s="22" t="s">
+      <c r="C6" s="18"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="18"/>
+      <c r="F6" s="18"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="22"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="23" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
       <c r="A7" s="8"/>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="24"/>
+      <c r="B7" s="24"/>
+      <c r="C7" s="24"/>
+      <c r="D7" s="24"/>
+      <c r="E7" s="24"/>
+      <c r="F7" s="24"/>
+      <c r="G7" s="24"/>
+      <c r="H7" s="24"/>
+      <c r="I7" s="24"/>
+      <c r="J7" s="24"/>
+      <c r="K7" s="25"/>
     </row>
     <row r="8" ht="12.75" customHeight="1">
-      <c r="A8" s="25"/>
-      <c r="B8" s="26"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="28"/>
-      <c r="F8" s="29" t="s">
+      <c r="A8" s="26"/>
+      <c r="B8" s="27"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="30" t="s">
+      <c r="G8" s="31" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="31"/>
-      <c r="I8" s="32" t="s">
+      <c r="H8" s="32"/>
+      <c r="I8" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="33"/>
-      <c r="K8" s="30" t="s">
+      <c r="J8" s="34"/>
+      <c r="K8" s="31" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
-      <c r="A9" s="25"/>
-      <c r="B9" s="34" t="s">
+      <c r="A9" s="26"/>
+      <c r="B9" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="35"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="38"/>
-      <c r="G9" s="34" t="s">
+      <c r="C9" s="36"/>
+      <c r="D9" s="37"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="39"/>
+      <c r="G9" s="35" t="s">
         <v>12</v>
       </c>
-      <c r="H9" s="39" t="s">
+      <c r="H9" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="I9" s="39" t="s">
+      <c r="I9" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="J9" s="34" t="s">
+      <c r="J9" s="35" t="s">
         <v>15</v>
       </c>
-      <c r="K9" s="40" t="s">
+      <c r="K9" s="41" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
-      <c r="A10" s="25"/>
-      <c r="B10" s="34" t="s">
+      <c r="A10" s="26"/>
+      <c r="B10" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="C10" s="41" t="s">
+      <c r="C10" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="42" t="s">
+      <c r="D10" s="43" t="s">
         <v>19</v>
       </c>
-      <c r="E10" s="37"/>
-      <c r="F10" s="30" t="s">
+      <c r="E10" s="38"/>
+      <c r="F10" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="34" t="s">
+      <c r="G10" s="35" t="s">
         <v>21</v>
       </c>
-      <c r="H10" s="39" t="s">
+      <c r="H10" s="40" t="s">
         <v>14</v>
       </c>
-      <c r="I10" s="43" t="s">
+      <c r="I10" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="J10" s="34" t="s">
+      <c r="J10" s="35" t="s">
         <v>23</v>
       </c>
-      <c r="K10" s="30" t="s">
+      <c r="K10" s="31" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1">
-      <c r="A11" s="25"/>
-      <c r="B11" s="38"/>
-      <c r="C11" s="38"/>
-      <c r="D11" s="44"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="40" t="s">
+      <c r="A11" s="26"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="39"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="46"/>
+      <c r="F11" s="39"/>
+      <c r="G11" s="41" t="s">
         <v>24</v>
       </c>
-      <c r="H11" s="46"/>
-      <c r="I11" s="47" t="s">
+      <c r="H11" s="47"/>
+      <c r="I11" s="48" t="s">
         <v>25</v>
       </c>
-      <c r="J11" s="40" t="s">
+      <c r="J11" s="41" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="40" t="s">
+      <c r="K11" s="41" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="25"/>
-      <c r="B12" s="48"/>
-      <c r="C12" s="48"/>
-      <c r="D12" s="49" t="s">
+      <c r="A12" s="26"/>
+      <c r="B12" s="49"/>
+      <c r="C12" s="49"/>
+      <c r="D12" s="50" t="s">
         <v>28</v>
       </c>
-      <c r="E12" s="50"/>
-      <c r="F12" s="51" t="s">
+      <c r="E12" s="51"/>
+      <c r="F12" s="52" t="s">
         <v>29</v>
       </c>
-      <c r="G12" s="52"/>
-      <c r="H12" s="52"/>
-      <c r="I12" s="52"/>
-      <c r="J12" s="48"/>
-      <c r="K12" s="51" t="s">
+      <c r="G12" s="53"/>
+      <c r="H12" s="53"/>
+      <c r="I12" s="53"/>
+      <c r="J12" s="49"/>
+      <c r="K12" s="52" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
-      <c r="A13" s="25"/>
-      <c r="B13" s="53">
+      <c r="A13" s="26"/>
+      <c r="B13" s="54">
         <v>1.0</v>
       </c>
-      <c r="C13" s="54" t="s">
+      <c r="C13" s="55" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="55" t="s">
+      <c r="D13" s="56" t="s">
         <v>32</v>
       </c>
-      <c r="E13" s="56"/>
-      <c r="F13" s="57"/>
-      <c r="G13" s="53"/>
-      <c r="H13" s="58" t="s">
+      <c r="E13" s="57"/>
+      <c r="F13" s="58"/>
+      <c r="G13" s="54"/>
+      <c r="H13" s="59" t="s">
         <v>33</v>
       </c>
-      <c r="I13" s="58" t="s">
+      <c r="I13" s="59" t="s">
         <v>34</v>
       </c>
-      <c r="J13" s="54" t="s">
+      <c r="J13" s="55" t="s">
         <v>35</v>
       </c>
-      <c r="K13" s="59"/>
+      <c r="K13" s="60"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
-      <c r="A14" s="25"/>
-      <c r="B14" s="53"/>
-      <c r="C14" s="53"/>
-      <c r="D14" s="55" t="s">
+      <c r="A14" s="26"/>
+      <c r="B14" s="54"/>
+      <c r="C14" s="54"/>
+      <c r="D14" s="56" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="56"/>
-      <c r="F14" s="60" t="s">
+      <c r="E14" s="57"/>
+      <c r="F14" s="61" t="s">
         <v>37</v>
       </c>
-      <c r="G14" s="53"/>
-      <c r="H14" s="53"/>
-      <c r="I14" s="53"/>
-      <c r="J14" s="53"/>
-      <c r="K14" s="51" t="s">
+      <c r="G14" s="54"/>
+      <c r="H14" s="54"/>
+      <c r="I14" s="54"/>
+      <c r="J14" s="54"/>
+      <c r="K14" s="52" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="25"/>
-      <c r="B15" s="59"/>
-      <c r="C15" s="59"/>
-      <c r="D15" s="61" t="s">
+      <c r="A15" s="26"/>
+      <c r="B15" s="60"/>
+      <c r="C15" s="60"/>
+      <c r="D15" s="62" t="s">
         <v>39</v>
       </c>
-      <c r="E15" s="62"/>
-      <c r="F15" s="59"/>
-      <c r="G15" s="59"/>
-      <c r="H15" s="59"/>
-      <c r="I15" s="59"/>
-      <c r="J15" s="59"/>
-      <c r="K15" s="59"/>
+      <c r="E15" s="63"/>
+      <c r="F15" s="60"/>
+      <c r="G15" s="60"/>
+      <c r="H15" s="60"/>
+      <c r="I15" s="60"/>
+      <c r="J15" s="60"/>
+      <c r="K15" s="60"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
-      <c r="A16" s="25"/>
-      <c r="B16" s="48"/>
-      <c r="C16" s="48"/>
-      <c r="D16" s="49" t="s">
+      <c r="A16" s="26"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="49"/>
+      <c r="D16" s="50" t="s">
         <v>40</v>
       </c>
-      <c r="E16" s="50"/>
-      <c r="F16" s="51" t="s">
+      <c r="E16" s="51"/>
+      <c r="F16" s="52" t="s">
         <v>41</v>
       </c>
-      <c r="G16" s="52"/>
-      <c r="H16" s="52"/>
-      <c r="I16" s="52"/>
-      <c r="J16" s="48"/>
-      <c r="K16" s="51" t="s">
+      <c r="G16" s="53"/>
+      <c r="H16" s="53"/>
+      <c r="I16" s="53"/>
+      <c r="J16" s="49"/>
+      <c r="K16" s="52" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1">
-      <c r="A17" s="25"/>
-      <c r="B17" s="53">
+      <c r="A17" s="26"/>
+      <c r="B17" s="54">
         <f>B13+1</f>
         <v>2</v>
       </c>
-      <c r="C17" s="54" t="s">
+      <c r="C17" s="55" t="s">
         <v>43</v>
       </c>
-      <c r="D17" s="55" t="s">
+      <c r="D17" s="56" t="s">
         <v>44</v>
       </c>
-      <c r="E17" s="56"/>
-      <c r="F17" s="57"/>
-      <c r="G17" s="53"/>
-      <c r="H17" s="58" t="s">
+      <c r="E17" s="57"/>
+      <c r="F17" s="58"/>
+      <c r="G17" s="54"/>
+      <c r="H17" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="I17" s="58" t="s">
+      <c r="I17" s="59" t="s">
         <v>46</v>
       </c>
-      <c r="J17" s="54" t="s">
+      <c r="J17" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="K17" s="59"/>
+      <c r="K17" s="60"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
-      <c r="A18" s="25"/>
-      <c r="B18" s="53"/>
-      <c r="C18" s="53"/>
-      <c r="D18" s="55" t="s">
+      <c r="A18" s="26"/>
+      <c r="B18" s="54"/>
+      <c r="C18" s="54"/>
+      <c r="D18" s="56" t="s">
         <v>48</v>
       </c>
-      <c r="E18" s="56"/>
-      <c r="F18" s="60" t="s">
+      <c r="E18" s="57"/>
+      <c r="F18" s="61" t="s">
         <v>49</v>
       </c>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="51" t="s">
+      <c r="G18" s="54"/>
+      <c r="H18" s="54"/>
+      <c r="I18" s="54"/>
+      <c r="J18" s="54"/>
+      <c r="K18" s="52" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1">
-      <c r="A19" s="25"/>
-      <c r="B19" s="59"/>
-      <c r="C19" s="59"/>
-      <c r="D19" s="61" t="s">
+      <c r="A19" s="26"/>
+      <c r="B19" s="60"/>
+      <c r="C19" s="60"/>
+      <c r="D19" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="E19" s="62"/>
-      <c r="F19" s="59"/>
-      <c r="G19" s="59"/>
-      <c r="H19" s="59"/>
-      <c r="I19" s="59"/>
-      <c r="J19" s="59"/>
-      <c r="K19" s="59"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="60"/>
+      <c r="G19" s="60"/>
+      <c r="H19" s="60"/>
+      <c r="I19" s="60"/>
+      <c r="J19" s="60"/>
+      <c r="K19" s="60"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
-      <c r="A20" s="25"/>
-      <c r="B20" s="48"/>
-      <c r="C20" s="48"/>
-      <c r="D20" s="49" t="s">
+      <c r="A20" s="26"/>
+      <c r="B20" s="49"/>
+      <c r="C20" s="49"/>
+      <c r="D20" s="50" t="s">
         <v>52</v>
       </c>
-      <c r="E20" s="50"/>
-      <c r="F20" s="51" t="s">
+      <c r="E20" s="51"/>
+      <c r="F20" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="G20" s="52"/>
-      <c r="H20" s="52"/>
-      <c r="I20" s="52"/>
-      <c r="J20" s="48"/>
-      <c r="K20" s="51" t="s">
+      <c r="G20" s="53"/>
+      <c r="H20" s="53"/>
+      <c r="I20" s="53"/>
+      <c r="J20" s="49"/>
+      <c r="K20" s="52" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="21" ht="12.75" customHeight="1">
-      <c r="A21" s="25"/>
-      <c r="B21" s="53">
+      <c r="A21" s="26"/>
+      <c r="B21" s="54">
         <f>B17+1</f>
         <v>3</v>
       </c>
-      <c r="C21" s="54" t="s">
+      <c r="C21" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="55" t="s">
+      <c r="D21" s="56" t="s">
         <v>56</v>
       </c>
-      <c r="E21" s="56"/>
-      <c r="F21" s="57"/>
-      <c r="G21" s="53"/>
-      <c r="H21" s="58" t="s">
+      <c r="E21" s="57"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="54"/>
+      <c r="H21" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="I21" s="58" t="s">
+      <c r="I21" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="J21" s="54" t="s">
+      <c r="J21" s="55" t="s">
         <v>59</v>
       </c>
-      <c r="K21" s="59"/>
+      <c r="K21" s="60"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
-      <c r="A22" s="25"/>
-      <c r="B22" s="53"/>
-      <c r="C22" s="53"/>
-      <c r="D22" s="55" t="s">
+      <c r="A22" s="26"/>
+      <c r="B22" s="54"/>
+      <c r="C22" s="54"/>
+      <c r="D22" s="56" t="s">
         <v>60</v>
       </c>
-      <c r="E22" s="56"/>
-      <c r="F22" s="60" t="s">
+      <c r="E22" s="57"/>
+      <c r="F22" s="61" t="s">
         <v>61</v>
       </c>
-      <c r="G22" s="53"/>
-      <c r="H22" s="53"/>
-      <c r="I22" s="53"/>
-      <c r="J22" s="53"/>
-      <c r="K22" s="51" t="s">
+      <c r="G22" s="54"/>
+      <c r="H22" s="54"/>
+      <c r="I22" s="54"/>
+      <c r="J22" s="54"/>
+      <c r="K22" s="52" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="23" ht="12.75" customHeight="1">
-      <c r="A23" s="25"/>
-      <c r="B23" s="59"/>
-      <c r="C23" s="59"/>
-      <c r="D23" s="61" t="s">
+      <c r="A23" s="26"/>
+      <c r="B23" s="60"/>
+      <c r="C23" s="60"/>
+      <c r="D23" s="62" t="s">
         <v>63</v>
       </c>
-      <c r="E23" s="62"/>
-      <c r="F23" s="59"/>
-      <c r="G23" s="59"/>
-      <c r="H23" s="59"/>
-      <c r="I23" s="59"/>
-      <c r="J23" s="59"/>
-      <c r="K23" s="59"/>
+      <c r="E23" s="63"/>
+      <c r="F23" s="60"/>
+      <c r="G23" s="60"/>
+      <c r="H23" s="60"/>
+      <c r="I23" s="60"/>
+      <c r="J23" s="60"/>
+      <c r="K23" s="60"/>
     </row>
     <row r="24" ht="12.75" customHeight="1">
-      <c r="A24" s="25"/>
-      <c r="B24" s="48"/>
-      <c r="C24" s="48"/>
-      <c r="D24" s="49" t="s">
+      <c r="A24" s="26"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="49"/>
+      <c r="D24" s="50" t="s">
         <v>64</v>
       </c>
-      <c r="E24" s="50"/>
-      <c r="F24" s="51" t="s">
+      <c r="E24" s="51"/>
+      <c r="F24" s="52" t="s">
         <v>65</v>
       </c>
-      <c r="G24" s="52"/>
-      <c r="H24" s="52"/>
-      <c r="I24" s="52"/>
-      <c r="J24" s="48"/>
-      <c r="K24" s="51" t="s">
+      <c r="G24" s="53"/>
+      <c r="H24" s="53"/>
+      <c r="I24" s="53"/>
+      <c r="J24" s="49"/>
+      <c r="K24" s="52" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="25" ht="12.75" customHeight="1">
-      <c r="A25" s="25"/>
-      <c r="B25" s="53">
+      <c r="A25" s="26"/>
+      <c r="B25" s="54">
         <f>B21+1</f>
         <v>4</v>
       </c>
-      <c r="C25" s="54" t="s">
+      <c r="C25" s="55" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="55" t="s">
+      <c r="D25" s="56" t="s">
         <v>68</v>
       </c>
-      <c r="E25" s="56"/>
-      <c r="F25" s="57"/>
-      <c r="G25" s="53"/>
-      <c r="H25" s="58" t="s">
+      <c r="E25" s="57"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="59" t="s">
         <v>69</v>
       </c>
-      <c r="I25" s="58" t="s">
+      <c r="I25" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="J25" s="54" t="s">
+      <c r="J25" s="55" t="s">
         <v>71</v>
       </c>
-      <c r="K25" s="59"/>
+      <c r="K25" s="60"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
-      <c r="A26" s="25"/>
-      <c r="B26" s="53"/>
-      <c r="C26" s="53"/>
-      <c r="D26" s="55" t="s">
+      <c r="A26" s="26"/>
+      <c r="B26" s="54"/>
+      <c r="C26" s="54"/>
+      <c r="D26" s="56" t="s">
         <v>72</v>
       </c>
-      <c r="E26" s="56"/>
-      <c r="F26" s="60" t="s">
+      <c r="E26" s="57"/>
+      <c r="F26" s="61" t="s">
         <v>73</v>
       </c>
-      <c r="G26" s="53"/>
-      <c r="H26" s="53"/>
-      <c r="I26" s="53"/>
-      <c r="J26" s="53"/>
-      <c r="K26" s="51" t="s">
+      <c r="G26" s="54"/>
+      <c r="H26" s="54"/>
+      <c r="I26" s="54"/>
+      <c r="J26" s="54"/>
+      <c r="K26" s="52" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1">
-      <c r="A27" s="25"/>
-      <c r="B27" s="59"/>
-      <c r="C27" s="59"/>
-      <c r="D27" s="61" t="s">
+      <c r="A27" s="26"/>
+      <c r="B27" s="60"/>
+      <c r="C27" s="60"/>
+      <c r="D27" s="62" t="s">
         <v>75</v>
       </c>
-      <c r="E27" s="62"/>
-      <c r="F27" s="59"/>
-      <c r="G27" s="59"/>
-      <c r="H27" s="59"/>
-      <c r="I27" s="59"/>
-      <c r="J27" s="59"/>
-      <c r="K27" s="59"/>
+      <c r="E27" s="63"/>
+      <c r="F27" s="60"/>
+      <c r="G27" s="60"/>
+      <c r="H27" s="60"/>
+      <c r="I27" s="60"/>
+      <c r="J27" s="60"/>
+      <c r="K27" s="60"/>
     </row>
     <row r="28" ht="12.75" customHeight="1">
-      <c r="A28" s="25"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="48"/>
-      <c r="D28" s="49" t="s">
+      <c r="A28" s="26"/>
+      <c r="B28" s="49"/>
+      <c r="C28" s="49"/>
+      <c r="D28" s="50" t="s">
         <v>76</v>
       </c>
-      <c r="E28" s="50"/>
-      <c r="F28" s="51" t="s">
+      <c r="E28" s="51"/>
+      <c r="F28" s="52" t="s">
         <v>77</v>
       </c>
-      <c r="G28" s="52"/>
-      <c r="H28" s="52"/>
-      <c r="I28" s="52"/>
-      <c r="J28" s="48"/>
-      <c r="K28" s="51" t="s">
+      <c r="G28" s="53"/>
+      <c r="H28" s="53"/>
+      <c r="I28" s="53"/>
+      <c r="J28" s="49"/>
+      <c r="K28" s="52" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="29" ht="12.75" customHeight="1">
-      <c r="A29" s="25"/>
-      <c r="B29" s="53">
+      <c r="A29" s="26"/>
+      <c r="B29" s="54">
         <f>B25+1</f>
         <v>5</v>
       </c>
-      <c r="C29" s="54" t="s">
+      <c r="C29" s="55" t="s">
         <v>79</v>
       </c>
-      <c r="D29" s="55" t="s">
+      <c r="D29" s="56" t="s">
         <v>80</v>
       </c>
-      <c r="E29" s="56"/>
-      <c r="F29" s="57"/>
-      <c r="G29" s="53"/>
-      <c r="H29" s="58" t="s">
+      <c r="E29" s="57"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="54"/>
+      <c r="H29" s="59" t="s">
         <v>81</v>
       </c>
-      <c r="I29" s="58" t="s">
+      <c r="I29" s="59" t="s">
         <v>82</v>
       </c>
-      <c r="J29" s="54" t="s">
+      <c r="J29" s="55" t="s">
         <v>83</v>
       </c>
-      <c r="K29" s="59"/>
+      <c r="K29" s="60"/>
     </row>
     <row r="30" ht="12.75" customHeight="1">
-      <c r="A30" s="25"/>
-      <c r="B30" s="53"/>
-      <c r="C30" s="53"/>
-      <c r="D30" s="55" t="s">
+      <c r="A30" s="26"/>
+      <c r="B30" s="54"/>
+      <c r="C30" s="54"/>
+      <c r="D30" s="56" t="s">
         <v>84</v>
       </c>
-      <c r="E30" s="56"/>
-      <c r="F30" s="60" t="s">
+      <c r="E30" s="57"/>
+      <c r="F30" s="61" t="s">
         <v>85</v>
       </c>
-      <c r="G30" s="53"/>
-      <c r="H30" s="53"/>
-      <c r="I30" s="53"/>
-      <c r="J30" s="53"/>
-      <c r="K30" s="51" t="s">
+      <c r="G30" s="54"/>
+      <c r="H30" s="54"/>
+      <c r="I30" s="54"/>
+      <c r="J30" s="54"/>
+      <c r="K30" s="52" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1">
-      <c r="A31" s="25"/>
-      <c r="B31" s="59"/>
-      <c r="C31" s="59"/>
-      <c r="D31" s="61" t="s">
+      <c r="A31" s="26"/>
+      <c r="B31" s="60"/>
+      <c r="C31" s="60"/>
+      <c r="D31" s="62" t="s">
         <v>87</v>
       </c>
-      <c r="E31" s="62"/>
-      <c r="F31" s="59"/>
-      <c r="G31" s="59"/>
-      <c r="H31" s="59"/>
-      <c r="I31" s="59"/>
-      <c r="J31" s="59"/>
-      <c r="K31" s="59"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="60"/>
+      <c r="G31" s="60"/>
+      <c r="H31" s="60"/>
+      <c r="I31" s="60"/>
+      <c r="J31" s="60"/>
+      <c r="K31" s="60"/>
     </row>
     <row r="32" ht="12.75" customHeight="1">
-      <c r="A32" s="25"/>
-      <c r="B32" s="48"/>
-      <c r="C32" s="48"/>
-      <c r="D32" s="49" t="s">
+      <c r="A32" s="26"/>
+      <c r="B32" s="49"/>
+      <c r="C32" s="49"/>
+      <c r="D32" s="50" t="s">
         <v>88</v>
       </c>
-      <c r="E32" s="50"/>
-      <c r="F32" s="51" t="s">
+      <c r="E32" s="51"/>
+      <c r="F32" s="52" t="s">
         <v>89</v>
       </c>
-      <c r="G32" s="52"/>
-      <c r="H32" s="52"/>
-      <c r="I32" s="52"/>
-      <c r="J32" s="48"/>
-      <c r="K32" s="51" t="s">
+      <c r="G32" s="53"/>
+      <c r="H32" s="53"/>
+      <c r="I32" s="53"/>
+      <c r="J32" s="49"/>
+      <c r="K32" s="52" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="33" ht="12.75" customHeight="1">
-      <c r="A33" s="25"/>
-      <c r="B33" s="53">
+      <c r="A33" s="26"/>
+      <c r="B33" s="54">
         <f>B29+1</f>
         <v>6</v>
       </c>
-      <c r="C33" s="54" t="s">
+      <c r="C33" s="55" t="s">
         <v>91</v>
       </c>
-      <c r="D33" s="55" t="s">
+      <c r="D33" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="E33" s="56"/>
-      <c r="F33" s="57"/>
-      <c r="G33" s="53"/>
-      <c r="H33" s="58" t="s">
+      <c r="E33" s="57"/>
+      <c r="F33" s="58"/>
+      <c r="G33" s="54"/>
+      <c r="H33" s="59" t="s">
         <v>93</v>
       </c>
-      <c r="I33" s="58" t="s">
+      <c r="I33" s="59" t="s">
         <v>94</v>
       </c>
-      <c r="J33" s="54" t="s">
+      <c r="J33" s="55" t="s">
         <v>95</v>
       </c>
-      <c r="K33" s="59"/>
+      <c r="K33" s="60"/>
     </row>
     <row r="34" ht="12.75" customHeight="1">
-      <c r="A34" s="25"/>
-      <c r="B34" s="53"/>
-      <c r="C34" s="53"/>
-      <c r="D34" s="55" t="s">
+      <c r="A34" s="26"/>
+      <c r="B34" s="54"/>
+      <c r="C34" s="54"/>
+      <c r="D34" s="56" t="s">
         <v>96</v>
       </c>
-      <c r="E34" s="56"/>
-      <c r="F34" s="60" t="s">
+      <c r="E34" s="57"/>
+      <c r="F34" s="61" t="s">
         <v>97</v>
       </c>
-      <c r="G34" s="53"/>
-      <c r="H34" s="53"/>
-      <c r="I34" s="53"/>
-      <c r="J34" s="53"/>
-      <c r="K34" s="51" t="s">
+      <c r="G34" s="54"/>
+      <c r="H34" s="54"/>
+      <c r="I34" s="54"/>
+      <c r="J34" s="54"/>
+      <c r="K34" s="52" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="35" ht="12.75" customHeight="1">
-      <c r="A35" s="25"/>
-      <c r="B35" s="59"/>
-      <c r="C35" s="59"/>
-      <c r="D35" s="61" t="s">
+      <c r="A35" s="26"/>
+      <c r="B35" s="60"/>
+      <c r="C35" s="60"/>
+      <c r="D35" s="62" t="s">
         <v>99</v>
       </c>
-      <c r="E35" s="62"/>
-      <c r="F35" s="59"/>
-      <c r="G35" s="59"/>
-      <c r="H35" s="59"/>
-      <c r="I35" s="59"/>
-      <c r="J35" s="59"/>
-      <c r="K35" s="59"/>
+      <c r="E35" s="63"/>
+      <c r="F35" s="60"/>
+      <c r="G35" s="60"/>
+      <c r="H35" s="60"/>
+      <c r="I35" s="60"/>
+      <c r="J35" s="60"/>
+      <c r="K35" s="60"/>
     </row>
     <row r="36" ht="12.75" customHeight="1">
-      <c r="A36" s="25"/>
-      <c r="B36" s="48"/>
-      <c r="C36" s="48"/>
-      <c r="D36" s="49" t="s">
+      <c r="A36" s="26"/>
+      <c r="B36" s="49"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="50" t="s">
         <v>100</v>
       </c>
-      <c r="E36" s="50"/>
-      <c r="F36" s="51" t="s">
+      <c r="E36" s="51"/>
+      <c r="F36" s="52" t="s">
         <v>101</v>
       </c>
-      <c r="G36" s="52"/>
-      <c r="H36" s="52"/>
-      <c r="I36" s="52"/>
-      <c r="J36" s="48"/>
-      <c r="K36" s="51" t="s">
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
+      <c r="I36" s="53"/>
+      <c r="J36" s="49"/>
+      <c r="K36" s="52" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="37" ht="12.75" customHeight="1">
-      <c r="A37" s="25"/>
-      <c r="B37" s="53">
+      <c r="A37" s="26"/>
+      <c r="B37" s="54">
         <f>B33+1</f>
         <v>7</v>
       </c>
-      <c r="C37" s="54" t="s">
+      <c r="C37" s="55" t="s">
         <v>103</v>
       </c>
-      <c r="D37" s="55" t="s">
+      <c r="D37" s="56" t="s">
         <v>104</v>
       </c>
-      <c r="E37" s="56"/>
-      <c r="F37" s="63"/>
-      <c r="G37" s="53"/>
-      <c r="H37" s="58" t="s">
+      <c r="E37" s="57"/>
+      <c r="F37" s="64"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="59" t="s">
         <v>105</v>
       </c>
-      <c r="I37" s="58" t="s">
+      <c r="I37" s="59" t="s">
         <v>106</v>
       </c>
-      <c r="J37" s="54" t="s">
+      <c r="J37" s="55" t="s">
         <v>107</v>
       </c>
-      <c r="K37" s="59"/>
+      <c r="K37" s="60"/>
     </row>
     <row r="38" ht="12.75" customHeight="1">
-      <c r="A38" s="25"/>
-      <c r="B38" s="53"/>
-      <c r="C38" s="53"/>
-      <c r="D38" s="55" t="s">
+      <c r="A38" s="26"/>
+      <c r="B38" s="54"/>
+      <c r="C38" s="54"/>
+      <c r="D38" s="56" t="s">
         <v>108</v>
       </c>
-      <c r="E38" s="56"/>
-      <c r="F38" s="60" t="s">
+      <c r="E38" s="57"/>
+      <c r="F38" s="61" t="s">
         <v>109</v>
       </c>
-      <c r="G38" s="53"/>
-      <c r="H38" s="53"/>
-      <c r="I38" s="53"/>
-      <c r="J38" s="53"/>
-      <c r="K38" s="51" t="s">
+      <c r="G38" s="54"/>
+      <c r="H38" s="54"/>
+      <c r="I38" s="54"/>
+      <c r="J38" s="54"/>
+      <c r="K38" s="52" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="39" ht="12.75" customHeight="1">
-      <c r="A39" s="25"/>
-      <c r="B39" s="59"/>
-      <c r="C39" s="59"/>
-      <c r="D39" s="61" t="s">
+      <c r="A39" s="26"/>
+      <c r="B39" s="60"/>
+      <c r="C39" s="60"/>
+      <c r="D39" s="62" t="s">
         <v>111</v>
       </c>
-      <c r="E39" s="62"/>
-      <c r="F39" s="59"/>
-      <c r="G39" s="59"/>
-      <c r="H39" s="59"/>
-      <c r="I39" s="59"/>
-      <c r="J39" s="59"/>
-      <c r="K39" s="59"/>
+      <c r="E39" s="63"/>
+      <c r="F39" s="60"/>
+      <c r="G39" s="60"/>
+      <c r="H39" s="60"/>
+      <c r="I39" s="60"/>
+      <c r="J39" s="60"/>
+      <c r="K39" s="60"/>
     </row>
     <row r="40" ht="12.75" customHeight="1">
-      <c r="A40" s="25"/>
-      <c r="B40" s="48"/>
-      <c r="C40" s="48"/>
-      <c r="D40" s="49" t="s">
+      <c r="A40" s="26"/>
+      <c r="B40" s="49"/>
+      <c r="C40" s="49"/>
+      <c r="D40" s="50" t="s">
         <v>112</v>
       </c>
-      <c r="E40" s="50"/>
-      <c r="F40" s="51" t="s">
+      <c r="E40" s="51"/>
+      <c r="F40" s="52" t="s">
         <v>113</v>
       </c>
-      <c r="G40" s="52"/>
-      <c r="H40" s="52"/>
-      <c r="I40" s="52"/>
-      <c r="J40" s="48"/>
-      <c r="K40" s="51" t="s">
+      <c r="G40" s="53"/>
+      <c r="H40" s="53"/>
+      <c r="I40" s="53"/>
+      <c r="J40" s="49"/>
+      <c r="K40" s="52" t="s">
         <v>114</v>
       </c>
     </row>
     <row r="41" ht="12.75" customHeight="1">
-      <c r="A41" s="25"/>
-      <c r="B41" s="53">
+      <c r="A41" s="26"/>
+      <c r="B41" s="54">
         <f>B37+1</f>
         <v>8</v>
       </c>
-      <c r="C41" s="54" t="s">
+      <c r="C41" s="55" t="s">
         <v>115</v>
       </c>
-      <c r="D41" s="55" t="s">
+      <c r="D41" s="56" t="s">
         <v>116</v>
       </c>
-      <c r="E41" s="56"/>
-      <c r="F41" s="57"/>
-      <c r="G41" s="53"/>
-      <c r="H41" s="58" t="s">
+      <c r="E41" s="57"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="59" t="s">
         <v>117</v>
       </c>
-      <c r="I41" s="58" t="s">
+      <c r="I41" s="59" t="s">
         <v>118</v>
       </c>
-      <c r="J41" s="54" t="s">
+      <c r="J41" s="55" t="s">
         <v>119</v>
       </c>
-      <c r="K41" s="59"/>
+      <c r="K41" s="60"/>
     </row>
     <row r="42" ht="12.75" customHeight="1">
-      <c r="A42" s="64"/>
-      <c r="B42" s="53"/>
-      <c r="C42" s="53"/>
-      <c r="D42" s="55" t="s">
+      <c r="A42" s="65"/>
+      <c r="B42" s="54"/>
+      <c r="C42" s="54"/>
+      <c r="D42" s="56" t="s">
         <v>120</v>
       </c>
-      <c r="E42" s="56"/>
-      <c r="F42" s="60" t="s">
+      <c r="E42" s="57"/>
+      <c r="F42" s="61" t="s">
         <v>121</v>
       </c>
-      <c r="G42" s="53"/>
-      <c r="H42" s="53"/>
-      <c r="I42" s="53"/>
-      <c r="J42" s="53"/>
-      <c r="K42" s="51" t="s">
+      <c r="G42" s="54"/>
+      <c r="H42" s="54"/>
+      <c r="I42" s="54"/>
+      <c r="J42" s="54"/>
+      <c r="K42" s="52" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="65"/>
-      <c r="B43" s="59"/>
-      <c r="C43" s="59"/>
-      <c r="D43" s="61" t="s">
+      <c r="A43" s="66"/>
+      <c r="B43" s="60"/>
+      <c r="C43" s="60"/>
+      <c r="D43" s="62" t="s">
         <v>123</v>
       </c>
-      <c r="E43" s="62"/>
-      <c r="F43" s="59"/>
-      <c r="G43" s="59"/>
-      <c r="H43" s="59"/>
-      <c r="I43" s="59"/>
-      <c r="J43" s="59"/>
-      <c r="K43" s="59"/>
+      <c r="E43" s="63"/>
+      <c r="F43" s="60"/>
+      <c r="G43" s="60"/>
+      <c r="H43" s="60"/>
+      <c r="I43" s="60"/>
+      <c r="J43" s="60"/>
+      <c r="K43" s="60"/>
     </row>
     <row r="44" ht="12.75" customHeight="1">
-      <c r="A44" s="66"/>
-      <c r="B44" s="66"/>
-      <c r="C44" s="66"/>
-      <c r="D44" s="66"/>
-      <c r="E44" s="66"/>
-      <c r="F44" s="66"/>
-      <c r="G44" s="66"/>
-      <c r="H44" s="66"/>
-      <c r="I44" s="66"/>
-      <c r="J44" s="66"/>
-      <c r="K44" s="66"/>
+      <c r="A44" s="67"/>
+      <c r="B44" s="67"/>
+      <c r="C44" s="67"/>
+      <c r="D44" s="67"/>
+      <c r="E44" s="67"/>
+      <c r="F44" s="67"/>
+      <c r="G44" s="67"/>
+      <c r="H44" s="67"/>
+      <c r="I44" s="67"/>
+      <c r="J44" s="67"/>
+      <c r="K44" s="67"/>
     </row>
     <row r="45" ht="15.75" customHeight="1"/>
     <row r="46" ht="15.75" customHeight="1"/>

</xml_diff>

<commit_message>
Fix date formatting issue in template
</commit_message>
<xml_diff>
--- a/api/Templates/CSFunding 2018-19 Bulk Invoice Summary - Template.xlsx
+++ b/api/Templates/CSFunding 2018-19 Bulk Invoice Summary - Template.xlsx
@@ -56,19 +56,13 @@
     <t>${ToPDE}</t>
   </si>
   <si>
-    <t>Date of Birth</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CS Student </t>
-  </si>
-  <si>
-    <t>Last Day</t>
-  </si>
-  <si>
     <t>JUL
 ${Districts[0].FirstYear}</t>
   </si>
   <si>
+    <t>Date of Birth</t>
+  </si>
+  <si>
     <t>AUG
 ${Districts[0].FirstYear}</t>
   </si>
@@ -116,13 +110,94 @@
 Due</t>
   </si>
   <si>
+    <t xml:space="preserve">CS Student </t>
+  </si>
+  <si>
+    <t>Nonspecial Education</t>
+  </si>
+  <si>
+    <t>${Districts[0].RegularEnrollments.July}</t>
+  </si>
+  <si>
+    <t>Last Day</t>
+  </si>
+  <si>
+    <t>${Districts[0].RegularEnrollments.August}</t>
+  </si>
+  <si>
+    <t>${Districts[0].RegularEnrollments.September}</t>
+  </si>
+  <si>
+    <t>${Districts[0].RegularEnrollments.October}</t>
+  </si>
+  <si>
+    <t>${Districts[0].RegularEnrollments.November}</t>
+  </si>
+  <si>
+    <t>${Districts[0].RegularEnrollments.December}</t>
+  </si>
+  <si>
+    <t>${Districts[0].RegularEnrollments.January}</t>
+  </si>
+  <si>
+    <t>${Districts[0].RegularEnrollments.February}</t>
+  </si>
+  <si>
+    <t>${Districts[0].RegularEnrollments.March}</t>
+  </si>
+  <si>
+    <t>${Districts[0].RegularEnrollments.April}</t>
+  </si>
+  <si>
+    <t>${Districts[0].RegularEnrollments.May}</t>
+  </si>
+  <si>
+    <t>${Districts[0].SchoolDistrict.RegularRate}</t>
+  </si>
+  <si>
     <t>Date of IEP</t>
   </si>
   <si>
     <t>Sequential</t>
   </si>
   <si>
-    <t>Nonspecial Education</t>
+    <t>Special Education</t>
+  </si>
+  <si>
+    <t>${Districts[0].SpecialEnrollments.July}</t>
+  </si>
+  <si>
+    <t>${Districts[0].SpecialEnrollments.August}</t>
+  </si>
+  <si>
+    <t>${Districts[0].SpecialEnrollments.September}</t>
+  </si>
+  <si>
+    <t>${Districts[0].SpecialEnrollments.October}</t>
+  </si>
+  <si>
+    <t>${Districts[0].SpecialEnrollments.November}</t>
+  </si>
+  <si>
+    <t>${Districts[0].SpecialEnrollments.December}</t>
+  </si>
+  <si>
+    <t>${Districts[0].SpecialEnrollments.January}</t>
+  </si>
+  <si>
+    <t>${Districts[0].SpecialEnrollments.February}</t>
+  </si>
+  <si>
+    <t>${Districts[0].SpecialEnrollments.March}</t>
+  </si>
+  <si>
+    <t>${Districts[0].SpecialEnrollments.April}</t>
+  </si>
+  <si>
+    <t>${Districts[0].SpecialEnrollments.May}</t>
+  </si>
+  <si>
+    <t>${Districts[0].SchoolDistrict.SpecialRate}</t>
   </si>
   <si>
     <t>Enrollment</t>
@@ -149,6 +224,9 @@
     <t>Student Name and Address</t>
   </si>
   <si>
+    <t>Total Amount Due Year to Date:</t>
+  </si>
+  <si>
     <t>Grade</t>
   </si>
   <si>
@@ -161,40 +239,19 @@
     <t>Education</t>
   </si>
   <si>
-    <t>${Districts[0].RegularEnrollments.July}</t>
-  </si>
-  <si>
-    <t>${Districts[0].RegularEnrollments.August}</t>
-  </si>
-  <si>
-    <t>${Districts[0].RegularEnrollments.September}</t>
-  </si>
-  <si>
-    <t>${Districts[0].RegularEnrollments.October}</t>
-  </si>
-  <si>
-    <t>${Districts[0].RegularEnrollments.November}</t>
-  </si>
-  <si>
-    <t>${Districts[0].RegularEnrollments.December}</t>
-  </si>
-  <si>
-    <t>${Districts[0].RegularEnrollments.January}</t>
-  </si>
-  <si>
-    <t>${Districts[0].RegularEnrollments.February}</t>
-  </si>
-  <si>
-    <t>${Districts[0].RegularEnrollments.March}</t>
-  </si>
-  <si>
-    <t>${Districts[0].RegularEnrollments.April}</t>
-  </si>
-  <si>
-    <t>${Districts[0].RegularEnrollments.May}</t>
-  </si>
-  <si>
-    <t>${Districts[0].SchoolDistrict.RegularRate}</t>
+    <t xml:space="preserve"> School District</t>
+  </si>
+  <si>
+    <t>Check</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   PDE Subsidy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Refund from</t>
+  </si>
+  <si>
+    <t>Month</t>
   </si>
   <si>
     <t>Form Sent to SD:</t>
@@ -203,18 +260,36 @@
     <t xml:space="preserve"> withdrew)</t>
   </si>
   <si>
+    <t xml:space="preserve"> Direct Payment</t>
+  </si>
+  <si>
     <t>Student</t>
   </si>
   <si>
     <t>Prior</t>
   </si>
   <si>
+    <t>Number</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[0].FullName}</t>
   </si>
   <si>
+    <t>Date</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  Deduction</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[0].DateOfBirth}</t>
   </si>
   <si>
+    <t xml:space="preserve">  Charter School</t>
+  </si>
+  <si>
+    <t>July, ${FirstYear}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[0].CurrentIep}</t>
   </si>
   <si>
@@ -224,6 +299,15 @@
     <t>${Districts[0].Students[0].Address1}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.July.Payment.CheckAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.July.Payment.CheckNumber}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.July.Payment.Date}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[0].FirstDay}</t>
   </si>
   <si>
@@ -233,6 +317,9 @@
     <t>${Districts[0].Students[0].IsSpecialEducation}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.July.Payment.UniPayAmount}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[0].Address2}</t>
   </si>
   <si>
@@ -245,6 +332,9 @@
     <t>${Districts[0].Students[0].Address3}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.July.Refund}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[1].FullName}</t>
   </si>
   <si>
@@ -254,6 +344,9 @@
     <t>${Districts[0].Students[1].CurrentIep}</t>
   </si>
   <si>
+    <t>August</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[1].PASecuredID}</t>
   </si>
   <si>
@@ -290,6 +383,9 @@
     <t>${Districts[0].Students[2].CurrentIep}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.August.Payment.CheckAmount}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[2].PASecuredID}</t>
   </si>
   <si>
@@ -314,6 +410,9 @@
     <t>${Districts[0].Students[2].FormerIep}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.August.Payment.CheckNumber}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[2].Address3}</t>
   </si>
   <si>
@@ -326,6 +425,9 @@
     <t>${Districts[0].Students[3].CurrentIep}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.August.Payment.Date}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[3].PASecuredID}</t>
   </si>
   <si>
@@ -362,6 +464,9 @@
     <t>${Districts[0].Students[4].CurrentIep}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.August.Payment.UniPayAmount}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[4].PASecuredID}</t>
   </si>
   <si>
@@ -389,6 +494,9 @@
     <t>${Districts[0].Students[4].Address3}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.August.Refund}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[5].FullName}</t>
   </si>
   <si>
@@ -398,6 +506,9 @@
     <t>${Districts[0].Students[5].CurrentIep}</t>
   </si>
   <si>
+    <t>September</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[5].PASecuredID}</t>
   </si>
   <si>
@@ -422,24 +533,75 @@
     <t>${Districts[0].Students[5].FormerIep}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.September.Payment.CheckAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.September.Payment.CheckNumber}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[5].Address3}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.September.Payment.Date}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.September.Payment.UniPayAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.September.Refund}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[6].FullName}</t>
   </si>
   <si>
     <t>${Districts[0].Students[6].DateOfBirth}</t>
   </si>
   <si>
+    <t>October</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[6].CurrentIep}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.October.Payment.CheckAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.October.Payment.CheckNumber}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.October.Payment.Date}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.October.Payment.UniPayAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.October.Refund}</t>
+  </si>
+  <si>
+    <t>November</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.November.Payment.CheckAmount}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[6].PASecuredID}</t>
   </si>
   <si>
     <t>${Districts[0].Students[6].Address1}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.November.Payment.CheckNumber}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.November.Payment.Date}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.November.Payment.UniPayAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.November.Refund}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[6].FirstDay}</t>
   </si>
   <si>
@@ -458,316 +620,154 @@
     <t>${Districts[0].Students[6].FormerIep}</t>
   </si>
   <si>
+    <t>December</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[6].Address3}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.December.Payment.CheckAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.December.Payment.CheckNumber}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.December.Payment.Date}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.December.Payment.UniPayAmount}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[7].FullName}</t>
   </si>
   <si>
     <t>${Districts[0].Students[7].DateOfBirth}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.December.Refund}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[7].CurrentIep}</t>
   </si>
   <si>
+    <t>January, ${SecondYear}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[7].PASecuredID}</t>
   </si>
   <si>
     <t>${Districts[0].Students[7].Address1}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.January.Payment.CheckAmount}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[7].FirstDay}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.January.Payment.CheckNumber}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[7].LastDay}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.January.Payment.Date}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[7].IsSpecialEducation}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.January.Payment.UniPayAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.January.Refund}</t>
+  </si>
+  <si>
+    <t>February</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.February.Payment.CheckAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.February.Payment.CheckNumber}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.February.Payment.Date}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.February.Payment.UniPayAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.February.Refund}</t>
+  </si>
+  <si>
+    <t>March</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.March.Payment.CheckAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.March.Payment.CheckNumber}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.March.Payment.Date}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.March.Payment.UniPayAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.March.Refund}</t>
+  </si>
+  <si>
+    <t>April</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.April.Payment.CheckAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.April.Payment.CheckNumber}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.April.Payment.Date}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.April.Payment.UniPayAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.April.Refund}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[7].Address2}</t>
   </si>
   <si>
+    <t>May</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[7].Grade}</t>
   </si>
   <si>
+    <t>${Districts[0].Transactions.May.Payment.CheckAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.May.Payment.CheckNumber}</t>
+  </si>
+  <si>
     <t>${Districts[0].Students[7].FormerIep}</t>
   </si>
   <si>
-    <t>Special Education</t>
-  </si>
-  <si>
-    <t>${Districts[0].SpecialEnrollments.July}</t>
-  </si>
-  <si>
-    <t>${Districts[0].SpecialEnrollments.August}</t>
-  </si>
-  <si>
-    <t>${Districts[0].SpecialEnrollments.September}</t>
-  </si>
-  <si>
-    <t>${Districts[0].SpecialEnrollments.October}</t>
-  </si>
-  <si>
-    <t>${Districts[0].SpecialEnrollments.November}</t>
-  </si>
-  <si>
-    <t>${Districts[0].SpecialEnrollments.December}</t>
-  </si>
-  <si>
-    <t>${Districts[0].SpecialEnrollments.January}</t>
-  </si>
-  <si>
-    <t>${Districts[0].SpecialEnrollments.February}</t>
-  </si>
-  <si>
-    <t>${Districts[0].SpecialEnrollments.March}</t>
-  </si>
-  <si>
-    <t>${Districts[0].SpecialEnrollments.April}</t>
-  </si>
-  <si>
-    <t>${Districts[0].SpecialEnrollments.May}</t>
-  </si>
-  <si>
-    <t>${Districts[0].SchoolDistrict.SpecialRate}</t>
+    <t>${Districts[0].Transactions.May.Payment.Date}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.May.Payment.UniPayAmount}</t>
+  </si>
+  <si>
+    <t>${Districts[0].Transactions.May.Refund}</t>
+  </si>
+  <si>
+    <t>June</t>
   </si>
   <si>
     <t>${Districts[0].Students[7].Address3}</t>
-  </si>
-  <si>
-    <t>Total Amount Due Year to Date:</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> School District</t>
-  </si>
-  <si>
-    <t>Check</t>
-  </si>
-  <si>
-    <t xml:space="preserve">   PDE Subsidy</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Refund from</t>
-  </si>
-  <si>
-    <t>Month</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Direct Payment</t>
-  </si>
-  <si>
-    <t>Number</t>
-  </si>
-  <si>
-    <t>Date</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  Charter School</t>
-  </si>
-  <si>
-    <t>July, ${FirstYear}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.July.Payment.CheckAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.July.Payment.CheckNumber}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.July.Payment.Date}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.July.Payment.UniPayAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.July.Refund}</t>
-  </si>
-  <si>
-    <t>August</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.August.Payment.CheckAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.August.Payment.CheckNumber}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.August.Payment.Date}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.August.Payment.UniPayAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.August.Refund}</t>
-  </si>
-  <si>
-    <t>September</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.September.Payment.CheckAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.September.Payment.CheckNumber}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.September.Payment.Date}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.September.Payment.UniPayAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.September.Refund}</t>
-  </si>
-  <si>
-    <t>October</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.October.Payment.CheckAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.October.Payment.CheckNumber}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.October.Payment.Date}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.October.Payment.UniPayAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.October.Refund}</t>
-  </si>
-  <si>
-    <t>November</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.November.Payment.CheckAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.November.Payment.CheckNumber}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.November.Payment.Date}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.November.Payment.UniPayAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.November.Refund}</t>
-  </si>
-  <si>
-    <t>December</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.December.Payment.CheckAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.December.Payment.CheckNumber}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.December.Payment.Date}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.December.Payment.UniPayAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.December.Refund}</t>
-  </si>
-  <si>
-    <t>January, ${SecondYear}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.January.Payment.CheckAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.January.Payment.CheckNumber}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.January.Payment.Date}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.January.Payment.UniPayAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.January.Refund}</t>
-  </si>
-  <si>
-    <t>February</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.February.Payment.CheckAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.February.Payment.CheckNumber}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.February.Payment.Date}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.February.Payment.UniPayAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.February.Refund}</t>
-  </si>
-  <si>
-    <t>March</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.March.Payment.CheckAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.March.Payment.CheckNumber}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.March.Payment.Date}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.March.Payment.UniPayAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.March.Refund}</t>
-  </si>
-  <si>
-    <t>April</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.April.Payment.CheckAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.April.Payment.CheckNumber}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.April.Payment.Date}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.April.Payment.UniPayAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.April.Refund}</t>
-  </si>
-  <si>
-    <t>May</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.May.Payment.CheckAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.May.Payment.CheckNumber}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.May.Payment.Date}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.May.Payment.UniPayAmount}</t>
-  </si>
-  <si>
-    <t>${Districts[0].Transactions.May.Refund}</t>
-  </si>
-  <si>
-    <t>June</t>
   </si>
   <si>
     <t>${Districts[0].Transactions.June.Payment.CheckAmount}</t>
@@ -838,13 +838,13 @@
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="10.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10.0"/>
+      <sz val="11.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
@@ -860,18 +860,18 @@
       <name val="Arial"/>
     </font>
     <font>
-      <i/>
-      <sz val="8.0"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-    </font>
-    <font>
       <sz val="9.0"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <sz val="10.0"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="8.0"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
     <font>
@@ -1023,16 +1023,6 @@
       <bottom/>
     </border>
     <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFAAAAAA"/>
       </left>
@@ -1045,6 +1035,16 @@
       </bottom>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -1097,6 +1097,17 @@
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -1104,6 +1115,31 @@
       <bottom style="thin">
         <color rgb="FF000000"/>
       </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+    </border>
+    <border>
+      <left/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
     </border>
     <border>
       <left style="thin">
@@ -1126,6 +1162,14 @@
       </bottom>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF000000"/>
       </left>
@@ -1139,6 +1183,11 @@
     </border>
     <border>
       <left/>
+      <right/>
+      <top/>
+    </border>
+    <border>
+      <left/>
       <right style="thin">
         <color rgb="FF000000"/>
       </right>
@@ -1148,6 +1197,34 @@
       <bottom style="thin">
         <color rgb="FFEAEAEA"/>
       </bottom>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FFD8D8D8"/>
+      </right>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFD8D8D8"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
     </border>
     <border>
       <left style="thin">
@@ -1171,113 +1248,6 @@
     </border>
     <border>
       <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <right/>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFEAEAEA"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFAAAAAA"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
-      <top/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF000000"/>
-      </left>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFAAAAAA"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-    </border>
-    <border>
-      <left/>
-      <top style="thin">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color rgb="FF000000"/>
-      </bottom>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color rgb="FFD8D8D8"/>
-      </right>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFD8D8D8"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color rgb="FF000000"/>
-      </top>
-      <bottom/>
-    </border>
-    <border>
-      <left style="thin">
         <color rgb="FFD8D8D8"/>
       </left>
       <top style="medium">
@@ -1309,6 +1279,27 @@
       </left>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFEAEAEA"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+    </border>
+    <border>
       <top style="medium">
         <color rgb="FF000000"/>
       </top>
@@ -1348,6 +1339,15 @@
       <right style="thin">
         <color rgb="FFD8D8D8"/>
       </right>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFAAAAAA"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
     </border>
     <border>
       <left/>
@@ -1440,16 +1440,19 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="1" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="2" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="2" fillId="2" fontId="1" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -1458,22 +1461,28 @@
     <xf borderId="3" fillId="2" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="2" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="4" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="3" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="4" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="5" fillId="2" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="6" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="5" fillId="2" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -1482,51 +1491,42 @@
     <xf borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="2" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="4" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="5" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="6" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="6" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="4" fillId="2" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="5" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="4" fillId="2" fontId="5" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+      <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="5" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf borderId="5" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
     <xf borderId="6" fillId="2" fontId="5" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
@@ -1545,45 +1545,54 @@
     <xf borderId="9" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="7" fillId="2" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
     <xf borderId="10" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="7" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
     <xf borderId="7" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="11" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="12" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="12" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="13" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="14" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="10" fillId="3" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf borderId="15" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="10" fillId="3" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="14" fillId="2" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="10" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="13" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="14" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    <xf borderId="14" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="10" fillId="3" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf borderId="14" fillId="4" fontId="8" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf borderId="10" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="15" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
     <xf borderId="16" fillId="3" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1596,217 +1605,208 @@
     <xf borderId="18" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
-    <xf borderId="19" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="19" fillId="2" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="20" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="center"/>
     </xf>
     <xf borderId="16" fillId="3" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="19" fillId="3" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="21" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="22" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="20" fillId="3" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="23" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="16" fillId="3" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
+    <xf borderId="5" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
     <xf borderId="17" fillId="3" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="16" fillId="3" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="5" fillId="2" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="16" fillId="3" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf borderId="14" fillId="2" fontId="8" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="14" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="6" fillId="2" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="24" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
+    <xf borderId="25" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
+    </xf>
+    <xf borderId="26" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="20" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="21" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="center" wrapText="1"/>
-    </xf>
-    <xf borderId="19" fillId="3" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="top"/>
     </xf>
-    <xf borderId="19" fillId="3" fontId="7" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="26" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
+    <xf borderId="20" fillId="3" fontId="9" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf borderId="26" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf borderId="10" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="14" fillId="4" fontId="9" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf borderId="22" fillId="2" fontId="10" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="26" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="27" fillId="2" fontId="10" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="23" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="28" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" vertical="bottom"/>
+    </xf>
+    <xf borderId="29" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="26" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="10" fillId="2" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="28" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="10" fillId="2" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="30" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
     <xf borderId="16" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="31" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="16" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="24" fillId="0" fontId="11" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="32" fillId="4" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="33" fillId="0" fontId="11" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="25" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="19" fillId="2" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="31" fillId="4" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="34" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="35" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="20" fillId="2" fontId="0" numFmtId="14" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="36" fillId="4" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="16" fillId="2" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="19" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="37" fillId="4" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="20" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf borderId="31" fillId="4" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
     </xf>
     <xf borderId="10" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf borderId="26" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+    <xf borderId="38" fillId="4" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="39" fillId="2" fontId="10" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="27" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="40" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="41" fillId="4" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="42" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="5" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="43" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="44" fillId="4" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf borderId="43" fillId="4" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="45" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="46" fillId="4" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="42" fillId="4" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="43" fillId="4" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="4" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+      <alignment readingOrder="0" vertical="bottom"/>
+    </xf>
+    <xf borderId="43" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="left" vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="12" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="28" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="29" fillId="2" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="30" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="31" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="32" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="6" fillId="2" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="33" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="33" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="33" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf borderId="33" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="34" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" vertical="bottom"/>
-    </xf>
-    <xf borderId="33" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="34" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="35" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="36" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="37" fillId="4" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="36" fillId="4" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="38" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="39" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="40" fillId="4" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="36" fillId="4" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="41" fillId="4" fontId="12" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
-    <xf borderId="42" fillId="4" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="43" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="5" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="44" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="45" fillId="4" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf borderId="44" fillId="4" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="46" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="47" fillId="4" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="43" fillId="4" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="44" fillId="4" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="0" fillId="4" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment readingOrder="0" vertical="bottom"/>
-    </xf>
-    <xf borderId="44" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
     <xf borderId="6" fillId="2" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="5" fillId="2" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="left" readingOrder="0" vertical="bottom"/>
     </xf>
+    <xf borderId="47" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="48" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
     <xf borderId="49" fillId="4" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
@@ -1816,7 +1816,7 @@
     <xf borderId="50" fillId="4" fontId="0" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="47" fillId="4" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="46" fillId="4" fontId="0" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" vertical="bottom"/>
     </xf>
     <xf borderId="49" fillId="4" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -1828,13 +1828,13 @@
     <xf borderId="51" fillId="4" fontId="0" numFmtId="166" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment readingOrder="0" vertical="bottom"/>
     </xf>
-    <xf borderId="35" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="35" fillId="2" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf borderId="35" fillId="2" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="30" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="30" fillId="2" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf borderId="30" fillId="2" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
     <xf borderId="52" fillId="2" fontId="0" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
@@ -1864,7 +1864,7 @@
     <xf borderId="5" fillId="2" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf borderId="54" fillId="2" fontId="4" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="54" fillId="2" fontId="3" numFmtId="165" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
     <xf borderId="0" fillId="2" fontId="15" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
@@ -1888,10 +1888,10 @@
     <xf borderId="59" fillId="2" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="34" fillId="2" fontId="4" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="28" fillId="2" fontId="3" numFmtId="49" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf borderId="60" fillId="2" fontId="4" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="60" fillId="2" fontId="3" numFmtId="167" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1941,25 +1941,25 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="7"/>
-      <c r="H1" s="5" t="s">
+      <c r="A1" s="3"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+      <c r="E1" s="2"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-      <c r="M1" s="3"/>
-      <c r="N1" s="9"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="2"/>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="8"/>
     </row>
     <row r="2" ht="13.5" customHeight="1">
-      <c r="A2" s="11"/>
+      <c r="A2" s="9"/>
       <c r="B2" s="12"/>
       <c r="C2" s="12"/>
       <c r="D2" s="12"/>
@@ -1977,7 +1977,7 @@
       <c r="N2" s="17"/>
     </row>
     <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="11"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -1995,7 +1995,7 @@
       <c r="N3" s="17"/>
     </row>
     <row r="4" ht="13.5" customHeight="1">
-      <c r="A4" s="11"/>
+      <c r="A4" s="9"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -2013,20 +2013,20 @@
       <c r="N4" s="17"/>
     </row>
     <row r="5" ht="19.5" customHeight="1">
-      <c r="A5" s="19"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="20"/>
-      <c r="J5" s="20"/>
-      <c r="K5" s="20"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="20"/>
-      <c r="N5" s="25"/>
+      <c r="A5" s="20"/>
+      <c r="B5" s="22"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="22"/>
+      <c r="E5" s="22"/>
+      <c r="F5" s="22"/>
+      <c r="G5" s="22"/>
+      <c r="H5" s="22"/>
+      <c r="I5" s="22"/>
+      <c r="J5" s="22"/>
+      <c r="K5" s="22"/>
+      <c r="L5" s="22"/>
+      <c r="M5" s="22"/>
+      <c r="N5" s="24"/>
     </row>
     <row r="6" ht="13.5" customHeight="1">
       <c r="A6" s="26" t="s">
@@ -2037,11 +2037,11 @@
       <c r="D6" s="15"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
-      <c r="G6" s="20"/>
+      <c r="G6" s="22"/>
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
-      <c r="K6" s="28" t="s">
+      <c r="K6" s="29" t="s">
         <v>8</v>
       </c>
       <c r="L6" s="15"/>
@@ -2063,7 +2063,7 @@
       <c r="H7" s="23"/>
       <c r="I7" s="23"/>
       <c r="J7" s="23"/>
-      <c r="K7" s="28" t="s">
+      <c r="K7" s="29" t="s">
         <v>10</v>
       </c>
       <c r="L7" s="15"/>
@@ -2083,7 +2083,7 @@
       <c r="H8" s="23"/>
       <c r="I8" s="23"/>
       <c r="J8" s="23"/>
-      <c r="K8" s="28" t="s">
+      <c r="K8" s="29" t="s">
         <v>12</v>
       </c>
       <c r="L8" s="15"/>
@@ -2093,7 +2093,7 @@
       </c>
     </row>
     <row r="9" ht="13.5" customHeight="1">
-      <c r="A9" s="8"/>
+      <c r="A9" s="10"/>
       <c r="B9" s="23"/>
       <c r="C9" s="34"/>
       <c r="D9" s="34"/>
@@ -2106,11 +2106,11 @@
       <c r="K9" s="15"/>
       <c r="L9" s="15"/>
       <c r="M9" s="15"/>
-      <c r="N9" s="25"/>
+      <c r="N9" s="24"/>
     </row>
     <row r="10" ht="13.5" customHeight="1">
-      <c r="A10" s="8"/>
-      <c r="B10" s="37"/>
+      <c r="A10" s="10"/>
+      <c r="B10" s="36"/>
       <c r="C10" s="38"/>
       <c r="D10" s="38"/>
       <c r="E10" s="38"/>
@@ -2122,158 +2122,158 @@
       <c r="K10" s="31"/>
       <c r="L10" s="31"/>
       <c r="M10" s="31"/>
-      <c r="N10" s="25"/>
+      <c r="N10" s="24"/>
     </row>
     <row r="11" ht="39.0" customHeight="1">
-      <c r="A11" s="44"/>
-      <c r="B11" s="45" t="s">
+      <c r="A11" s="40"/>
+      <c r="B11" s="42" t="s">
+        <v>14</v>
+      </c>
+      <c r="C11" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="C11" s="45" t="s">
+      <c r="E11" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="45" t="s">
+      <c r="F11" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="E11" s="45" t="s">
+      <c r="G11" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="F11" s="45" t="s">
+      <c r="H11" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="45" t="s">
+      <c r="I11" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="45" t="s">
+      <c r="J11" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="I11" s="45" t="s">
+      <c r="K11" s="42" t="s">
         <v>24</v>
       </c>
-      <c r="J11" s="45" t="s">
+      <c r="L11" s="42" t="s">
         <v>25</v>
       </c>
-      <c r="K11" s="45" t="s">
+      <c r="M11" s="42" t="s">
         <v>26</v>
       </c>
-      <c r="L11" s="45" t="s">
+      <c r="N11" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="M11" s="45" t="s">
-        <v>28</v>
-      </c>
-      <c r="N11" s="48" t="s">
+    </row>
+    <row r="12" ht="13.5" customHeight="1">
+      <c r="A12" s="46" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="12" ht="13.5" customHeight="1">
-      <c r="A12" s="59" t="s">
+      <c r="B12" s="48" t="s">
+        <v>30</v>
+      </c>
+      <c r="C12" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="B12" s="60" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="60" t="s">
-        <v>46</v>
-      </c>
-      <c r="D12" s="60" t="s">
-        <v>47</v>
-      </c>
-      <c r="E12" s="60" t="s">
-        <v>48</v>
-      </c>
-      <c r="F12" s="60" t="s">
-        <v>49</v>
-      </c>
-      <c r="G12" s="60" t="s">
-        <v>50</v>
-      </c>
-      <c r="H12" s="60" t="s">
-        <v>51</v>
-      </c>
-      <c r="I12" s="60" t="s">
-        <v>52</v>
-      </c>
-      <c r="J12" s="60" t="s">
-        <v>53</v>
-      </c>
-      <c r="K12" s="60" t="s">
-        <v>54</v>
-      </c>
-      <c r="L12" s="60" t="s">
-        <v>55</v>
-      </c>
-      <c r="M12" s="66" t="s">
-        <v>56</v>
-      </c>
-      <c r="N12" s="83" t="str">
+      <c r="D12" s="48" t="s">
+        <v>33</v>
+      </c>
+      <c r="E12" s="48" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12" s="48" t="s">
+        <v>35</v>
+      </c>
+      <c r="G12" s="48" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="48" t="s">
+        <v>37</v>
+      </c>
+      <c r="I12" s="48" t="s">
+        <v>38</v>
+      </c>
+      <c r="J12" s="48" t="s">
+        <v>39</v>
+      </c>
+      <c r="K12" s="48" t="s">
+        <v>40</v>
+      </c>
+      <c r="L12" s="48" t="s">
+        <v>41</v>
+      </c>
+      <c r="M12" s="50" t="s">
+        <v>42</v>
+      </c>
+      <c r="N12" s="56" t="str">
         <f t="shared" ref="N12:N13" si="1">ROUND(SUMIF(B12:L12,"&gt;0")*M12/12,2)</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="13" ht="13.5" customHeight="1">
-      <c r="A13" s="59" t="s">
-        <v>156</v>
-      </c>
-      <c r="B13" s="60" t="s">
-        <v>157</v>
-      </c>
-      <c r="C13" s="60" t="s">
-        <v>158</v>
-      </c>
-      <c r="D13" s="60" t="s">
-        <v>159</v>
-      </c>
-      <c r="E13" s="60" t="s">
-        <v>160</v>
-      </c>
-      <c r="F13" s="60" t="s">
-        <v>161</v>
-      </c>
-      <c r="G13" s="60" t="s">
-        <v>162</v>
-      </c>
-      <c r="H13" s="60" t="s">
-        <v>163</v>
-      </c>
-      <c r="I13" s="60" t="s">
-        <v>164</v>
-      </c>
-      <c r="J13" s="60" t="s">
-        <v>165</v>
-      </c>
-      <c r="K13" s="60" t="s">
-        <v>166</v>
-      </c>
-      <c r="L13" s="60" t="s">
-        <v>167</v>
-      </c>
-      <c r="M13" s="66" t="s">
-        <v>168</v>
-      </c>
-      <c r="N13" s="83" t="str">
+      <c r="A13" s="46" t="s">
+        <v>45</v>
+      </c>
+      <c r="B13" s="48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="D13" s="48" t="s">
+        <v>48</v>
+      </c>
+      <c r="E13" s="48" t="s">
+        <v>49</v>
+      </c>
+      <c r="F13" s="48" t="s">
+        <v>50</v>
+      </c>
+      <c r="G13" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="H13" s="48" t="s">
+        <v>52</v>
+      </c>
+      <c r="I13" s="48" t="s">
+        <v>53</v>
+      </c>
+      <c r="J13" s="48" t="s">
+        <v>54</v>
+      </c>
+      <c r="K13" s="48" t="s">
+        <v>55</v>
+      </c>
+      <c r="L13" s="48" t="s">
+        <v>56</v>
+      </c>
+      <c r="M13" s="50" t="s">
+        <v>57</v>
+      </c>
+      <c r="N13" s="56" t="str">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="14" ht="13.5" customHeight="1">
-      <c r="A14" s="85"/>
-      <c r="B14" s="86"/>
-      <c r="C14" s="86"/>
-      <c r="D14" s="86"/>
-      <c r="E14" s="86"/>
-      <c r="F14" s="86"/>
-      <c r="G14" s="86"/>
-      <c r="H14" s="86"/>
-      <c r="I14" s="86"/>
-      <c r="J14" s="86"/>
-      <c r="K14" s="86"/>
-      <c r="L14" s="86"/>
-      <c r="M14" s="86"/>
-      <c r="N14" s="88"/>
+      <c r="A14" s="59"/>
+      <c r="B14" s="60"/>
+      <c r="C14" s="60"/>
+      <c r="D14" s="60"/>
+      <c r="E14" s="60"/>
+      <c r="F14" s="60"/>
+      <c r="G14" s="60"/>
+      <c r="H14" s="60"/>
+      <c r="I14" s="60"/>
+      <c r="J14" s="60"/>
+      <c r="K14" s="60"/>
+      <c r="L14" s="60"/>
+      <c r="M14" s="60"/>
+      <c r="N14" s="62"/>
     </row>
     <row r="15" ht="13.5" customHeight="1">
-      <c r="A15" s="8"/>
+      <c r="A15" s="10"/>
       <c r="B15" s="15"/>
       <c r="C15" s="15"/>
       <c r="D15" s="15"/>
@@ -2284,17 +2284,17 @@
       <c r="I15" s="15"/>
       <c r="J15" s="15"/>
       <c r="K15" s="15"/>
-      <c r="L15" s="89"/>
-      <c r="M15" s="90" t="s">
-        <v>170</v>
-      </c>
-      <c r="N15" s="91" t="str">
+      <c r="L15" s="64"/>
+      <c r="M15" s="66" t="s">
+        <v>66</v>
+      </c>
+      <c r="N15" s="68" t="str">
         <f>SUM(N12:N13)</f>
         <v>#VALUE!</v>
       </c>
     </row>
     <row r="16" ht="13.5" customHeight="1">
-      <c r="A16" s="8"/>
+      <c r="A16" s="10"/>
       <c r="B16" s="15"/>
       <c r="C16" s="15"/>
       <c r="D16" s="15"/>
@@ -2307,377 +2307,377 @@
       <c r="K16" s="15"/>
       <c r="L16" s="15"/>
       <c r="M16" s="15"/>
-      <c r="N16" s="25"/>
+      <c r="N16" s="24"/>
     </row>
     <row r="17" ht="13.5" customHeight="1">
-      <c r="A17" s="8"/>
+      <c r="A17" s="10"/>
       <c r="B17" s="15"/>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
-      <c r="E17" s="28" t="s">
-        <v>171</v>
+      <c r="E17" s="29" t="s">
+        <v>71</v>
       </c>
       <c r="F17" s="15"/>
-      <c r="G17" s="92" t="s">
-        <v>172</v>
-      </c>
-      <c r="H17" s="92" t="s">
-        <v>172</v>
-      </c>
-      <c r="I17" s="28" t="s">
-        <v>173</v>
+      <c r="G17" s="70" t="s">
+        <v>72</v>
+      </c>
+      <c r="H17" s="70" t="s">
+        <v>72</v>
+      </c>
+      <c r="I17" s="29" t="s">
+        <v>73</v>
       </c>
       <c r="J17" s="15"/>
-      <c r="K17" s="28" t="s">
-        <v>174</v>
+      <c r="K17" s="29" t="s">
+        <v>74</v>
       </c>
       <c r="L17" s="15"/>
       <c r="M17" s="15"/>
-      <c r="N17" s="25"/>
+      <c r="N17" s="24"/>
     </row>
     <row r="18" ht="13.5" customHeight="1">
-      <c r="A18" s="8"/>
+      <c r="A18" s="10"/>
       <c r="B18" s="15"/>
-      <c r="C18" s="93" t="s">
-        <v>175</v>
-      </c>
-      <c r="D18" s="94"/>
-      <c r="E18" s="95" t="s">
-        <v>176</v>
-      </c>
-      <c r="F18" s="94"/>
-      <c r="G18" s="96" t="s">
+      <c r="C18" s="72" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="74"/>
+      <c r="E18" s="76" t="s">
+        <v>78</v>
+      </c>
+      <c r="F18" s="74"/>
+      <c r="G18" s="78" t="s">
+        <v>81</v>
+      </c>
+      <c r="H18" s="80" t="s">
+        <v>83</v>
+      </c>
+      <c r="I18" s="76" t="s">
+        <v>84</v>
+      </c>
+      <c r="J18" s="82"/>
+      <c r="K18" s="76" t="s">
+        <v>86</v>
+      </c>
+      <c r="L18" s="84"/>
+      <c r="M18" s="15"/>
+      <c r="N18" s="24"/>
+    </row>
+    <row r="19" ht="13.5" customHeight="1">
+      <c r="A19" s="10"/>
+      <c r="B19" s="15"/>
+      <c r="C19" s="86" t="s">
+        <v>87</v>
+      </c>
+      <c r="D19" s="88"/>
+      <c r="E19" s="90"/>
+      <c r="F19" s="92" t="s">
+        <v>91</v>
+      </c>
+      <c r="G19" s="94" t="s">
+        <v>92</v>
+      </c>
+      <c r="H19" s="96" t="s">
+        <v>93</v>
+      </c>
+      <c r="I19" s="98"/>
+      <c r="J19" s="100" t="s">
+        <v>97</v>
+      </c>
+      <c r="K19" s="102"/>
+      <c r="L19" s="105" t="s">
+        <v>102</v>
+      </c>
+      <c r="M19" s="106"/>
+      <c r="N19" s="24"/>
+    </row>
+    <row r="20" ht="13.5" customHeight="1">
+      <c r="A20" s="10"/>
+      <c r="B20" s="15"/>
+      <c r="C20" s="107" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="108"/>
+      <c r="E20" s="109"/>
+      <c r="F20" s="110" t="s">
+        <v>119</v>
+      </c>
+      <c r="G20" s="111" t="s">
+        <v>128</v>
+      </c>
+      <c r="H20" s="112" t="s">
+        <v>133</v>
+      </c>
+      <c r="I20" s="113"/>
+      <c r="J20" s="114" t="s">
+        <v>146</v>
+      </c>
+      <c r="K20" s="102"/>
+      <c r="L20" s="115" t="s">
+        <v>156</v>
+      </c>
+      <c r="M20" s="106"/>
+      <c r="N20" s="24"/>
+    </row>
+    <row r="21" ht="13.5" customHeight="1">
+      <c r="A21" s="10"/>
+      <c r="B21" s="15"/>
+      <c r="C21" s="29" t="s">
+        <v>160</v>
+      </c>
+      <c r="D21" s="116"/>
+      <c r="E21" s="109"/>
+      <c r="F21" s="110" t="s">
+        <v>169</v>
+      </c>
+      <c r="G21" s="111" t="s">
+        <v>170</v>
+      </c>
+      <c r="H21" s="112" t="s">
+        <v>172</v>
+      </c>
+      <c r="I21" s="113"/>
+      <c r="J21" s="114" t="s">
+        <v>173</v>
+      </c>
+      <c r="K21" s="102"/>
+      <c r="L21" s="115" t="s">
+        <v>174</v>
+      </c>
+      <c r="M21" s="106"/>
+      <c r="N21" s="24"/>
+    </row>
+    <row r="22" ht="13.5" customHeight="1">
+      <c r="A22" s="10"/>
+      <c r="B22" s="15"/>
+      <c r="C22" s="29" t="s">
         <v>177</v>
       </c>
-      <c r="H18" s="97" t="s">
-        <v>178</v>
-      </c>
-      <c r="I18" s="95" t="s">
+      <c r="D22" s="116"/>
+      <c r="E22" s="109"/>
+      <c r="F22" s="110" t="s">
         <v>179</v>
       </c>
-      <c r="J18" s="98"/>
-      <c r="K18" s="95" t="s">
+      <c r="G22" s="111" t="s">
         <v>180</v>
       </c>
-      <c r="L18" s="99"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="25"/>
-    </row>
-    <row r="19" ht="13.5" customHeight="1">
-      <c r="A19" s="8"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="100" t="s">
+      <c r="H22" s="112" t="s">
         <v>181</v>
       </c>
-      <c r="D19" s="101"/>
-      <c r="E19" s="102"/>
-      <c r="F19" s="103" t="s">
+      <c r="I22" s="113"/>
+      <c r="J22" s="114" t="s">
         <v>182</v>
       </c>
-      <c r="G19" s="104" t="s">
+      <c r="K22" s="102"/>
+      <c r="L22" s="115" t="s">
         <v>183</v>
       </c>
-      <c r="H19" s="105" t="s">
+      <c r="M22" s="106"/>
+      <c r="N22" s="24"/>
+    </row>
+    <row r="23" ht="13.5" customHeight="1">
+      <c r="A23" s="10"/>
+      <c r="B23" s="15"/>
+      <c r="C23" s="29" t="s">
         <v>184</v>
       </c>
-      <c r="I19" s="106"/>
-      <c r="J19" s="107" t="s">
+      <c r="D23" s="116"/>
+      <c r="E23" s="109"/>
+      <c r="F23" s="110" t="s">
         <v>185</v>
       </c>
-      <c r="K19" s="108"/>
-      <c r="L19" s="109" t="s">
-        <v>186</v>
-      </c>
-      <c r="M19" s="110"/>
-      <c r="N19" s="25"/>
-    </row>
-    <row r="20" ht="13.5" customHeight="1">
-      <c r="A20" s="8"/>
-      <c r="B20" s="15"/>
-      <c r="C20" s="111" t="s">
-        <v>187</v>
-      </c>
-      <c r="D20" s="112"/>
-      <c r="E20" s="113"/>
-      <c r="F20" s="114" t="s">
+      <c r="G23" s="111" t="s">
         <v>188</v>
       </c>
-      <c r="G20" s="115" t="s">
+      <c r="H23" s="112" t="s">
         <v>189</v>
       </c>
-      <c r="H20" s="116" t="s">
+      <c r="I23" s="113"/>
+      <c r="J23" s="114" t="s">
         <v>190</v>
       </c>
-      <c r="I20" s="117"/>
-      <c r="J20" s="118" t="s">
+      <c r="K23" s="102"/>
+      <c r="L23" s="115" t="s">
         <v>191</v>
       </c>
-      <c r="K20" s="108"/>
-      <c r="L20" s="119" t="s">
-        <v>192</v>
-      </c>
-      <c r="M20" s="110"/>
-      <c r="N20" s="25"/>
-    </row>
-    <row r="21" ht="13.5" customHeight="1">
-      <c r="A21" s="8"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="28" t="s">
-        <v>193</v>
-      </c>
-      <c r="D21" s="120"/>
-      <c r="E21" s="113"/>
-      <c r="F21" s="114" t="s">
-        <v>194</v>
-      </c>
-      <c r="G21" s="115" t="s">
-        <v>195</v>
-      </c>
-      <c r="H21" s="116" t="s">
-        <v>196</v>
-      </c>
-      <c r="I21" s="117"/>
-      <c r="J21" s="118" t="s">
-        <v>197</v>
-      </c>
-      <c r="K21" s="108"/>
-      <c r="L21" s="119" t="s">
+      <c r="M23" s="106"/>
+      <c r="N23" s="118"/>
+    </row>
+    <row r="24" ht="13.5" customHeight="1">
+      <c r="A24" s="10"/>
+      <c r="B24" s="15"/>
+      <c r="C24" s="29" t="s">
         <v>198</v>
       </c>
-      <c r="M21" s="110"/>
-      <c r="N21" s="25"/>
-    </row>
-    <row r="22" ht="13.5" customHeight="1">
-      <c r="A22" s="8"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="28" t="s">
-        <v>199</v>
-      </c>
-      <c r="D22" s="120"/>
-      <c r="E22" s="113"/>
-      <c r="F22" s="114" t="s">
+      <c r="D24" s="116"/>
+      <c r="E24" s="109"/>
+      <c r="F24" s="110" t="s">
         <v>200</v>
       </c>
-      <c r="G22" s="115" t="s">
+      <c r="G24" s="111" t="s">
         <v>201</v>
       </c>
-      <c r="H22" s="116" t="s">
+      <c r="H24" s="112" t="s">
         <v>202</v>
       </c>
-      <c r="I22" s="117"/>
-      <c r="J22" s="118" t="s">
+      <c r="I24" s="113"/>
+      <c r="J24" s="114" t="s">
         <v>203</v>
       </c>
-      <c r="K22" s="108"/>
-      <c r="L22" s="119" t="s">
-        <v>204</v>
-      </c>
-      <c r="M22" s="110"/>
-      <c r="N22" s="25"/>
-    </row>
-    <row r="23" ht="13.5" customHeight="1">
-      <c r="A23" s="8"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="28" t="s">
-        <v>205</v>
-      </c>
-      <c r="D23" s="120"/>
-      <c r="E23" s="113"/>
-      <c r="F23" s="114" t="s">
+      <c r="K24" s="102"/>
+      <c r="L24" s="115" t="s">
         <v>206</v>
       </c>
-      <c r="G23" s="115" t="s">
-        <v>207</v>
-      </c>
-      <c r="H23" s="116" t="s">
+      <c r="M24" s="106"/>
+      <c r="N24" s="24"/>
+    </row>
+    <row r="25" ht="13.5" customHeight="1">
+      <c r="A25" s="10"/>
+      <c r="B25" s="15"/>
+      <c r="C25" s="119" t="s">
         <v>208</v>
       </c>
-      <c r="I23" s="117"/>
-      <c r="J23" s="118" t="s">
-        <v>209</v>
-      </c>
-      <c r="K23" s="108"/>
-      <c r="L23" s="119" t="s">
-        <v>210</v>
-      </c>
-      <c r="M23" s="110"/>
-      <c r="N23" s="121"/>
-    </row>
-    <row r="24" ht="13.5" customHeight="1">
-      <c r="A24" s="8"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="28" t="s">
+      <c r="D25" s="116"/>
+      <c r="E25" s="109"/>
+      <c r="F25" s="110" t="s">
         <v>211</v>
       </c>
-      <c r="D24" s="120"/>
-      <c r="E24" s="113"/>
-      <c r="F24" s="114" t="s">
-        <v>212</v>
-      </c>
-      <c r="G24" s="115" t="s">
+      <c r="G25" s="111" t="s">
         <v>213</v>
       </c>
-      <c r="H24" s="116" t="s">
-        <v>214</v>
-      </c>
-      <c r="I24" s="117"/>
-      <c r="J24" s="118" t="s">
+      <c r="H25" s="112" t="s">
         <v>215</v>
       </c>
-      <c r="K24" s="108"/>
-      <c r="L24" s="119" t="s">
-        <v>216</v>
-      </c>
-      <c r="M24" s="110"/>
-      <c r="N24" s="25"/>
-    </row>
-    <row r="25" ht="13.5" customHeight="1">
-      <c r="A25" s="8"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="122" t="s">
+      <c r="I25" s="113"/>
+      <c r="J25" s="114" t="s">
         <v>217</v>
       </c>
-      <c r="D25" s="120"/>
-      <c r="E25" s="113"/>
-      <c r="F25" s="114" t="s">
+      <c r="K25" s="102"/>
+      <c r="L25" s="115" t="s">
         <v>218</v>
       </c>
-      <c r="G25" s="115" t="s">
+      <c r="M25" s="106"/>
+      <c r="N25" s="24"/>
+    </row>
+    <row r="26" ht="13.5" customHeight="1">
+      <c r="A26" s="10"/>
+      <c r="B26" s="15"/>
+      <c r="C26" s="29" t="s">
         <v>219</v>
       </c>
-      <c r="H25" s="116" t="s">
+      <c r="D26" s="116"/>
+      <c r="E26" s="109"/>
+      <c r="F26" s="110" t="s">
         <v>220</v>
       </c>
-      <c r="I25" s="117"/>
-      <c r="J25" s="118" t="s">
+      <c r="G26" s="111" t="s">
         <v>221</v>
       </c>
-      <c r="K25" s="108"/>
-      <c r="L25" s="119" t="s">
+      <c r="H26" s="112" t="s">
         <v>222</v>
       </c>
-      <c r="M25" s="110"/>
-      <c r="N25" s="25"/>
-    </row>
-    <row r="26" ht="13.5" customHeight="1">
-      <c r="A26" s="8"/>
-      <c r="B26" s="15"/>
-      <c r="C26" s="28" t="s">
+      <c r="I26" s="113"/>
+      <c r="J26" s="114" t="s">
         <v>223</v>
       </c>
-      <c r="D26" s="120"/>
-      <c r="E26" s="113"/>
-      <c r="F26" s="114" t="s">
+      <c r="K26" s="102"/>
+      <c r="L26" s="115" t="s">
         <v>224</v>
       </c>
-      <c r="G26" s="115" t="s">
+      <c r="M26" s="106"/>
+      <c r="N26" s="24"/>
+    </row>
+    <row r="27" ht="13.5" customHeight="1">
+      <c r="A27" s="10"/>
+      <c r="B27" s="15"/>
+      <c r="C27" s="29" t="s">
         <v>225</v>
       </c>
-      <c r="H26" s="116" t="s">
+      <c r="D27" s="116"/>
+      <c r="E27" s="109"/>
+      <c r="F27" s="110" t="s">
         <v>226</v>
       </c>
-      <c r="I26" s="117"/>
-      <c r="J26" s="118" t="s">
+      <c r="G27" s="111" t="s">
         <v>227</v>
       </c>
-      <c r="K26" s="108"/>
-      <c r="L26" s="119" t="s">
+      <c r="H27" s="112" t="s">
         <v>228</v>
       </c>
-      <c r="M26" s="110"/>
-      <c r="N26" s="25"/>
-    </row>
-    <row r="27" ht="13.5" customHeight="1">
-      <c r="A27" s="8"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="28" t="s">
+      <c r="I27" s="113"/>
+      <c r="J27" s="114" t="s">
         <v>229</v>
       </c>
-      <c r="D27" s="120"/>
-      <c r="E27" s="113"/>
-      <c r="F27" s="114" t="s">
+      <c r="K27" s="102"/>
+      <c r="L27" s="115" t="s">
         <v>230</v>
       </c>
-      <c r="G27" s="115" t="s">
+      <c r="M27" s="106"/>
+      <c r="N27" s="24"/>
+    </row>
+    <row r="28" ht="13.5" customHeight="1">
+      <c r="A28" s="10"/>
+      <c r="B28" s="15"/>
+      <c r="C28" s="29" t="s">
         <v>231</v>
       </c>
-      <c r="H27" s="116" t="s">
+      <c r="D28" s="116"/>
+      <c r="E28" s="109"/>
+      <c r="F28" s="110" t="s">
         <v>232</v>
       </c>
-      <c r="I27" s="117"/>
-      <c r="J27" s="118" t="s">
+      <c r="G28" s="111" t="s">
         <v>233</v>
       </c>
-      <c r="K27" s="108"/>
-      <c r="L27" s="119" t="s">
+      <c r="H28" s="112" t="s">
         <v>234</v>
       </c>
-      <c r="M27" s="110"/>
-      <c r="N27" s="25"/>
-    </row>
-    <row r="28" ht="13.5" customHeight="1">
-      <c r="A28" s="8"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="28" t="s">
+      <c r="I28" s="113"/>
+      <c r="J28" s="114" t="s">
         <v>235</v>
       </c>
-      <c r="D28" s="120"/>
-      <c r="E28" s="113"/>
-      <c r="F28" s="114" t="s">
+      <c r="K28" s="102"/>
+      <c r="L28" s="115" t="s">
         <v>236</v>
       </c>
-      <c r="G28" s="115" t="s">
-        <v>237</v>
-      </c>
-      <c r="H28" s="116" t="s">
+      <c r="M28" s="106"/>
+      <c r="N28" s="24"/>
+    </row>
+    <row r="29" ht="13.5" customHeight="1">
+      <c r="A29" s="10"/>
+      <c r="B29" s="15"/>
+      <c r="C29" s="29" t="s">
         <v>238</v>
       </c>
-      <c r="I28" s="117"/>
-      <c r="J28" s="118" t="s">
-        <v>239</v>
-      </c>
-      <c r="K28" s="108"/>
-      <c r="L28" s="119" t="s">
+      <c r="D29" s="116"/>
+      <c r="E29" s="109"/>
+      <c r="F29" s="110" t="s">
         <v>240</v>
       </c>
-      <c r="M28" s="110"/>
-      <c r="N28" s="25"/>
-    </row>
-    <row r="29" ht="13.5" customHeight="1">
-      <c r="A29" s="8"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="28" t="s">
+      <c r="G29" s="111" t="s">
         <v>241</v>
       </c>
-      <c r="D29" s="120"/>
-      <c r="E29" s="113"/>
-      <c r="F29" s="114" t="s">
-        <v>242</v>
-      </c>
-      <c r="G29" s="115" t="s">
+      <c r="H29" s="112" t="s">
         <v>243</v>
       </c>
-      <c r="H29" s="116" t="s">
+      <c r="I29" s="113"/>
+      <c r="J29" s="114" t="s">
         <v>244</v>
       </c>
-      <c r="I29" s="117"/>
-      <c r="J29" s="118" t="s">
+      <c r="K29" s="102"/>
+      <c r="L29" s="115" t="s">
         <v>245</v>
       </c>
-      <c r="K29" s="108"/>
-      <c r="L29" s="119" t="s">
+      <c r="M29" s="106"/>
+      <c r="N29" s="24"/>
+    </row>
+    <row r="30" ht="13.5" customHeight="1">
+      <c r="A30" s="10"/>
+      <c r="B30" s="15"/>
+      <c r="C30" s="76" t="s">
         <v>246</v>
       </c>
-      <c r="M29" s="110"/>
-      <c r="N29" s="25"/>
-    </row>
-    <row r="30" ht="13.5" customHeight="1">
-      <c r="A30" s="8"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="95" t="s">
-        <v>247</v>
-      </c>
-      <c r="D30" s="123"/>
+      <c r="D30" s="122"/>
       <c r="E30" s="124"/>
       <c r="F30" s="125" t="s">
         <v>248</v>
@@ -2692,15 +2692,15 @@
       <c r="J30" s="129" t="s">
         <v>251</v>
       </c>
-      <c r="K30" s="108"/>
+      <c r="K30" s="102"/>
       <c r="L30" s="130" t="s">
         <v>252</v>
       </c>
-      <c r="M30" s="110"/>
-      <c r="N30" s="25"/>
+      <c r="M30" s="106"/>
+      <c r="N30" s="24"/>
     </row>
     <row r="31" ht="13.5" customHeight="1">
-      <c r="A31" s="8"/>
+      <c r="A31" s="10"/>
       <c r="B31" s="15"/>
       <c r="C31" s="131"/>
       <c r="D31" s="131"/>
@@ -2722,7 +2722,7 @@
         <v>0</v>
       </c>
       <c r="M31" s="15"/>
-      <c r="N31" s="25"/>
+      <c r="N31" s="24"/>
     </row>
     <row r="32" ht="13.5" customHeight="1">
       <c r="A32" s="135"/>
@@ -2742,7 +2742,7 @@
       <c r="K32" s="134"/>
       <c r="L32" s="134"/>
       <c r="M32" s="15"/>
-      <c r="N32" s="25"/>
+      <c r="N32" s="24"/>
     </row>
     <row r="33" ht="13.5" customHeight="1">
       <c r="A33" s="140"/>
@@ -2760,7 +2760,7 @@
       <c r="K33" s="134"/>
       <c r="L33" s="134"/>
       <c r="M33" s="15"/>
-      <c r="N33" s="25"/>
+      <c r="N33" s="24"/>
     </row>
     <row r="34" ht="13.5" customHeight="1">
       <c r="A34" s="140"/>
@@ -2778,7 +2778,7 @@
       <c r="K34" s="15"/>
       <c r="L34" s="15"/>
       <c r="M34" s="15"/>
-      <c r="N34" s="25"/>
+      <c r="N34" s="24"/>
     </row>
     <row r="35" ht="13.5" customHeight="1">
       <c r="A35" s="140"/>
@@ -2795,7 +2795,7 @@
       <c r="J35" s="15"/>
       <c r="K35" s="15"/>
       <c r="L35" s="15"/>
-      <c r="M35" s="90" t="s">
+      <c r="M35" s="66" t="s">
         <v>257</v>
       </c>
       <c r="N35" s="143">
@@ -2831,25 +2831,25 @@
       </c>
       <c r="D37" s="148"/>
       <c r="E37" s="149"/>
-      <c r="F37" s="99"/>
-      <c r="G37" s="99"/>
-      <c r="H37" s="99"/>
-      <c r="I37" s="99"/>
-      <c r="J37" s="99"/>
-      <c r="K37" s="99"/>
-      <c r="L37" s="99"/>
-      <c r="M37" s="99"/>
+      <c r="F37" s="84"/>
+      <c r="G37" s="84"/>
+      <c r="H37" s="84"/>
+      <c r="I37" s="84"/>
+      <c r="J37" s="84"/>
+      <c r="K37" s="84"/>
+      <c r="L37" s="84"/>
+      <c r="M37" s="84"/>
       <c r="N37" s="150"/>
     </row>
     <row r="38" ht="13.5" customHeight="1">
-      <c r="D38" s="99"/>
-      <c r="F38" s="99"/>
-      <c r="G38" s="99"/>
-      <c r="H38" s="99"/>
-      <c r="I38" s="99"/>
-      <c r="J38" s="99"/>
-      <c r="K38" s="99"/>
-      <c r="L38" s="99"/>
+      <c r="D38" s="84"/>
+      <c r="F38" s="84"/>
+      <c r="G38" s="84"/>
+      <c r="H38" s="84"/>
+      <c r="I38" s="84"/>
+      <c r="J38" s="84"/>
+      <c r="K38" s="84"/>
+      <c r="L38" s="84"/>
       <c r="M38" s="151" t="str">
         <f>IF(N15-N35&gt;=0,"Net Due to Charter School:","Net Due to School District:")</f>
         <v>#VALUE!</v>
@@ -3860,37 +3860,37 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="2"/>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
+      <c r="A1" s="1"/>
+      <c r="B1" s="2"/>
+      <c r="C1" s="2"/>
       <c r="D1" s="4"/>
       <c r="E1" s="4"/>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="6" t="s">
         <v>0</v>
       </c>
       <c r="G1" s="4"/>
       <c r="H1" s="4"/>
       <c r="I1" s="4"/>
       <c r="J1" s="4"/>
-      <c r="K1" s="6"/>
+      <c r="K1" s="7"/>
     </row>
     <row r="2">
-      <c r="A2" s="8"/>
-      <c r="B2" s="10"/>
-      <c r="C2" s="10"/>
-      <c r="D2" s="10"/>
-      <c r="E2" s="10"/>
+      <c r="A2" s="10"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11"/>
+      <c r="D2" s="11"/>
+      <c r="E2" s="11"/>
       <c r="F2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
+      <c r="J2" s="11"/>
       <c r="K2" s="14"/>
     </row>
     <row r="3" ht="13.5" customHeight="1">
-      <c r="A3" s="8"/>
+      <c r="A3" s="10"/>
       <c r="B3" s="12"/>
       <c r="C3" s="12"/>
       <c r="D3" s="12"/>
@@ -3905,7 +3905,7 @@
       <c r="K3" s="17"/>
     </row>
     <row r="4" ht="12.75" customHeight="1">
-      <c r="A4" s="8"/>
+      <c r="A4" s="10"/>
       <c r="B4" s="12"/>
       <c r="C4" s="12"/>
       <c r="D4" s="12"/>
@@ -3920,39 +3920,39 @@
       <c r="K4" s="17"/>
     </row>
     <row r="5" ht="12.75" customHeight="1">
-      <c r="A5" s="8"/>
-      <c r="B5" s="21" t="s">
+      <c r="A5" s="10"/>
+      <c r="B5" s="19" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
+      <c r="C5" s="21"/>
+      <c r="D5" s="21"/>
       <c r="E5" s="15"/>
       <c r="F5" s="15"/>
       <c r="G5" s="23"/>
       <c r="H5" s="23"/>
       <c r="I5" s="23"/>
       <c r="J5" s="23"/>
-      <c r="K5" s="24"/>
+      <c r="K5" s="25"/>
     </row>
     <row r="6" ht="12.75" customHeight="1">
-      <c r="A6" s="8"/>
-      <c r="B6" s="21" t="s">
+      <c r="A6" s="10"/>
+      <c r="B6" s="19" t="s">
         <v>7</v>
       </c>
       <c r="C6" s="15"/>
-      <c r="D6" s="22"/>
+      <c r="D6" s="21"/>
       <c r="E6" s="15"/>
       <c r="F6" s="15"/>
       <c r="G6" s="27"/>
       <c r="H6" s="27"/>
-      <c r="I6" s="29"/>
-      <c r="J6" s="22"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="21"/>
       <c r="K6" s="30" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="7" ht="12.75" customHeight="1">
-      <c r="A7" s="8"/>
+      <c r="A7" s="10"/>
       <c r="B7" s="31"/>
       <c r="C7" s="31"/>
       <c r="D7" s="31"/>
@@ -3966,745 +3966,745 @@
     </row>
     <row r="8" ht="12.75" customHeight="1">
       <c r="A8" s="35"/>
-      <c r="B8" s="36"/>
-      <c r="C8" s="36"/>
+      <c r="B8" s="37"/>
+      <c r="C8" s="37"/>
       <c r="D8" s="39"/>
-      <c r="E8" s="40"/>
-      <c r="F8" s="41" t="s">
-        <v>14</v>
-      </c>
-      <c r="G8" s="42" t="s">
+      <c r="E8" s="41"/>
+      <c r="F8" s="43" t="s">
         <v>15</v>
       </c>
-      <c r="H8" s="43"/>
-      <c r="I8" s="46" t="s">
-        <v>16</v>
-      </c>
-      <c r="J8" s="47"/>
-      <c r="K8" s="42" t="s">
-        <v>30</v>
+      <c r="G8" s="45" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="47"/>
+      <c r="I8" s="49" t="s">
+        <v>31</v>
+      </c>
+      <c r="J8" s="51"/>
+      <c r="K8" s="45" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" ht="12.75" customHeight="1">
       <c r="A9" s="35"/>
-      <c r="B9" s="49" t="s">
-        <v>31</v>
-      </c>
-      <c r="C9" s="50"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="52"/>
-      <c r="F9" s="53"/>
-      <c r="G9" s="49" t="s">
-        <v>33</v>
-      </c>
-      <c r="H9" s="54" t="s">
-        <v>34</v>
-      </c>
-      <c r="I9" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="J9" s="49" t="s">
-        <v>36</v>
-      </c>
-      <c r="K9" s="55" t="s">
-        <v>37</v>
+      <c r="B9" s="52" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" s="53"/>
+      <c r="D9" s="54"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="57"/>
+      <c r="G9" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="58" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="J9" s="52" t="s">
+        <v>61</v>
+      </c>
+      <c r="K9" s="61" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="10" ht="12.75" customHeight="1">
       <c r="A10" s="35"/>
-      <c r="B10" s="49" t="s">
-        <v>38</v>
-      </c>
-      <c r="C10" s="56" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="57" t="s">
-        <v>40</v>
-      </c>
-      <c r="E10" s="52"/>
-      <c r="F10" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="G10" s="49" t="s">
-        <v>42</v>
-      </c>
-      <c r="H10" s="54" t="s">
-        <v>35</v>
-      </c>
-      <c r="I10" s="58" t="s">
+      <c r="B10" s="52" t="s">
+        <v>63</v>
+      </c>
+      <c r="C10" s="63" t="s">
+        <v>64</v>
+      </c>
+      <c r="D10" s="65" t="s">
+        <v>65</v>
+      </c>
+      <c r="E10" s="55"/>
+      <c r="F10" s="45" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="52" t="s">
+        <v>68</v>
+      </c>
+      <c r="H10" s="58" t="s">
+        <v>60</v>
+      </c>
+      <c r="I10" s="67" t="s">
+        <v>69</v>
+      </c>
+      <c r="J10" s="52" t="s">
+        <v>70</v>
+      </c>
+      <c r="K10" s="45" t="s">
         <v>43</v>
-      </c>
-      <c r="J10" s="49" t="s">
-        <v>44</v>
-      </c>
-      <c r="K10" s="42" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="11" ht="13.5" customHeight="1">
       <c r="A11" s="35"/>
-      <c r="B11" s="53"/>
-      <c r="C11" s="53"/>
-      <c r="D11" s="61"/>
-      <c r="E11" s="62"/>
-      <c r="F11" s="53"/>
-      <c r="G11" s="55" t="s">
-        <v>57</v>
-      </c>
-      <c r="H11" s="63"/>
-      <c r="I11" s="64" t="s">
-        <v>58</v>
-      </c>
-      <c r="J11" s="55" t="s">
-        <v>59</v>
-      </c>
-      <c r="K11" s="55" t="s">
-        <v>60</v>
+      <c r="B11" s="57"/>
+      <c r="C11" s="57"/>
+      <c r="D11" s="69"/>
+      <c r="E11" s="71"/>
+      <c r="F11" s="57"/>
+      <c r="G11" s="61" t="s">
+        <v>76</v>
+      </c>
+      <c r="H11" s="73"/>
+      <c r="I11" s="75" t="s">
+        <v>77</v>
+      </c>
+      <c r="J11" s="61" t="s">
+        <v>79</v>
+      </c>
+      <c r="K11" s="61" t="s">
+        <v>80</v>
       </c>
     </row>
     <row r="12" ht="13.5" customHeight="1">
       <c r="A12" s="35"/>
-      <c r="B12" s="65"/>
-      <c r="C12" s="65"/>
-      <c r="D12" s="67" t="s">
-        <v>61</v>
-      </c>
-      <c r="E12" s="68"/>
-      <c r="F12" s="69" t="s">
-        <v>62</v>
-      </c>
-      <c r="G12" s="70"/>
-      <c r="H12" s="70"/>
-      <c r="I12" s="70"/>
-      <c r="J12" s="65"/>
-      <c r="K12" s="69" t="s">
-        <v>63</v>
+      <c r="B12" s="77"/>
+      <c r="C12" s="77"/>
+      <c r="D12" s="79" t="s">
+        <v>82</v>
+      </c>
+      <c r="E12" s="81"/>
+      <c r="F12" s="83" t="s">
+        <v>85</v>
+      </c>
+      <c r="G12" s="85"/>
+      <c r="H12" s="85"/>
+      <c r="I12" s="85"/>
+      <c r="J12" s="77"/>
+      <c r="K12" s="83" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="13" ht="12.75" customHeight="1">
       <c r="A13" s="35"/>
-      <c r="B13" s="71">
+      <c r="B13" s="87">
         <v>1.0</v>
       </c>
-      <c r="C13" s="72" t="s">
-        <v>64</v>
-      </c>
-      <c r="D13" s="73" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="74"/>
-      <c r="F13" s="75"/>
-      <c r="G13" s="71"/>
-      <c r="H13" s="76" t="s">
-        <v>66</v>
-      </c>
-      <c r="I13" s="76" t="s">
-        <v>67</v>
-      </c>
-      <c r="J13" s="72" t="s">
-        <v>68</v>
-      </c>
-      <c r="K13" s="77"/>
+      <c r="C13" s="89" t="s">
+        <v>89</v>
+      </c>
+      <c r="D13" s="91" t="s">
+        <v>90</v>
+      </c>
+      <c r="E13" s="93"/>
+      <c r="F13" s="95"/>
+      <c r="G13" s="87"/>
+      <c r="H13" s="97" t="s">
+        <v>94</v>
+      </c>
+      <c r="I13" s="97" t="s">
+        <v>95</v>
+      </c>
+      <c r="J13" s="89" t="s">
+        <v>96</v>
+      </c>
+      <c r="K13" s="99"/>
     </row>
     <row r="14" ht="12.75" customHeight="1">
       <c r="A14" s="35"/>
-      <c r="B14" s="71"/>
-      <c r="C14" s="71"/>
-      <c r="D14" s="73" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="74"/>
-      <c r="F14" s="78" t="s">
-        <v>70</v>
-      </c>
-      <c r="G14" s="71"/>
-      <c r="H14" s="71"/>
-      <c r="I14" s="71"/>
-      <c r="J14" s="71"/>
-      <c r="K14" s="69" t="s">
-        <v>71</v>
+      <c r="B14" s="87"/>
+      <c r="C14" s="87"/>
+      <c r="D14" s="91" t="s">
+        <v>98</v>
+      </c>
+      <c r="E14" s="93"/>
+      <c r="F14" s="101" t="s">
+        <v>99</v>
+      </c>
+      <c r="G14" s="87"/>
+      <c r="H14" s="87"/>
+      <c r="I14" s="87"/>
+      <c r="J14" s="87"/>
+      <c r="K14" s="83" t="s">
+        <v>100</v>
       </c>
     </row>
     <row r="15" ht="13.5" customHeight="1">
       <c r="A15" s="35"/>
-      <c r="B15" s="77"/>
-      <c r="C15" s="77"/>
-      <c r="D15" s="79" t="s">
-        <v>72</v>
-      </c>
-      <c r="E15" s="80"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="77"/>
-      <c r="H15" s="77"/>
-      <c r="I15" s="77"/>
-      <c r="J15" s="77"/>
-      <c r="K15" s="77"/>
+      <c r="B15" s="99"/>
+      <c r="C15" s="99"/>
+      <c r="D15" s="103" t="s">
+        <v>101</v>
+      </c>
+      <c r="E15" s="104"/>
+      <c r="F15" s="99"/>
+      <c r="G15" s="99"/>
+      <c r="H15" s="99"/>
+      <c r="I15" s="99"/>
+      <c r="J15" s="99"/>
+      <c r="K15" s="99"/>
     </row>
     <row r="16" ht="12.75" customHeight="1">
       <c r="A16" s="35"/>
-      <c r="B16" s="65"/>
-      <c r="C16" s="65"/>
-      <c r="D16" s="67" t="s">
-        <v>73</v>
-      </c>
-      <c r="E16" s="68"/>
-      <c r="F16" s="69" t="s">
-        <v>74</v>
-      </c>
-      <c r="G16" s="70"/>
-      <c r="H16" s="70"/>
-      <c r="I16" s="70"/>
-      <c r="J16" s="65"/>
-      <c r="K16" s="69" t="s">
-        <v>75</v>
+      <c r="B16" s="77"/>
+      <c r="C16" s="77"/>
+      <c r="D16" s="79" t="s">
+        <v>103</v>
+      </c>
+      <c r="E16" s="81"/>
+      <c r="F16" s="83" t="s">
+        <v>104</v>
+      </c>
+      <c r="G16" s="85"/>
+      <c r="H16" s="85"/>
+      <c r="I16" s="85"/>
+      <c r="J16" s="77"/>
+      <c r="K16" s="83" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="17" ht="12.75" customHeight="1">
       <c r="A17" s="35"/>
-      <c r="B17" s="71">
+      <c r="B17" s="87">
         <f>B13+1</f>
         <v>2</v>
       </c>
-      <c r="C17" s="72" t="s">
-        <v>76</v>
-      </c>
-      <c r="D17" s="73" t="s">
-        <v>77</v>
-      </c>
-      <c r="E17" s="74"/>
-      <c r="F17" s="75"/>
-      <c r="G17" s="71"/>
-      <c r="H17" s="76" t="s">
-        <v>78</v>
-      </c>
-      <c r="I17" s="76" t="s">
-        <v>79</v>
-      </c>
-      <c r="J17" s="72" t="s">
-        <v>80</v>
-      </c>
-      <c r="K17" s="77"/>
+      <c r="C17" s="89" t="s">
+        <v>107</v>
+      </c>
+      <c r="D17" s="91" t="s">
+        <v>108</v>
+      </c>
+      <c r="E17" s="93"/>
+      <c r="F17" s="95"/>
+      <c r="G17" s="87"/>
+      <c r="H17" s="97" t="s">
+        <v>109</v>
+      </c>
+      <c r="I17" s="97" t="s">
+        <v>110</v>
+      </c>
+      <c r="J17" s="89" t="s">
+        <v>111</v>
+      </c>
+      <c r="K17" s="99"/>
     </row>
     <row r="18" ht="12.75" customHeight="1">
       <c r="A18" s="35"/>
-      <c r="B18" s="71"/>
-      <c r="C18" s="71"/>
-      <c r="D18" s="73" t="s">
-        <v>81</v>
-      </c>
-      <c r="E18" s="74"/>
-      <c r="F18" s="78" t="s">
-        <v>82</v>
-      </c>
-      <c r="G18" s="71"/>
-      <c r="H18" s="71"/>
-      <c r="I18" s="71"/>
-      <c r="J18" s="71"/>
-      <c r="K18" s="69" t="s">
-        <v>83</v>
+      <c r="B18" s="87"/>
+      <c r="C18" s="87"/>
+      <c r="D18" s="91" t="s">
+        <v>112</v>
+      </c>
+      <c r="E18" s="93"/>
+      <c r="F18" s="101" t="s">
+        <v>113</v>
+      </c>
+      <c r="G18" s="87"/>
+      <c r="H18" s="87"/>
+      <c r="I18" s="87"/>
+      <c r="J18" s="87"/>
+      <c r="K18" s="83" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="19" ht="12.75" customHeight="1">
       <c r="A19" s="35"/>
-      <c r="B19" s="77"/>
-      <c r="C19" s="77"/>
-      <c r="D19" s="79" t="s">
-        <v>84</v>
-      </c>
-      <c r="E19" s="80"/>
-      <c r="F19" s="77"/>
-      <c r="G19" s="77"/>
-      <c r="H19" s="77"/>
-      <c r="I19" s="77"/>
-      <c r="J19" s="77"/>
-      <c r="K19" s="77"/>
+      <c r="B19" s="99"/>
+      <c r="C19" s="99"/>
+      <c r="D19" s="103" t="s">
+        <v>115</v>
+      </c>
+      <c r="E19" s="104"/>
+      <c r="F19" s="99"/>
+      <c r="G19" s="99"/>
+      <c r="H19" s="99"/>
+      <c r="I19" s="99"/>
+      <c r="J19" s="99"/>
+      <c r="K19" s="99"/>
     </row>
     <row r="20" ht="12.75" customHeight="1">
       <c r="A20" s="35"/>
-      <c r="B20" s="65"/>
-      <c r="C20" s="65"/>
-      <c r="D20" s="67" t="s">
-        <v>85</v>
-      </c>
-      <c r="E20" s="68"/>
-      <c r="F20" s="69" t="s">
-        <v>86</v>
-      </c>
-      <c r="G20" s="70"/>
-      <c r="H20" s="70"/>
-      <c r="I20" s="70"/>
-      <c r="J20" s="65"/>
-      <c r="K20" s="69" t="s">
-        <v>87</v>
+      <c r="B20" s="77"/>
+      <c r="C20" s="77"/>
+      <c r="D20" s="79" t="s">
+        <v>116</v>
+      </c>
+      <c r="E20" s="81"/>
+      <c r="F20" s="83" t="s">
+        <v>117</v>
+      </c>
+      <c r="G20" s="85"/>
+      <c r="H20" s="85"/>
+      <c r="I20" s="85"/>
+      <c r="J20" s="77"/>
+      <c r="K20" s="83" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="21" ht="12.75" customHeight="1">
       <c r="A21" s="35"/>
-      <c r="B21" s="71">
+      <c r="B21" s="87">
         <f>B17+1</f>
         <v>3</v>
       </c>
-      <c r="C21" s="72" t="s">
-        <v>88</v>
-      </c>
-      <c r="D21" s="73" t="s">
-        <v>89</v>
-      </c>
-      <c r="E21" s="74"/>
-      <c r="F21" s="75"/>
-      <c r="G21" s="71"/>
-      <c r="H21" s="76" t="s">
-        <v>90</v>
-      </c>
-      <c r="I21" s="76" t="s">
-        <v>91</v>
-      </c>
-      <c r="J21" s="72" t="s">
-        <v>92</v>
-      </c>
-      <c r="K21" s="77"/>
+      <c r="C21" s="89" t="s">
+        <v>120</v>
+      </c>
+      <c r="D21" s="91" t="s">
+        <v>121</v>
+      </c>
+      <c r="E21" s="93"/>
+      <c r="F21" s="95"/>
+      <c r="G21" s="87"/>
+      <c r="H21" s="97" t="s">
+        <v>122</v>
+      </c>
+      <c r="I21" s="97" t="s">
+        <v>123</v>
+      </c>
+      <c r="J21" s="89" t="s">
+        <v>124</v>
+      </c>
+      <c r="K21" s="99"/>
     </row>
     <row r="22" ht="12.75" customHeight="1">
       <c r="A22" s="35"/>
-      <c r="B22" s="71"/>
-      <c r="C22" s="71"/>
-      <c r="D22" s="73" t="s">
-        <v>93</v>
-      </c>
-      <c r="E22" s="74"/>
-      <c r="F22" s="78" t="s">
-        <v>94</v>
-      </c>
-      <c r="G22" s="71"/>
-      <c r="H22" s="71"/>
-      <c r="I22" s="71"/>
-      <c r="J22" s="71"/>
-      <c r="K22" s="69" t="s">
-        <v>95</v>
+      <c r="B22" s="87"/>
+      <c r="C22" s="87"/>
+      <c r="D22" s="91" t="s">
+        <v>125</v>
+      </c>
+      <c r="E22" s="93"/>
+      <c r="F22" s="101" t="s">
+        <v>126</v>
+      </c>
+      <c r="G22" s="87"/>
+      <c r="H22" s="87"/>
+      <c r="I22" s="87"/>
+      <c r="J22" s="87"/>
+      <c r="K22" s="83" t="s">
+        <v>127</v>
       </c>
     </row>
     <row r="23" ht="12.75" customHeight="1">
       <c r="A23" s="35"/>
-      <c r="B23" s="77"/>
-      <c r="C23" s="77"/>
-      <c r="D23" s="79" t="s">
-        <v>96</v>
-      </c>
-      <c r="E23" s="80"/>
-      <c r="F23" s="77"/>
-      <c r="G23" s="77"/>
-      <c r="H23" s="77"/>
-      <c r="I23" s="77"/>
-      <c r="J23" s="77"/>
-      <c r="K23" s="77"/>
+      <c r="B23" s="99"/>
+      <c r="C23" s="99"/>
+      <c r="D23" s="103" t="s">
+        <v>129</v>
+      </c>
+      <c r="E23" s="104"/>
+      <c r="F23" s="99"/>
+      <c r="G23" s="99"/>
+      <c r="H23" s="99"/>
+      <c r="I23" s="99"/>
+      <c r="J23" s="99"/>
+      <c r="K23" s="99"/>
     </row>
     <row r="24" ht="12.75" customHeight="1">
       <c r="A24" s="35"/>
-      <c r="B24" s="65"/>
-      <c r="C24" s="65"/>
-      <c r="D24" s="67" t="s">
-        <v>97</v>
-      </c>
-      <c r="E24" s="68"/>
-      <c r="F24" s="69" t="s">
-        <v>98</v>
-      </c>
-      <c r="G24" s="70"/>
-      <c r="H24" s="70"/>
-      <c r="I24" s="70"/>
-      <c r="J24" s="65"/>
-      <c r="K24" s="69" t="s">
-        <v>99</v>
+      <c r="B24" s="77"/>
+      <c r="C24" s="77"/>
+      <c r="D24" s="79" t="s">
+        <v>130</v>
+      </c>
+      <c r="E24" s="81"/>
+      <c r="F24" s="83" t="s">
+        <v>131</v>
+      </c>
+      <c r="G24" s="85"/>
+      <c r="H24" s="85"/>
+      <c r="I24" s="85"/>
+      <c r="J24" s="77"/>
+      <c r="K24" s="83" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="25" ht="12.75" customHeight="1">
       <c r="A25" s="35"/>
-      <c r="B25" s="71">
+      <c r="B25" s="87">
         <f>B21+1</f>
         <v>4</v>
       </c>
-      <c r="C25" s="72" t="s">
-        <v>100</v>
-      </c>
-      <c r="D25" s="73" t="s">
-        <v>101</v>
-      </c>
-      <c r="E25" s="74"/>
-      <c r="F25" s="75"/>
-      <c r="G25" s="71"/>
-      <c r="H25" s="76" t="s">
-        <v>102</v>
-      </c>
-      <c r="I25" s="76" t="s">
-        <v>103</v>
-      </c>
-      <c r="J25" s="72" t="s">
-        <v>104</v>
-      </c>
-      <c r="K25" s="77"/>
+      <c r="C25" s="89" t="s">
+        <v>134</v>
+      </c>
+      <c r="D25" s="91" t="s">
+        <v>135</v>
+      </c>
+      <c r="E25" s="93"/>
+      <c r="F25" s="95"/>
+      <c r="G25" s="87"/>
+      <c r="H25" s="97" t="s">
+        <v>136</v>
+      </c>
+      <c r="I25" s="97" t="s">
+        <v>137</v>
+      </c>
+      <c r="J25" s="89" t="s">
+        <v>138</v>
+      </c>
+      <c r="K25" s="99"/>
     </row>
     <row r="26" ht="12.75" customHeight="1">
       <c r="A26" s="35"/>
-      <c r="B26" s="71"/>
-      <c r="C26" s="71"/>
-      <c r="D26" s="73" t="s">
-        <v>105</v>
-      </c>
-      <c r="E26" s="74"/>
-      <c r="F26" s="78" t="s">
-        <v>106</v>
-      </c>
-      <c r="G26" s="71"/>
-      <c r="H26" s="71"/>
-      <c r="I26" s="71"/>
-      <c r="J26" s="71"/>
-      <c r="K26" s="69" t="s">
-        <v>107</v>
+      <c r="B26" s="87"/>
+      <c r="C26" s="87"/>
+      <c r="D26" s="91" t="s">
+        <v>139</v>
+      </c>
+      <c r="E26" s="93"/>
+      <c r="F26" s="101" t="s">
+        <v>140</v>
+      </c>
+      <c r="G26" s="87"/>
+      <c r="H26" s="87"/>
+      <c r="I26" s="87"/>
+      <c r="J26" s="87"/>
+      <c r="K26" s="83" t="s">
+        <v>141</v>
       </c>
     </row>
     <row r="27" ht="12.75" customHeight="1">
       <c r="A27" s="35"/>
-      <c r="B27" s="77"/>
-      <c r="C27" s="77"/>
-      <c r="D27" s="79" t="s">
-        <v>108</v>
-      </c>
-      <c r="E27" s="80"/>
-      <c r="F27" s="77"/>
-      <c r="G27" s="77"/>
-      <c r="H27" s="77"/>
-      <c r="I27" s="77"/>
-      <c r="J27" s="77"/>
-      <c r="K27" s="77"/>
+      <c r="B27" s="99"/>
+      <c r="C27" s="99"/>
+      <c r="D27" s="103" t="s">
+        <v>142</v>
+      </c>
+      <c r="E27" s="104"/>
+      <c r="F27" s="99"/>
+      <c r="G27" s="99"/>
+      <c r="H27" s="99"/>
+      <c r="I27" s="99"/>
+      <c r="J27" s="99"/>
+      <c r="K27" s="99"/>
     </row>
     <row r="28" ht="12.75" customHeight="1">
       <c r="A28" s="35"/>
-      <c r="B28" s="65"/>
-      <c r="C28" s="65"/>
-      <c r="D28" s="67" t="s">
-        <v>109</v>
-      </c>
-      <c r="E28" s="68"/>
-      <c r="F28" s="69" t="s">
-        <v>110</v>
-      </c>
-      <c r="G28" s="70"/>
-      <c r="H28" s="70"/>
-      <c r="I28" s="70"/>
-      <c r="J28" s="65"/>
-      <c r="K28" s="69" t="s">
-        <v>111</v>
+      <c r="B28" s="77"/>
+      <c r="C28" s="77"/>
+      <c r="D28" s="79" t="s">
+        <v>143</v>
+      </c>
+      <c r="E28" s="81"/>
+      <c r="F28" s="83" t="s">
+        <v>144</v>
+      </c>
+      <c r="G28" s="85"/>
+      <c r="H28" s="85"/>
+      <c r="I28" s="85"/>
+      <c r="J28" s="77"/>
+      <c r="K28" s="83" t="s">
+        <v>145</v>
       </c>
     </row>
     <row r="29" ht="12.75" customHeight="1">
       <c r="A29" s="35"/>
-      <c r="B29" s="71">
+      <c r="B29" s="87">
         <f>B25+1</f>
         <v>5</v>
       </c>
-      <c r="C29" s="72" t="s">
-        <v>112</v>
-      </c>
-      <c r="D29" s="73" t="s">
-        <v>113</v>
-      </c>
-      <c r="E29" s="74"/>
-      <c r="F29" s="75"/>
-      <c r="G29" s="71"/>
-      <c r="H29" s="76" t="s">
-        <v>114</v>
-      </c>
-      <c r="I29" s="76" t="s">
-        <v>115</v>
-      </c>
-      <c r="J29" s="72" t="s">
-        <v>116</v>
-      </c>
-      <c r="K29" s="77"/>
+      <c r="C29" s="89" t="s">
+        <v>147</v>
+      </c>
+      <c r="D29" s="91" t="s">
+        <v>148</v>
+      </c>
+      <c r="E29" s="93"/>
+      <c r="F29" s="95"/>
+      <c r="G29" s="87"/>
+      <c r="H29" s="97" t="s">
+        <v>149</v>
+      </c>
+      <c r="I29" s="97" t="s">
+        <v>150</v>
+      </c>
+      <c r="J29" s="89" t="s">
+        <v>151</v>
+      </c>
+      <c r="K29" s="99"/>
     </row>
     <row r="30" ht="12.75" customHeight="1">
       <c r="A30" s="35"/>
-      <c r="B30" s="71"/>
-      <c r="C30" s="71"/>
-      <c r="D30" s="73" t="s">
-        <v>117</v>
-      </c>
-      <c r="E30" s="74"/>
-      <c r="F30" s="78" t="s">
-        <v>118</v>
-      </c>
-      <c r="G30" s="71"/>
-      <c r="H30" s="71"/>
-      <c r="I30" s="71"/>
-      <c r="J30" s="71"/>
-      <c r="K30" s="69" t="s">
-        <v>119</v>
+      <c r="B30" s="87"/>
+      <c r="C30" s="87"/>
+      <c r="D30" s="91" t="s">
+        <v>152</v>
+      </c>
+      <c r="E30" s="93"/>
+      <c r="F30" s="101" t="s">
+        <v>153</v>
+      </c>
+      <c r="G30" s="87"/>
+      <c r="H30" s="87"/>
+      <c r="I30" s="87"/>
+      <c r="J30" s="87"/>
+      <c r="K30" s="83" t="s">
+        <v>154</v>
       </c>
     </row>
     <row r="31" ht="12.75" customHeight="1">
       <c r="A31" s="35"/>
-      <c r="B31" s="77"/>
-      <c r="C31" s="77"/>
-      <c r="D31" s="79" t="s">
-        <v>120</v>
-      </c>
-      <c r="E31" s="80"/>
-      <c r="F31" s="77"/>
-      <c r="G31" s="77"/>
-      <c r="H31" s="77"/>
-      <c r="I31" s="77"/>
-      <c r="J31" s="77"/>
-      <c r="K31" s="77"/>
+      <c r="B31" s="99"/>
+      <c r="C31" s="99"/>
+      <c r="D31" s="103" t="s">
+        <v>155</v>
+      </c>
+      <c r="E31" s="104"/>
+      <c r="F31" s="99"/>
+      <c r="G31" s="99"/>
+      <c r="H31" s="99"/>
+      <c r="I31" s="99"/>
+      <c r="J31" s="99"/>
+      <c r="K31" s="99"/>
     </row>
     <row r="32" ht="12.75" customHeight="1">
       <c r="A32" s="35"/>
-      <c r="B32" s="65"/>
-      <c r="C32" s="65"/>
-      <c r="D32" s="67" t="s">
-        <v>121</v>
-      </c>
-      <c r="E32" s="68"/>
-      <c r="F32" s="69" t="s">
-        <v>122</v>
-      </c>
-      <c r="G32" s="70"/>
-      <c r="H32" s="70"/>
-      <c r="I32" s="70"/>
-      <c r="J32" s="65"/>
-      <c r="K32" s="69" t="s">
-        <v>123</v>
+      <c r="B32" s="77"/>
+      <c r="C32" s="77"/>
+      <c r="D32" s="79" t="s">
+        <v>157</v>
+      </c>
+      <c r="E32" s="81"/>
+      <c r="F32" s="83" t="s">
+        <v>158</v>
+      </c>
+      <c r="G32" s="85"/>
+      <c r="H32" s="85"/>
+      <c r="I32" s="85"/>
+      <c r="J32" s="77"/>
+      <c r="K32" s="83" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="33" ht="12.75" customHeight="1">
       <c r="A33" s="35"/>
-      <c r="B33" s="71">
+      <c r="B33" s="87">
         <f>B29+1</f>
         <v>6</v>
       </c>
-      <c r="C33" s="72" t="s">
-        <v>124</v>
-      </c>
-      <c r="D33" s="73" t="s">
-        <v>125</v>
-      </c>
-      <c r="E33" s="74"/>
-      <c r="F33" s="75"/>
-      <c r="G33" s="71"/>
-      <c r="H33" s="76" t="s">
-        <v>126</v>
-      </c>
-      <c r="I33" s="76" t="s">
-        <v>127</v>
-      </c>
-      <c r="J33" s="72" t="s">
-        <v>128</v>
-      </c>
-      <c r="K33" s="77"/>
+      <c r="C33" s="89" t="s">
+        <v>161</v>
+      </c>
+      <c r="D33" s="91" t="s">
+        <v>162</v>
+      </c>
+      <c r="E33" s="93"/>
+      <c r="F33" s="95"/>
+      <c r="G33" s="87"/>
+      <c r="H33" s="97" t="s">
+        <v>163</v>
+      </c>
+      <c r="I33" s="97" t="s">
+        <v>164</v>
+      </c>
+      <c r="J33" s="89" t="s">
+        <v>165</v>
+      </c>
+      <c r="K33" s="99"/>
     </row>
     <row r="34" ht="12.75" customHeight="1">
       <c r="A34" s="35"/>
-      <c r="B34" s="71"/>
-      <c r="C34" s="71"/>
-      <c r="D34" s="73" t="s">
-        <v>129</v>
-      </c>
-      <c r="E34" s="74"/>
-      <c r="F34" s="78" t="s">
-        <v>130</v>
-      </c>
-      <c r="G34" s="71"/>
-      <c r="H34" s="71"/>
-      <c r="I34" s="71"/>
-      <c r="J34" s="71"/>
-      <c r="K34" s="69" t="s">
-        <v>131</v>
+      <c r="B34" s="87"/>
+      <c r="C34" s="87"/>
+      <c r="D34" s="91" t="s">
+        <v>166</v>
+      </c>
+      <c r="E34" s="93"/>
+      <c r="F34" s="101" t="s">
+        <v>167</v>
+      </c>
+      <c r="G34" s="87"/>
+      <c r="H34" s="87"/>
+      <c r="I34" s="87"/>
+      <c r="J34" s="87"/>
+      <c r="K34" s="83" t="s">
+        <v>168</v>
       </c>
     </row>
     <row r="35" ht="12.75" customHeight="1">
       <c r="A35" s="35"/>
-      <c r="B35" s="77"/>
-      <c r="C35" s="77"/>
-      <c r="D35" s="79" t="s">
-        <v>132</v>
-      </c>
-      <c r="E35" s="80"/>
-      <c r="F35" s="77"/>
-      <c r="G35" s="77"/>
-      <c r="H35" s="77"/>
-      <c r="I35" s="77"/>
-      <c r="J35" s="77"/>
-      <c r="K35" s="77"/>
+      <c r="B35" s="99"/>
+      <c r="C35" s="99"/>
+      <c r="D35" s="103" t="s">
+        <v>171</v>
+      </c>
+      <c r="E35" s="104"/>
+      <c r="F35" s="99"/>
+      <c r="G35" s="99"/>
+      <c r="H35" s="99"/>
+      <c r="I35" s="99"/>
+      <c r="J35" s="99"/>
+      <c r="K35" s="99"/>
     </row>
     <row r="36" ht="12.75" customHeight="1">
       <c r="A36" s="35"/>
-      <c r="B36" s="65"/>
-      <c r="C36" s="65"/>
-      <c r="D36" s="67" t="s">
-        <v>133</v>
-      </c>
-      <c r="E36" s="68"/>
-      <c r="F36" s="69" t="s">
-        <v>134</v>
-      </c>
-      <c r="G36" s="70"/>
-      <c r="H36" s="70"/>
-      <c r="I36" s="70"/>
-      <c r="J36" s="65"/>
-      <c r="K36" s="69" t="s">
-        <v>135</v>
+      <c r="B36" s="77"/>
+      <c r="C36" s="77"/>
+      <c r="D36" s="79" t="s">
+        <v>175</v>
+      </c>
+      <c r="E36" s="81"/>
+      <c r="F36" s="83" t="s">
+        <v>176</v>
+      </c>
+      <c r="G36" s="85"/>
+      <c r="H36" s="85"/>
+      <c r="I36" s="85"/>
+      <c r="J36" s="77"/>
+      <c r="K36" s="83" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="37" ht="12.75" customHeight="1">
       <c r="A37" s="35"/>
-      <c r="B37" s="71">
+      <c r="B37" s="87">
         <f>B33+1</f>
         <v>7</v>
       </c>
-      <c r="C37" s="72" t="s">
-        <v>136</v>
-      </c>
-      <c r="D37" s="73" t="s">
-        <v>137</v>
-      </c>
-      <c r="E37" s="74"/>
-      <c r="F37" s="81"/>
-      <c r="G37" s="71"/>
-      <c r="H37" s="76" t="s">
-        <v>138</v>
-      </c>
-      <c r="I37" s="76" t="s">
-        <v>139</v>
-      </c>
-      <c r="J37" s="72" t="s">
-        <v>140</v>
-      </c>
-      <c r="K37" s="77"/>
+      <c r="C37" s="89" t="s">
+        <v>186</v>
+      </c>
+      <c r="D37" s="91" t="s">
+        <v>187</v>
+      </c>
+      <c r="E37" s="93"/>
+      <c r="F37" s="117"/>
+      <c r="G37" s="87"/>
+      <c r="H37" s="97" t="s">
+        <v>192</v>
+      </c>
+      <c r="I37" s="97" t="s">
+        <v>193</v>
+      </c>
+      <c r="J37" s="89" t="s">
+        <v>194</v>
+      </c>
+      <c r="K37" s="99"/>
     </row>
     <row r="38" ht="12.75" customHeight="1">
       <c r="A38" s="35"/>
-      <c r="B38" s="71"/>
-      <c r="C38" s="71"/>
-      <c r="D38" s="73" t="s">
-        <v>141</v>
-      </c>
-      <c r="E38" s="74"/>
-      <c r="F38" s="78" t="s">
-        <v>142</v>
-      </c>
-      <c r="G38" s="71"/>
-      <c r="H38" s="71"/>
-      <c r="I38" s="71"/>
-      <c r="J38" s="71"/>
-      <c r="K38" s="69" t="s">
-        <v>143</v>
+      <c r="B38" s="87"/>
+      <c r="C38" s="87"/>
+      <c r="D38" s="91" t="s">
+        <v>195</v>
+      </c>
+      <c r="E38" s="93"/>
+      <c r="F38" s="101" t="s">
+        <v>196</v>
+      </c>
+      <c r="G38" s="87"/>
+      <c r="H38" s="87"/>
+      <c r="I38" s="87"/>
+      <c r="J38" s="87"/>
+      <c r="K38" s="83" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="39" ht="12.75" customHeight="1">
       <c r="A39" s="35"/>
-      <c r="B39" s="77"/>
-      <c r="C39" s="77"/>
-      <c r="D39" s="79" t="s">
-        <v>144</v>
-      </c>
-      <c r="E39" s="80"/>
-      <c r="F39" s="77"/>
-      <c r="G39" s="77"/>
-      <c r="H39" s="77"/>
-      <c r="I39" s="77"/>
-      <c r="J39" s="77"/>
-      <c r="K39" s="77"/>
+      <c r="B39" s="99"/>
+      <c r="C39" s="99"/>
+      <c r="D39" s="103" t="s">
+        <v>199</v>
+      </c>
+      <c r="E39" s="104"/>
+      <c r="F39" s="99"/>
+      <c r="G39" s="99"/>
+      <c r="H39" s="99"/>
+      <c r="I39" s="99"/>
+      <c r="J39" s="99"/>
+      <c r="K39" s="99"/>
     </row>
     <row r="40" ht="12.75" customHeight="1">
       <c r="A40" s="35"/>
-      <c r="B40" s="65"/>
-      <c r="C40" s="65"/>
-      <c r="D40" s="67" t="s">
-        <v>145</v>
-      </c>
-      <c r="E40" s="68"/>
-      <c r="F40" s="69" t="s">
-        <v>146</v>
-      </c>
-      <c r="G40" s="70"/>
-      <c r="H40" s="70"/>
-      <c r="I40" s="70"/>
-      <c r="J40" s="65"/>
-      <c r="K40" s="69" t="s">
-        <v>147</v>
+      <c r="B40" s="77"/>
+      <c r="C40" s="77"/>
+      <c r="D40" s="79" t="s">
+        <v>204</v>
+      </c>
+      <c r="E40" s="81"/>
+      <c r="F40" s="83" t="s">
+        <v>205</v>
+      </c>
+      <c r="G40" s="85"/>
+      <c r="H40" s="85"/>
+      <c r="I40" s="85"/>
+      <c r="J40" s="77"/>
+      <c r="K40" s="83" t="s">
+        <v>207</v>
       </c>
     </row>
     <row r="41" ht="12.75" customHeight="1">
       <c r="A41" s="35"/>
-      <c r="B41" s="71">
+      <c r="B41" s="87">
         <f>B37+1</f>
         <v>8</v>
       </c>
-      <c r="C41" s="72" t="s">
-        <v>148</v>
-      </c>
-      <c r="D41" s="73" t="s">
-        <v>149</v>
-      </c>
-      <c r="E41" s="74"/>
-      <c r="F41" s="75"/>
-      <c r="G41" s="71"/>
-      <c r="H41" s="76" t="s">
-        <v>150</v>
-      </c>
-      <c r="I41" s="76" t="s">
-        <v>151</v>
-      </c>
-      <c r="J41" s="72" t="s">
-        <v>152</v>
-      </c>
-      <c r="K41" s="77"/>
+      <c r="C41" s="89" t="s">
+        <v>209</v>
+      </c>
+      <c r="D41" s="91" t="s">
+        <v>210</v>
+      </c>
+      <c r="E41" s="93"/>
+      <c r="F41" s="95"/>
+      <c r="G41" s="87"/>
+      <c r="H41" s="97" t="s">
+        <v>212</v>
+      </c>
+      <c r="I41" s="97" t="s">
+        <v>214</v>
+      </c>
+      <c r="J41" s="89" t="s">
+        <v>216</v>
+      </c>
+      <c r="K41" s="99"/>
     </row>
     <row r="42" ht="12.75" customHeight="1">
-      <c r="A42" s="82"/>
-      <c r="B42" s="71"/>
-      <c r="C42" s="71"/>
-      <c r="D42" s="73" t="s">
-        <v>153</v>
-      </c>
-      <c r="E42" s="74"/>
-      <c r="F42" s="78" t="s">
-        <v>154</v>
-      </c>
-      <c r="G42" s="71"/>
-      <c r="H42" s="71"/>
-      <c r="I42" s="71"/>
-      <c r="J42" s="71"/>
-      <c r="K42" s="69" t="s">
-        <v>155</v>
+      <c r="A42" s="120"/>
+      <c r="B42" s="87"/>
+      <c r="C42" s="87"/>
+      <c r="D42" s="91" t="s">
+        <v>237</v>
+      </c>
+      <c r="E42" s="93"/>
+      <c r="F42" s="101" t="s">
+        <v>239</v>
+      </c>
+      <c r="G42" s="87"/>
+      <c r="H42" s="87"/>
+      <c r="I42" s="87"/>
+      <c r="J42" s="87"/>
+      <c r="K42" s="83" t="s">
+        <v>242</v>
       </c>
     </row>
     <row r="43" ht="12.75" customHeight="1">
-      <c r="A43" s="84"/>
-      <c r="B43" s="77"/>
-      <c r="C43" s="77"/>
-      <c r="D43" s="79" t="s">
-        <v>169</v>
-      </c>
-      <c r="E43" s="80"/>
-      <c r="F43" s="77"/>
-      <c r="G43" s="77"/>
-      <c r="H43" s="77"/>
-      <c r="I43" s="77"/>
-      <c r="J43" s="77"/>
-      <c r="K43" s="77"/>
+      <c r="A43" s="121"/>
+      <c r="B43" s="99"/>
+      <c r="C43" s="99"/>
+      <c r="D43" s="103" t="s">
+        <v>247</v>
+      </c>
+      <c r="E43" s="104"/>
+      <c r="F43" s="99"/>
+      <c r="G43" s="99"/>
+      <c r="H43" s="99"/>
+      <c r="I43" s="99"/>
+      <c r="J43" s="99"/>
+      <c r="K43" s="99"/>
     </row>
     <row r="44" ht="12.75" customHeight="1">
-      <c r="A44" s="87"/>
-      <c r="B44" s="87"/>
-      <c r="C44" s="87"/>
-      <c r="D44" s="87"/>
-      <c r="E44" s="87"/>
-      <c r="F44" s="87"/>
-      <c r="G44" s="87"/>
-      <c r="H44" s="87"/>
-      <c r="I44" s="87"/>
-      <c r="J44" s="87"/>
-      <c r="K44" s="87"/>
+      <c r="A44" s="123"/>
+      <c r="B44" s="123"/>
+      <c r="C44" s="123"/>
+      <c r="D44" s="123"/>
+      <c r="E44" s="123"/>
+      <c r="F44" s="123"/>
+      <c r="G44" s="123"/>
+      <c r="H44" s="123"/>
+      <c r="I44" s="123"/>
+      <c r="J44" s="123"/>
+      <c r="K44" s="123"/>
     </row>
     <row r="45" ht="15.75" customHeight="1"/>
     <row r="46" ht="15.75" customHeight="1"/>

</xml_diff>